<commit_message>
[MS-OXWSCONT] fix watchman error
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites\ExchangeWebServices\Docs\MS-OXWSCONT\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
   </bookViews>
@@ -7437,6 +7432,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -7472,6 +7484,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7906,7 +7935,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:11" ht="30">
+    <row r="15" spans="1:11">
       <c r="A15" s="24" t="s">
         <v>3</v>
       </c>
@@ -8107,7 +8136,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:13" s="19" customFormat="1" ht="60">
+    <row r="24" spans="1:13" s="19" customFormat="1" ht="45">
       <c r="A24" s="18" t="s">
         <v>46</v>
       </c>
@@ -8132,7 +8161,7 @@
       </c>
       <c r="I24" s="20"/>
     </row>
-    <row r="25" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="25" spans="1:13" s="19" customFormat="1">
       <c r="A25" s="18" t="s">
         <v>47</v>
       </c>
@@ -8157,7 +8186,7 @@
       </c>
       <c r="I25" s="20"/>
     </row>
-    <row r="26" spans="1:13" s="19" customFormat="1" ht="30">
+    <row r="26" spans="1:13" s="19" customFormat="1">
       <c r="A26" s="45" t="s">
         <v>172</v>
       </c>
@@ -8284,7 +8313,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:13" s="19" customFormat="1" ht="60">
+    <row r="31" spans="1:13" s="19" customFormat="1" ht="45">
       <c r="A31" s="18" t="s">
         <v>51</v>
       </c>
@@ -8534,7 +8563,7 @@
       </c>
       <c r="I40" s="27"/>
     </row>
-    <row r="41" spans="1:9" ht="30">
+    <row r="41" spans="1:9">
       <c r="A41" s="45" t="s">
         <v>649</v>
       </c>
@@ -8584,7 +8613,7 @@
       </c>
       <c r="I42" s="47"/>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9">
       <c r="A43" s="18" t="s">
         <v>61</v>
       </c>
@@ -8634,7 +8663,7 @@
       </c>
       <c r="I44" s="47"/>
     </row>
-    <row r="45" spans="1:9" ht="45">
+    <row r="45" spans="1:9" ht="30">
       <c r="A45" s="18" t="s">
         <v>628</v>
       </c>
@@ -8659,7 +8688,7 @@
       </c>
       <c r="I45" s="47"/>
     </row>
-    <row r="46" spans="1:9" ht="315">
+    <row r="46" spans="1:9" ht="300">
       <c r="A46" s="18" t="s">
         <v>629</v>
       </c>
@@ -8784,7 +8813,7 @@
       </c>
       <c r="I50" s="47"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9">
       <c r="A51" s="18" t="s">
         <v>634</v>
       </c>
@@ -8809,7 +8838,7 @@
       </c>
       <c r="I51" s="47"/>
     </row>
-    <row r="52" spans="1:9" ht="45">
+    <row r="52" spans="1:9" ht="30">
       <c r="A52" s="18" t="s">
         <v>635</v>
       </c>
@@ -8859,7 +8888,7 @@
       </c>
       <c r="I53" s="47"/>
     </row>
-    <row r="54" spans="1:9" ht="45">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="18" t="s">
         <v>637</v>
       </c>
@@ -8934,7 +8963,7 @@
       </c>
       <c r="I56" s="47"/>
     </row>
-    <row r="57" spans="1:9" ht="30">
+    <row r="57" spans="1:9">
       <c r="A57" s="18" t="s">
         <v>640</v>
       </c>
@@ -8984,7 +9013,7 @@
       </c>
       <c r="I58" s="47"/>
     </row>
-    <row r="59" spans="1:9" ht="30">
+    <row r="59" spans="1:9">
       <c r="A59" s="18" t="s">
         <v>642</v>
       </c>
@@ -9034,7 +9063,7 @@
       </c>
       <c r="I60" s="47"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9">
       <c r="A61" s="18" t="s">
         <v>644</v>
       </c>
@@ -9059,7 +9088,7 @@
       </c>
       <c r="I61" s="47"/>
     </row>
-    <row r="62" spans="1:9" ht="30">
+    <row r="62" spans="1:9">
       <c r="A62" s="18" t="s">
         <v>645</v>
       </c>
@@ -9209,7 +9238,7 @@
       </c>
       <c r="I67" s="47"/>
     </row>
-    <row r="68" spans="1:9" ht="120">
+    <row r="68" spans="1:9" ht="105">
       <c r="A68" s="45" t="s">
         <v>656</v>
       </c>
@@ -9384,7 +9413,7 @@
       </c>
       <c r="I74" s="47"/>
     </row>
-    <row r="75" spans="1:9" ht="45">
+    <row r="75" spans="1:9" ht="30">
       <c r="A75" s="45" t="s">
         <v>660</v>
       </c>
@@ -9561,7 +9590,7 @@
       </c>
       <c r="I81" s="27"/>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9">
       <c r="A82" s="25" t="s">
         <v>73</v>
       </c>
@@ -9611,7 +9640,7 @@
       </c>
       <c r="I83" s="27"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9">
       <c r="A84" s="25" t="s">
         <v>75</v>
       </c>
@@ -9661,7 +9690,7 @@
       </c>
       <c r="I85" s="27"/>
     </row>
-    <row r="86" spans="1:9" ht="30">
+    <row r="86" spans="1:9">
       <c r="A86" s="25" t="s">
         <v>77</v>
       </c>
@@ -9686,7 +9715,7 @@
       </c>
       <c r="I86" s="27"/>
     </row>
-    <row r="87" spans="1:9" ht="30">
+    <row r="87" spans="1:9">
       <c r="A87" s="25" t="s">
         <v>78</v>
       </c>
@@ -9711,7 +9740,7 @@
       </c>
       <c r="I87" s="27"/>
     </row>
-    <row r="88" spans="1:9" ht="30">
+    <row r="88" spans="1:9">
       <c r="A88" s="25" t="s">
         <v>79</v>
       </c>
@@ -9761,7 +9790,7 @@
       </c>
       <c r="I89" s="27"/>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9">
       <c r="A90" s="25" t="s">
         <v>81</v>
       </c>
@@ -9886,7 +9915,7 @@
       </c>
       <c r="I94" s="47"/>
     </row>
-    <row r="95" spans="1:9" ht="30">
+    <row r="95" spans="1:9">
       <c r="A95" s="25" t="s">
         <v>85</v>
       </c>
@@ -10011,7 +10040,7 @@
       </c>
       <c r="I99" s="47"/>
     </row>
-    <row r="100" spans="1:9" ht="45">
+    <row r="100" spans="1:9" ht="30">
       <c r="A100" s="45" t="s">
         <v>687</v>
       </c>
@@ -10086,7 +10115,7 @@
       </c>
       <c r="I102" s="27"/>
     </row>
-    <row r="103" spans="1:9" ht="45">
+    <row r="103" spans="1:9" ht="30">
       <c r="A103" s="25" t="s">
         <v>90</v>
       </c>
@@ -10161,7 +10190,7 @@
       </c>
       <c r="I105" s="27"/>
     </row>
-    <row r="106" spans="1:9" ht="30">
+    <row r="106" spans="1:9">
       <c r="A106" s="25" t="s">
         <v>93</v>
       </c>
@@ -10436,7 +10465,7 @@
       </c>
       <c r="I116" s="27"/>
     </row>
-    <row r="117" spans="1:9" ht="45">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="25" t="s">
         <v>104</v>
       </c>
@@ -10461,7 +10490,7 @@
       </c>
       <c r="I117" s="27"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9">
       <c r="A118" s="25" t="s">
         <v>105</v>
       </c>
@@ -10511,7 +10540,7 @@
       </c>
       <c r="I119" s="27"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9">
       <c r="A120" s="25" t="s">
         <v>107</v>
       </c>
@@ -10611,7 +10640,7 @@
       </c>
       <c r="I123" s="27"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9">
       <c r="A124" s="25" t="s">
         <v>111</v>
       </c>
@@ -10661,7 +10690,7 @@
       </c>
       <c r="I125" s="27"/>
     </row>
-    <row r="126" spans="1:9" ht="30">
+    <row r="126" spans="1:9">
       <c r="A126" s="25" t="s">
         <v>113</v>
       </c>
@@ -10711,7 +10740,7 @@
       </c>
       <c r="I127" s="27"/>
     </row>
-    <row r="128" spans="1:9" ht="30">
+    <row r="128" spans="1:9">
       <c r="A128" s="25" t="s">
         <v>115</v>
       </c>
@@ -10761,7 +10790,7 @@
       </c>
       <c r="I129" s="27"/>
     </row>
-    <row r="130" spans="1:9" ht="30">
+    <row r="130" spans="1:9">
       <c r="A130" s="25" t="s">
         <v>117</v>
       </c>
@@ -10836,7 +10865,7 @@
       </c>
       <c r="I132" s="27"/>
     </row>
-    <row r="133" spans="1:9" ht="45">
+    <row r="133" spans="1:9" ht="30">
       <c r="A133" s="25" t="s">
         <v>120</v>
       </c>
@@ -10861,7 +10890,7 @@
       </c>
       <c r="I133" s="27"/>
     </row>
-    <row r="134" spans="1:9" ht="30">
+    <row r="134" spans="1:9">
       <c r="A134" s="25" t="s">
         <v>121</v>
       </c>
@@ -10911,7 +10940,7 @@
       </c>
       <c r="I135" s="27"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9">
       <c r="A136" s="25" t="s">
         <v>123</v>
       </c>
@@ -10961,7 +10990,7 @@
       </c>
       <c r="I137" s="27"/>
     </row>
-    <row r="138" spans="1:9" ht="30">
+    <row r="138" spans="1:9">
       <c r="A138" s="25" t="s">
         <v>125</v>
       </c>
@@ -11163,7 +11192,7 @@
       </c>
       <c r="I145" s="27"/>
     </row>
-    <row r="146" spans="1:9" ht="45">
+    <row r="146" spans="1:9" ht="30">
       <c r="A146" s="25" t="s">
         <v>131</v>
       </c>
@@ -11288,7 +11317,7 @@
       </c>
       <c r="I150" s="27"/>
     </row>
-    <row r="151" spans="1:9" ht="30">
+    <row r="151" spans="1:9">
       <c r="A151" s="25" t="s">
         <v>136</v>
       </c>
@@ -11338,7 +11367,7 @@
       </c>
       <c r="I152" s="27"/>
     </row>
-    <row r="153" spans="1:9" ht="30">
+    <row r="153" spans="1:9">
       <c r="A153" s="25" t="s">
         <v>138</v>
       </c>
@@ -11538,7 +11567,7 @@
       </c>
       <c r="I160" s="27"/>
     </row>
-    <row r="161" spans="1:9" ht="30">
+    <row r="161" spans="1:9">
       <c r="A161" s="25" t="s">
         <v>146</v>
       </c>
@@ -11588,7 +11617,7 @@
       </c>
       <c r="I162" s="27"/>
     </row>
-    <row r="163" spans="1:9" ht="45">
+    <row r="163" spans="1:9" ht="30">
       <c r="A163" s="25" t="s">
         <v>148</v>
       </c>
@@ -11638,7 +11667,7 @@
       </c>
       <c r="I164" s="27"/>
     </row>
-    <row r="165" spans="1:9" ht="45">
+    <row r="165" spans="1:9" ht="30">
       <c r="A165" s="18" t="s">
         <v>150</v>
       </c>
@@ -11688,7 +11717,7 @@
       </c>
       <c r="I166" s="27"/>
     </row>
-    <row r="167" spans="1:9" ht="30">
+    <row r="167" spans="1:9">
       <c r="A167" s="45" t="s">
         <v>744</v>
       </c>
@@ -11817,7 +11846,7 @@
       </c>
       <c r="I171" s="47"/>
     </row>
-    <row r="172" spans="1:9" ht="30">
+    <row r="172" spans="1:9">
       <c r="A172" s="45" t="s">
         <v>749</v>
       </c>
@@ -11842,7 +11871,7 @@
       </c>
       <c r="I172" s="47"/>
     </row>
-    <row r="173" spans="1:9" ht="30">
+    <row r="173" spans="1:9">
       <c r="A173" s="45" t="s">
         <v>750</v>
       </c>
@@ -11894,7 +11923,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="30">
+    <row r="175" spans="1:9">
       <c r="A175" s="45" t="s">
         <v>752</v>
       </c>
@@ -11919,7 +11948,7 @@
       </c>
       <c r="I175" s="47"/>
     </row>
-    <row r="176" spans="1:9" ht="30">
+    <row r="176" spans="1:9">
       <c r="A176" s="45" t="s">
         <v>753</v>
       </c>
@@ -11944,7 +11973,7 @@
       </c>
       <c r="I176" s="47"/>
     </row>
-    <row r="177" spans="1:9" ht="30">
+    <row r="177" spans="1:9">
       <c r="A177" s="45" t="s">
         <v>754</v>
       </c>
@@ -11996,7 +12025,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="30">
+    <row r="179" spans="1:9">
       <c r="A179" s="45" t="s">
         <v>756</v>
       </c>
@@ -12073,7 +12102,7 @@
       </c>
       <c r="I181" s="47"/>
     </row>
-    <row r="182" spans="1:9" ht="30">
+    <row r="182" spans="1:9">
       <c r="A182" s="45" t="s">
         <v>759</v>
       </c>
@@ -12098,7 +12127,7 @@
       </c>
       <c r="I182" s="47"/>
     </row>
-    <row r="183" spans="1:9" ht="30">
+    <row r="183" spans="1:9">
       <c r="A183" s="45" t="s">
         <v>760</v>
       </c>
@@ -12150,7 +12179,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="30">
+    <row r="185" spans="1:9">
       <c r="A185" s="45" t="s">
         <v>762</v>
       </c>
@@ -12175,7 +12204,7 @@
       </c>
       <c r="I185" s="47"/>
     </row>
-    <row r="186" spans="1:9" ht="30">
+    <row r="186" spans="1:9">
       <c r="A186" s="45" t="s">
         <v>763</v>
       </c>
@@ -12252,7 +12281,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="30">
+    <row r="189" spans="1:9">
       <c r="A189" s="45" t="s">
         <v>766</v>
       </c>
@@ -12277,7 +12306,7 @@
       </c>
       <c r="I189" s="47"/>
     </row>
-    <row r="190" spans="1:9" ht="30">
+    <row r="190" spans="1:9">
       <c r="A190" s="45" t="s">
         <v>767</v>
       </c>
@@ -12302,7 +12331,7 @@
       </c>
       <c r="I190" s="47"/>
     </row>
-    <row r="191" spans="1:9" ht="30">
+    <row r="191" spans="1:9">
       <c r="A191" s="45" t="s">
         <v>768</v>
       </c>
@@ -12354,7 +12383,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="30">
+    <row r="193" spans="1:9">
       <c r="A193" s="45" t="s">
         <v>770</v>
       </c>
@@ -12379,7 +12408,7 @@
       </c>
       <c r="I193" s="47"/>
     </row>
-    <row r="194" spans="1:9" ht="30">
+    <row r="194" spans="1:9">
       <c r="A194" s="45" t="s">
         <v>771</v>
       </c>
@@ -12404,7 +12433,7 @@
       </c>
       <c r="I194" s="47"/>
     </row>
-    <row r="195" spans="1:9" ht="30">
+    <row r="195" spans="1:9">
       <c r="A195" s="45" t="s">
         <v>772</v>
       </c>
@@ -12429,7 +12458,7 @@
       </c>
       <c r="I195" s="47"/>
     </row>
-    <row r="196" spans="1:9" ht="30">
+    <row r="196" spans="1:9">
       <c r="A196" s="45" t="s">
         <v>773</v>
       </c>
@@ -12558,7 +12587,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="30">
+    <row r="201" spans="1:9">
       <c r="A201" s="45" t="s">
         <v>778</v>
       </c>
@@ -12610,7 +12639,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="203" spans="1:9" ht="30">
+    <row r="203" spans="1:9">
       <c r="A203" s="45" t="s">
         <v>780</v>
       </c>
@@ -12635,7 +12664,7 @@
       </c>
       <c r="I203" s="47"/>
     </row>
-    <row r="204" spans="1:9" ht="30">
+    <row r="204" spans="1:9">
       <c r="A204" s="45" t="s">
         <v>781</v>
       </c>
@@ -12660,7 +12689,7 @@
       </c>
       <c r="I204" s="47"/>
     </row>
-    <row r="205" spans="1:9" ht="30">
+    <row r="205" spans="1:9">
       <c r="A205" s="45" t="s">
         <v>782</v>
       </c>
@@ -12712,7 +12741,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="207" spans="1:9" ht="30">
+    <row r="207" spans="1:9">
       <c r="A207" s="45" t="s">
         <v>784</v>
       </c>
@@ -12762,7 +12791,7 @@
       </c>
       <c r="I208" s="47"/>
     </row>
-    <row r="209" spans="1:9" ht="30">
+    <row r="209" spans="1:9">
       <c r="A209" s="45" t="s">
         <v>786</v>
       </c>
@@ -12814,7 +12843,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="211" spans="1:9" ht="30">
+    <row r="211" spans="1:9">
       <c r="A211" s="45" t="s">
         <v>856</v>
       </c>
@@ -12864,7 +12893,7 @@
       </c>
       <c r="I212" s="47"/>
     </row>
-    <row r="213" spans="1:9" ht="30">
+    <row r="213" spans="1:9">
       <c r="A213" s="45" t="s">
         <v>858</v>
       </c>
@@ -12889,7 +12918,7 @@
       </c>
       <c r="I213" s="47"/>
     </row>
-    <row r="214" spans="1:9" ht="30">
+    <row r="214" spans="1:9">
       <c r="A214" s="45" t="s">
         <v>859</v>
       </c>
@@ -13039,7 +13068,7 @@
       </c>
       <c r="I219" s="47"/>
     </row>
-    <row r="220" spans="1:9" ht="30">
+    <row r="220" spans="1:9">
       <c r="A220" s="45" t="s">
         <v>865</v>
       </c>
@@ -13064,7 +13093,7 @@
       </c>
       <c r="I220" s="47"/>
     </row>
-    <row r="221" spans="1:9" ht="30">
+    <row r="221" spans="1:9">
       <c r="A221" s="45" t="s">
         <v>866</v>
       </c>
@@ -13114,7 +13143,7 @@
       </c>
       <c r="I222" s="47"/>
     </row>
-    <row r="223" spans="1:9" ht="30">
+    <row r="223" spans="1:9">
       <c r="A223" s="45" t="s">
         <v>868</v>
       </c>
@@ -13139,7 +13168,7 @@
       </c>
       <c r="I223" s="47"/>
     </row>
-    <row r="224" spans="1:9" ht="30">
+    <row r="224" spans="1:9">
       <c r="A224" s="45" t="s">
         <v>869</v>
       </c>
@@ -13164,7 +13193,7 @@
       </c>
       <c r="I224" s="47"/>
     </row>
-    <row r="225" spans="1:9" ht="30">
+    <row r="225" spans="1:9">
       <c r="A225" s="45" t="s">
         <v>870</v>
       </c>
@@ -13189,7 +13218,7 @@
       </c>
       <c r="I225" s="47"/>
     </row>
-    <row r="226" spans="1:9" ht="30">
+    <row r="226" spans="1:9">
       <c r="A226" s="45" t="s">
         <v>871</v>
       </c>
@@ -13239,7 +13268,7 @@
       </c>
       <c r="I227" s="47"/>
     </row>
-    <row r="228" spans="1:9" ht="30">
+    <row r="228" spans="1:9">
       <c r="A228" s="45" t="s">
         <v>873</v>
       </c>
@@ -13264,7 +13293,7 @@
       </c>
       <c r="I228" s="47"/>
     </row>
-    <row r="229" spans="1:9" ht="30">
+    <row r="229" spans="1:9">
       <c r="A229" s="45" t="s">
         <v>874</v>
       </c>
@@ -13289,7 +13318,7 @@
       </c>
       <c r="I229" s="47"/>
     </row>
-    <row r="230" spans="1:9" ht="30">
+    <row r="230" spans="1:9">
       <c r="A230" s="45" t="s">
         <v>875</v>
       </c>
@@ -13339,7 +13368,7 @@
       </c>
       <c r="I231" s="47"/>
     </row>
-    <row r="232" spans="1:9" ht="30">
+    <row r="232" spans="1:9">
       <c r="A232" s="45" t="s">
         <v>877</v>
       </c>
@@ -13364,7 +13393,7 @@
       </c>
       <c r="I232" s="47"/>
     </row>
-    <row r="233" spans="1:9" ht="45">
+    <row r="233" spans="1:9" ht="30">
       <c r="A233" s="25" t="s">
         <v>152</v>
       </c>
@@ -13489,7 +13518,7 @@
       </c>
       <c r="I237" s="27"/>
     </row>
-    <row r="238" spans="1:9" ht="45">
+    <row r="238" spans="1:9" ht="30">
       <c r="A238" s="25" t="s">
         <v>157</v>
       </c>
@@ -13889,7 +13918,7 @@
       </c>
       <c r="I253" s="27"/>
     </row>
-    <row r="254" spans="1:9" ht="45">
+    <row r="254" spans="1:9" ht="30">
       <c r="A254" s="25" t="s">
         <v>174</v>
       </c>
@@ -13914,7 +13943,7 @@
       </c>
       <c r="I254" s="27"/>
     </row>
-    <row r="255" spans="1:9" ht="45">
+    <row r="255" spans="1:9" ht="30">
       <c r="A255" s="25" t="s">
         <v>175</v>
       </c>
@@ -14114,7 +14143,7 @@
       </c>
       <c r="I262" s="27"/>
     </row>
-    <row r="263" spans="1:9" ht="75">
+    <row r="263" spans="1:9" ht="60">
       <c r="A263" s="25" t="s">
         <v>183</v>
       </c>
@@ -14214,7 +14243,7 @@
       </c>
       <c r="I266" s="27"/>
     </row>
-    <row r="267" spans="1:9" ht="45">
+    <row r="267" spans="1:9" ht="30">
       <c r="A267" s="18" t="s">
         <v>1139</v>
       </c>
@@ -14239,7 +14268,7 @@
       </c>
       <c r="I267" s="47"/>
     </row>
-    <row r="268" spans="1:9" ht="195">
+    <row r="268" spans="1:9" ht="165">
       <c r="A268" s="18" t="s">
         <v>1140</v>
       </c>
@@ -14264,7 +14293,7 @@
       </c>
       <c r="I268" s="47"/>
     </row>
-    <row r="269" spans="1:9" ht="45">
+    <row r="269" spans="1:9" ht="30">
       <c r="A269" s="18" t="s">
         <v>1141</v>
       </c>
@@ -14414,7 +14443,7 @@
       </c>
       <c r="I274" s="47"/>
     </row>
-    <row r="275" spans="1:9" ht="45">
+    <row r="275" spans="1:9" ht="30">
       <c r="A275" s="18" t="s">
         <v>1147</v>
       </c>
@@ -14489,7 +14518,7 @@
       </c>
       <c r="I277" s="47"/>
     </row>
-    <row r="278" spans="1:9" ht="45">
+    <row r="278" spans="1:9" ht="30">
       <c r="A278" s="18" t="s">
         <v>1154</v>
       </c>
@@ -14539,7 +14568,7 @@
       </c>
       <c r="I279" s="47"/>
     </row>
-    <row r="280" spans="1:9" ht="45">
+    <row r="280" spans="1:9" ht="30">
       <c r="A280" s="45" t="s">
         <v>1186</v>
       </c>
@@ -14564,7 +14593,7 @@
       </c>
       <c r="I280" s="47"/>
     </row>
-    <row r="281" spans="1:9" ht="45">
+    <row r="281" spans="1:9" ht="30">
       <c r="A281" s="18" t="s">
         <v>1156</v>
       </c>
@@ -14614,7 +14643,7 @@
       </c>
       <c r="I282" s="47"/>
     </row>
-    <row r="283" spans="1:9" ht="45">
+    <row r="283" spans="1:9" ht="30">
       <c r="A283" s="18" t="s">
         <v>1171</v>
       </c>
@@ -14639,7 +14668,7 @@
       </c>
       <c r="I283" s="47"/>
     </row>
-    <row r="284" spans="1:9" ht="195">
+    <row r="284" spans="1:9" ht="150">
       <c r="A284" s="18" t="s">
         <v>1172</v>
       </c>
@@ -14839,7 +14868,7 @@
       </c>
       <c r="I291" s="47"/>
     </row>
-    <row r="292" spans="1:9" ht="45">
+    <row r="292" spans="1:9" ht="30">
       <c r="A292" s="18" t="s">
         <v>1180</v>
       </c>
@@ -14889,7 +14918,7 @@
       </c>
       <c r="I293" s="47"/>
     </row>
-    <row r="294" spans="1:9" ht="45">
+    <row r="294" spans="1:9" ht="30">
       <c r="A294" s="18" t="s">
         <v>1182</v>
       </c>
@@ -15039,7 +15068,7 @@
       </c>
       <c r="I299" s="27"/>
     </row>
-    <row r="300" spans="1:9" ht="30">
+    <row r="300" spans="1:9">
       <c r="A300" s="25" t="s">
         <v>259</v>
       </c>
@@ -15064,7 +15093,7 @@
       </c>
       <c r="I300" s="27"/>
     </row>
-    <row r="301" spans="1:9" ht="30">
+    <row r="301" spans="1:9">
       <c r="A301" s="25" t="s">
         <v>260</v>
       </c>
@@ -15189,7 +15218,7 @@
       </c>
       <c r="I305" s="27"/>
     </row>
-    <row r="306" spans="1:9" ht="30">
+    <row r="306" spans="1:9">
       <c r="A306" s="25" t="s">
         <v>265</v>
       </c>
@@ -15264,7 +15293,7 @@
       </c>
       <c r="I308" s="27"/>
     </row>
-    <row r="309" spans="1:9" ht="30">
+    <row r="309" spans="1:9">
       <c r="A309" s="25" t="s">
         <v>268</v>
       </c>
@@ -15339,7 +15368,7 @@
       </c>
       <c r="I311" s="27"/>
     </row>
-    <row r="312" spans="1:9" ht="30">
+    <row r="312" spans="1:9">
       <c r="A312" s="25" t="s">
         <v>271</v>
       </c>
@@ -15389,7 +15418,7 @@
       </c>
       <c r="I313" s="27"/>
     </row>
-    <row r="314" spans="1:9" ht="30">
+    <row r="314" spans="1:9">
       <c r="A314" s="25" t="s">
         <v>273</v>
       </c>
@@ -15439,7 +15468,7 @@
       </c>
       <c r="I315" s="27"/>
     </row>
-    <row r="316" spans="1:9" ht="30">
+    <row r="316" spans="1:9">
       <c r="A316" s="25" t="s">
         <v>275</v>
       </c>
@@ -15514,7 +15543,7 @@
       </c>
       <c r="I318" s="27"/>
     </row>
-    <row r="319" spans="1:9" ht="45">
+    <row r="319" spans="1:9" ht="30">
       <c r="A319" s="25" t="s">
         <v>278</v>
       </c>
@@ -15564,7 +15593,7 @@
       </c>
       <c r="I320" s="27"/>
     </row>
-    <row r="321" spans="1:9" ht="45">
+    <row r="321" spans="1:9" ht="30">
       <c r="A321" s="25" t="s">
         <v>280</v>
       </c>
@@ -15639,7 +15668,7 @@
       </c>
       <c r="I323" s="27"/>
     </row>
-    <row r="324" spans="1:9" ht="45">
+    <row r="324" spans="1:9" ht="30">
       <c r="A324" s="25" t="s">
         <v>283</v>
       </c>
@@ -15789,7 +15818,7 @@
       </c>
       <c r="I329" s="47"/>
     </row>
-    <row r="330" spans="1:9" ht="30">
+    <row r="330" spans="1:9">
       <c r="A330" s="45" t="s">
         <v>1214</v>
       </c>
@@ -15864,7 +15893,7 @@
       </c>
       <c r="I332" s="47"/>
     </row>
-    <row r="333" spans="1:9" ht="45">
+    <row r="333" spans="1:9" ht="30">
       <c r="A333" s="25" t="s">
         <v>287</v>
       </c>
@@ -15964,7 +15993,7 @@
       </c>
       <c r="I336" s="27"/>
     </row>
-    <row r="337" spans="1:9" ht="30">
+    <row r="337" spans="1:9">
       <c r="A337" s="25" t="s">
         <v>291</v>
       </c>
@@ -16116,7 +16145,7 @@
       </c>
       <c r="I342" s="47"/>
     </row>
-    <row r="343" spans="1:9" ht="30">
+    <row r="343" spans="1:9">
       <c r="A343" s="45" t="s">
         <v>1237</v>
       </c>
@@ -16137,7 +16166,7 @@
         <v>15</v>
       </c>
       <c r="H343" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I343" s="47"/>
     </row>
@@ -16187,7 +16216,7 @@
         <v>15</v>
       </c>
       <c r="H345" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I345" s="47"/>
     </row>
@@ -16216,7 +16245,7 @@
       </c>
       <c r="I346" s="47"/>
     </row>
-    <row r="347" spans="1:9" ht="30">
+    <row r="347" spans="1:9">
       <c r="A347" s="45" t="s">
         <v>1241</v>
       </c>
@@ -16237,7 +16266,7 @@
         <v>15</v>
       </c>
       <c r="H347" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I347" s="47"/>
     </row>
@@ -16364,7 +16393,7 @@
         <v>15</v>
       </c>
       <c r="H352" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I352" s="47"/>
     </row>
@@ -16443,7 +16472,7 @@
       </c>
       <c r="I355" s="27"/>
     </row>
-    <row r="356" spans="1:9" ht="45">
+    <row r="356" spans="1:9" ht="30">
       <c r="A356" s="18" t="s">
         <v>296</v>
       </c>
@@ -16680,7 +16709,7 @@
       </c>
       <c r="I364" s="27"/>
     </row>
-    <row r="365" spans="1:9" ht="150">
+    <row r="365" spans="1:9" ht="135">
       <c r="A365" s="25" t="s">
         <v>304</v>
       </c>
@@ -16755,7 +16784,7 @@
       </c>
       <c r="I367" s="27"/>
     </row>
-    <row r="368" spans="1:9" ht="45">
+    <row r="368" spans="1:9" ht="30">
       <c r="A368" s="25" t="s">
         <v>307</v>
       </c>
@@ -16880,7 +16909,7 @@
       </c>
       <c r="I372" s="27"/>
     </row>
-    <row r="373" spans="1:9" ht="150">
+    <row r="373" spans="1:9" ht="135">
       <c r="A373" s="25" t="s">
         <v>312</v>
       </c>
@@ -17055,7 +17084,7 @@
       </c>
       <c r="I379" s="27"/>
     </row>
-    <row r="380" spans="1:9" ht="45">
+    <row r="380" spans="1:9" ht="30">
       <c r="A380" s="25" t="s">
         <v>319</v>
       </c>
@@ -17080,7 +17109,7 @@
       </c>
       <c r="I380" s="27"/>
     </row>
-    <row r="381" spans="1:9" ht="150">
+    <row r="381" spans="1:9" ht="135">
       <c r="A381" s="25" t="s">
         <v>320</v>
       </c>
@@ -17505,7 +17534,7 @@
       </c>
       <c r="I397" s="27"/>
     </row>
-    <row r="398" spans="1:9" ht="45">
+    <row r="398" spans="1:9" ht="30">
       <c r="A398" s="25" t="s">
         <v>337</v>
       </c>
@@ -17555,7 +17584,7 @@
       </c>
       <c r="I399" s="27"/>
     </row>
-    <row r="400" spans="1:9" ht="45">
+    <row r="400" spans="1:9" ht="30">
       <c r="A400" s="25" t="s">
         <v>339</v>
       </c>
@@ -17580,7 +17609,7 @@
       </c>
       <c r="I400" s="27"/>
     </row>
-    <row r="401" spans="1:9" ht="45">
+    <row r="401" spans="1:9" ht="30">
       <c r="A401" s="25" t="s">
         <v>340</v>
       </c>
@@ -17682,7 +17711,7 @@
       </c>
       <c r="I404" s="47"/>
     </row>
-    <row r="405" spans="1:9" ht="45">
+    <row r="405" spans="1:9" ht="30">
       <c r="A405" s="45" t="s">
         <v>1049</v>
       </c>
@@ -17707,7 +17736,7 @@
       </c>
       <c r="I405" s="47"/>
     </row>
-    <row r="406" spans="1:9" ht="30">
+    <row r="406" spans="1:9">
       <c r="A406" s="45" t="s">
         <v>1050</v>
       </c>
@@ -17732,7 +17761,7 @@
       </c>
       <c r="I406" s="47"/>
     </row>
-    <row r="407" spans="1:9" ht="30">
+    <row r="407" spans="1:9">
       <c r="A407" s="45" t="s">
         <v>1051</v>
       </c>
@@ -17757,7 +17786,7 @@
       </c>
       <c r="I407" s="47"/>
     </row>
-    <row r="408" spans="1:9" ht="30">
+    <row r="408" spans="1:9">
       <c r="A408" s="45" t="s">
         <v>1052</v>
       </c>
@@ -17782,7 +17811,7 @@
       </c>
       <c r="I408" s="47"/>
     </row>
-    <row r="409" spans="1:9" ht="30">
+    <row r="409" spans="1:9">
       <c r="A409" s="45" t="s">
         <v>1053</v>
       </c>
@@ -17834,7 +17863,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="411" spans="1:9" ht="240">
+    <row r="411" spans="1:9" ht="225">
       <c r="A411" s="45" t="s">
         <v>1066</v>
       </c>
@@ -17859,7 +17888,7 @@
       </c>
       <c r="I411" s="47"/>
     </row>
-    <row r="412" spans="1:9" ht="60">
+    <row r="412" spans="1:9" ht="45">
       <c r="A412" s="45" t="s">
         <v>1067</v>
       </c>
@@ -17905,7 +17934,7 @@
         <v>15</v>
       </c>
       <c r="H413" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I413" s="47"/>
     </row>
@@ -17930,11 +17959,11 @@
         <v>15</v>
       </c>
       <c r="H414" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I414" s="47"/>
     </row>
-    <row r="415" spans="1:9" ht="30">
+    <row r="415" spans="1:9">
       <c r="A415" s="45" t="s">
         <v>1070</v>
       </c>
@@ -17955,7 +17984,7 @@
         <v>15</v>
       </c>
       <c r="H415" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I415" s="47"/>
     </row>
@@ -18055,11 +18084,11 @@
         <v>15</v>
       </c>
       <c r="H419" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I419" s="47"/>
     </row>
-    <row r="420" spans="1:9" ht="30">
+    <row r="420" spans="1:9">
       <c r="A420" s="45" t="s">
         <v>1075</v>
       </c>
@@ -18080,7 +18109,7 @@
         <v>15</v>
       </c>
       <c r="H420" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I420" s="47"/>
     </row>
@@ -18184,7 +18213,7 @@
       </c>
       <c r="I424" s="27"/>
     </row>
-    <row r="425" spans="1:9" ht="45">
+    <row r="425" spans="1:9" ht="30">
       <c r="A425" s="25" t="s">
         <v>189</v>
       </c>
@@ -18284,7 +18313,7 @@
       </c>
       <c r="I428" s="27"/>
     </row>
-    <row r="429" spans="1:9" ht="45">
+    <row r="429" spans="1:9" ht="30">
       <c r="A429" s="25" t="s">
         <v>193</v>
       </c>
@@ -18334,7 +18363,7 @@
       </c>
       <c r="I430" s="27"/>
     </row>
-    <row r="431" spans="1:9" ht="105">
+    <row r="431" spans="1:9" ht="75">
       <c r="A431" s="25" t="s">
         <v>195</v>
       </c>
@@ -18405,7 +18434,7 @@
         <v>15</v>
       </c>
       <c r="H433" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I433" s="27"/>
     </row>
@@ -18430,7 +18459,7 @@
         <v>15</v>
       </c>
       <c r="H434" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I434" s="27"/>
     </row>
@@ -18459,7 +18488,7 @@
       </c>
       <c r="I435" s="27"/>
     </row>
-    <row r="436" spans="1:9" ht="60">
+    <row r="436" spans="1:9" ht="45">
       <c r="A436" s="25" t="s">
         <v>200</v>
       </c>
@@ -18480,7 +18509,7 @@
         <v>15</v>
       </c>
       <c r="H436" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I436" s="27"/>
     </row>
@@ -18505,11 +18534,11 @@
         <v>15</v>
       </c>
       <c r="H437" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I437" s="27"/>
     </row>
-    <row r="438" spans="1:9" ht="45">
+    <row r="438" spans="1:9" ht="30">
       <c r="A438" s="25" t="s">
         <v>202</v>
       </c>
@@ -18530,11 +18559,11 @@
         <v>15</v>
       </c>
       <c r="H438" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I438" s="27"/>
     </row>
-    <row r="439" spans="1:9" ht="60">
+    <row r="439" spans="1:9" ht="45">
       <c r="A439" s="25" t="s">
         <v>203</v>
       </c>
@@ -18555,11 +18584,11 @@
         <v>15</v>
       </c>
       <c r="H439" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I439" s="27"/>
     </row>
-    <row r="440" spans="1:9" ht="60">
+    <row r="440" spans="1:9" ht="45">
       <c r="A440" s="25" t="s">
         <v>204</v>
       </c>
@@ -18580,11 +18609,11 @@
         <v>15</v>
       </c>
       <c r="H440" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I440" s="27"/>
     </row>
-    <row r="441" spans="1:9" ht="45">
+    <row r="441" spans="1:9" ht="30">
       <c r="A441" s="25" t="s">
         <v>205</v>
       </c>
@@ -18605,11 +18634,11 @@
         <v>15</v>
       </c>
       <c r="H441" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I441" s="27"/>
     </row>
-    <row r="442" spans="1:9" ht="60">
+    <row r="442" spans="1:9" ht="45">
       <c r="A442" s="25" t="s">
         <v>206</v>
       </c>
@@ -18630,11 +18659,11 @@
         <v>15</v>
       </c>
       <c r="H442" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I442" s="27"/>
     </row>
-    <row r="443" spans="1:9" ht="60">
+    <row r="443" spans="1:9" ht="45">
       <c r="A443" s="25" t="s">
         <v>207</v>
       </c>
@@ -18655,7 +18684,7 @@
         <v>15</v>
       </c>
       <c r="H443" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I443" s="27"/>
     </row>
@@ -18680,7 +18709,7 @@
         <v>15</v>
       </c>
       <c r="H444" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I444" s="27"/>
     </row>
@@ -18844,7 +18873,7 @@
       </c>
       <c r="I450" s="27"/>
     </row>
-    <row r="451" spans="1:9" ht="255">
+    <row r="451" spans="1:9" ht="240">
       <c r="A451" s="25" t="s">
         <v>215</v>
       </c>
@@ -19019,7 +19048,7 @@
       </c>
       <c r="I457" s="27"/>
     </row>
-    <row r="458" spans="1:9" ht="90">
+    <row r="458" spans="1:9" ht="75">
       <c r="A458" s="25" t="s">
         <v>222</v>
       </c>
@@ -19494,7 +19523,7 @@
       </c>
       <c r="I476" s="27"/>
     </row>
-    <row r="477" spans="1:9" ht="45">
+    <row r="477" spans="1:9" ht="30">
       <c r="A477" s="18" t="s">
         <v>241</v>
       </c>
@@ -19648,7 +19677,7 @@
       </c>
       <c r="I482" s="27"/>
     </row>
-    <row r="483" spans="1:9" ht="300">
+    <row r="483" spans="1:9" ht="285">
       <c r="A483" s="25" t="s">
         <v>243</v>
       </c>
@@ -19823,7 +19852,7 @@
       </c>
       <c r="I489" s="27"/>
     </row>
-    <row r="490" spans="1:9" ht="255">
+    <row r="490" spans="1:9" ht="240">
       <c r="A490" s="25" t="s">
         <v>250</v>
       </c>
@@ -19898,7 +19927,7 @@
       </c>
       <c r="I492" s="27"/>
     </row>
-    <row r="493" spans="1:9" ht="30">
+    <row r="493" spans="1:9">
       <c r="A493" s="25" t="s">
         <v>253</v>
       </c>
@@ -20023,7 +20052,7 @@
       </c>
       <c r="I497" s="27"/>
     </row>
-    <row r="498" spans="1:9" ht="60">
+    <row r="498" spans="1:9" ht="45">
       <c r="A498" s="25" t="s">
         <v>344</v>
       </c>
@@ -20173,7 +20202,7 @@
       </c>
       <c r="I503" s="27"/>
     </row>
-    <row r="504" spans="1:9" ht="60">
+    <row r="504" spans="1:9" ht="45">
       <c r="A504" s="25" t="s">
         <v>350</v>
       </c>
@@ -20323,7 +20352,7 @@
       </c>
       <c r="I509" s="27"/>
     </row>
-    <row r="510" spans="1:9" ht="75">
+    <row r="510" spans="1:9" ht="60">
       <c r="A510" s="25" t="s">
         <v>356</v>
       </c>
@@ -20473,7 +20502,7 @@
       </c>
       <c r="I515" s="27"/>
     </row>
-    <row r="516" spans="1:9" ht="90">
+    <row r="516" spans="1:9" ht="75">
       <c r="A516" s="25" t="s">
         <v>362</v>
       </c>
@@ -20623,7 +20652,7 @@
       </c>
       <c r="I521" s="27"/>
     </row>
-    <row r="522" spans="1:9" ht="75">
+    <row r="522" spans="1:9" ht="60">
       <c r="A522" s="25" t="s">
         <v>368</v>
       </c>
@@ -20773,7 +20802,7 @@
       </c>
       <c r="I527" s="47"/>
     </row>
-    <row r="528" spans="1:9" ht="285">
+    <row r="528" spans="1:9" ht="255">
       <c r="A528" s="45" t="s">
         <v>1449</v>
       </c>
@@ -20798,7 +20827,7 @@
       </c>
       <c r="I528" s="47"/>
     </row>
-    <row r="529" spans="1:9" ht="30">
+    <row r="529" spans="1:9">
       <c r="A529" s="45" t="s">
         <v>1450</v>
       </c>
@@ -20973,7 +21002,7 @@
       </c>
       <c r="I535" s="47"/>
     </row>
-    <row r="536" spans="1:9" ht="60">
+    <row r="536" spans="1:9" ht="45">
       <c r="A536" s="45" t="s">
         <v>1456</v>
       </c>
@@ -21073,7 +21102,7 @@
       </c>
       <c r="I539" s="47"/>
     </row>
-    <row r="540" spans="1:9" ht="45">
+    <row r="540" spans="1:9" ht="30">
       <c r="A540" s="45" t="s">
         <v>1460</v>
       </c>
@@ -21148,7 +21177,7 @@
       </c>
       <c r="I542" s="47"/>
     </row>
-    <row r="543" spans="1:9" ht="120">
+    <row r="543" spans="1:9" ht="105">
       <c r="A543" s="45" t="s">
         <v>1463</v>
       </c>
@@ -21173,7 +21202,7 @@
       </c>
       <c r="I543" s="47"/>
     </row>
-    <row r="544" spans="1:9" ht="60">
+    <row r="544" spans="1:9" ht="45">
       <c r="A544" s="45" t="s">
         <v>1464</v>
       </c>
@@ -21198,7 +21227,7 @@
       </c>
       <c r="I544" s="47"/>
     </row>
-    <row r="545" spans="1:9" ht="45">
+    <row r="545" spans="1:9" ht="30">
       <c r="A545" s="45" t="s">
         <v>1465</v>
       </c>
@@ -21323,7 +21352,7 @@
       </c>
       <c r="I549" s="47"/>
     </row>
-    <row r="550" spans="1:9" ht="45">
+    <row r="550" spans="1:9" ht="30">
       <c r="A550" s="45" t="s">
         <v>1470</v>
       </c>
@@ -21373,7 +21402,7 @@
       </c>
       <c r="I551" s="47"/>
     </row>
-    <row r="552" spans="1:9" ht="45">
+    <row r="552" spans="1:9" ht="30">
       <c r="A552" s="45" t="s">
         <v>1472</v>
       </c>
@@ -21423,7 +21452,7 @@
       </c>
       <c r="I553" s="47"/>
     </row>
-    <row r="554" spans="1:9" ht="45">
+    <row r="554" spans="1:9" ht="30">
       <c r="A554" s="45" t="s">
         <v>1474</v>
       </c>
@@ -21623,7 +21652,7 @@
       </c>
       <c r="I561" s="47"/>
     </row>
-    <row r="562" spans="1:9" ht="30">
+    <row r="562" spans="1:9">
       <c r="A562" s="45" t="s">
         <v>1482</v>
       </c>
@@ -21773,7 +21802,7 @@
       </c>
       <c r="I567" s="47"/>
     </row>
-    <row r="568" spans="1:9" ht="240">
+    <row r="568" spans="1:9" ht="210">
       <c r="A568" s="45" t="s">
         <v>1488</v>
       </c>
@@ -21823,7 +21852,7 @@
       </c>
       <c r="I569" s="47"/>
     </row>
-    <row r="570" spans="1:9" ht="30">
+    <row r="570" spans="1:9">
       <c r="A570" s="45" t="s">
         <v>1490</v>
       </c>
@@ -21898,7 +21927,7 @@
       </c>
       <c r="I572" s="47"/>
     </row>
-    <row r="573" spans="1:9" ht="30">
+    <row r="573" spans="1:9">
       <c r="A573" s="45" t="s">
         <v>1493</v>
       </c>
@@ -21973,7 +22002,7 @@
       </c>
       <c r="I575" s="47"/>
     </row>
-    <row r="576" spans="1:9" ht="60">
+    <row r="576" spans="1:9" ht="45">
       <c r="A576" s="45" t="s">
         <v>1496</v>
       </c>
@@ -21998,7 +22027,7 @@
       </c>
       <c r="I576" s="47"/>
     </row>
-    <row r="577" spans="1:9" ht="45">
+    <row r="577" spans="1:9" ht="30">
       <c r="A577" s="45" t="s">
         <v>1497</v>
       </c>
@@ -22073,7 +22102,7 @@
       </c>
       <c r="I579" s="47"/>
     </row>
-    <row r="580" spans="1:9" ht="45">
+    <row r="580" spans="1:9" ht="30">
       <c r="A580" s="45" t="s">
         <v>1500</v>
       </c>
@@ -22248,7 +22277,7 @@
         <v>15</v>
       </c>
       <c r="H586" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I586" s="47"/>
     </row>
@@ -22277,7 +22306,7 @@
       </c>
       <c r="I587" s="47"/>
     </row>
-    <row r="588" spans="1:9" ht="45">
+    <row r="588" spans="1:9" ht="30">
       <c r="A588" s="45" t="s">
         <v>1506</v>
       </c>
@@ -22327,7 +22356,7 @@
       </c>
       <c r="I589" s="47"/>
     </row>
-    <row r="590" spans="1:9" ht="45">
+    <row r="590" spans="1:9" ht="30">
       <c r="A590" s="45" t="s">
         <v>1508</v>
       </c>
@@ -22402,7 +22431,7 @@
       </c>
       <c r="I592" s="47"/>
     </row>
-    <row r="593" spans="1:9" ht="30">
+    <row r="593" spans="1:9">
       <c r="A593" s="45" t="s">
         <v>1511</v>
       </c>
@@ -22427,7 +22456,7 @@
       </c>
       <c r="I593" s="47"/>
     </row>
-    <row r="594" spans="1:9" ht="240">
+    <row r="594" spans="1:9" ht="225">
       <c r="A594" s="45" t="s">
         <v>1512</v>
       </c>
@@ -22779,7 +22808,7 @@
       </c>
       <c r="I607" s="47"/>
     </row>
-    <row r="608" spans="1:9" ht="30">
+    <row r="608" spans="1:9">
       <c r="A608" s="45" t="s">
         <v>1526</v>
       </c>
@@ -22804,14 +22833,14 @@
       </c>
       <c r="I608" s="47"/>
     </row>
-    <row r="609" spans="1:9" ht="45">
+    <row r="609" spans="1:9" ht="30">
       <c r="A609" s="45" t="s">
         <v>1527</v>
       </c>
       <c r="B609" s="46" t="s">
         <v>1390</v>
       </c>
-      <c r="C609" s="47" t="s">
+      <c r="C609" s="16" t="s">
         <v>1394</v>
       </c>
       <c r="D609" s="45"/>
@@ -22825,7 +22854,7 @@
         <v>15</v>
       </c>
       <c r="H609" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I609" s="47"/>
     </row>
@@ -22854,7 +22883,7 @@
       </c>
       <c r="I610" s="47"/>
     </row>
-    <row r="611" spans="1:9" ht="30">
+    <row r="611" spans="1:9">
       <c r="A611" s="45" t="s">
         <v>1529</v>
       </c>
@@ -22954,7 +22983,7 @@
       </c>
       <c r="I614" s="47"/>
     </row>
-    <row r="615" spans="1:9" ht="60">
+    <row r="615" spans="1:9" ht="45">
       <c r="A615" s="45" t="s">
         <v>1533</v>
       </c>
@@ -23129,7 +23158,7 @@
       </c>
       <c r="I621" s="47"/>
     </row>
-    <row r="622" spans="1:9" ht="120">
+    <row r="622" spans="1:9" ht="105">
       <c r="A622" s="45" t="s">
         <v>1540</v>
       </c>
@@ -23154,7 +23183,7 @@
       </c>
       <c r="I622" s="47"/>
     </row>
-    <row r="623" spans="1:9" ht="60">
+    <row r="623" spans="1:9" ht="45">
       <c r="A623" s="45" t="s">
         <v>1541</v>
       </c>
@@ -23179,7 +23208,7 @@
       </c>
       <c r="I623" s="47"/>
     </row>
-    <row r="624" spans="1:9" ht="45">
+    <row r="624" spans="1:9" ht="30">
       <c r="A624" s="45" t="s">
         <v>1542</v>
       </c>
@@ -23304,7 +23333,7 @@
       </c>
       <c r="I628" s="47"/>
     </row>
-    <row r="629" spans="1:9" ht="45">
+    <row r="629" spans="1:9" ht="30">
       <c r="A629" s="45" t="s">
         <v>1547</v>
       </c>
@@ -23479,7 +23508,7 @@
       </c>
       <c r="I635" s="47"/>
     </row>
-    <row r="636" spans="1:9" ht="60">
+    <row r="636" spans="1:9" ht="45">
       <c r="A636" s="45" t="s">
         <v>1554</v>
       </c>
@@ -23504,7 +23533,7 @@
       </c>
       <c r="I636" s="47"/>
     </row>
-    <row r="637" spans="1:9" ht="30">
+    <row r="637" spans="1:9">
       <c r="A637" s="45" t="s">
         <v>1555</v>
       </c>
@@ -23629,7 +23658,7 @@
       </c>
       <c r="I641" s="47"/>
     </row>
-    <row r="642" spans="1:9" ht="225">
+    <row r="642" spans="1:9" ht="195">
       <c r="A642" s="45" t="s">
         <v>1560</v>
       </c>
@@ -23829,7 +23858,7 @@
       </c>
       <c r="I649" s="47"/>
     </row>
-    <row r="650" spans="1:9" ht="30">
+    <row r="650" spans="1:9">
       <c r="A650" s="45" t="s">
         <v>1568</v>
       </c>
@@ -23879,7 +23908,7 @@
       </c>
       <c r="I651" s="47"/>
     </row>
-    <row r="652" spans="1:9" ht="45">
+    <row r="652" spans="1:9" ht="30">
       <c r="A652" s="45" t="s">
         <v>1570</v>
       </c>
@@ -23904,7 +23933,7 @@
       </c>
       <c r="I652" s="47"/>
     </row>
-    <row r="653" spans="1:9" ht="45">
+    <row r="653" spans="1:9" ht="30">
       <c r="A653" s="45" t="s">
         <v>1571</v>
       </c>
@@ -23954,7 +23983,7 @@
       </c>
       <c r="I654" s="47"/>
     </row>
-    <row r="655" spans="1:9" ht="60">
+    <row r="655" spans="1:9" ht="45">
       <c r="A655" s="18" t="s">
         <v>371</v>
       </c>
@@ -24033,7 +24062,7 @@
       </c>
       <c r="I657" s="27"/>
     </row>
-    <row r="658" spans="1:9" ht="60">
+    <row r="658" spans="1:9" ht="45">
       <c r="A658" s="18" t="s">
         <v>624</v>
       </c>
@@ -24060,7 +24089,7 @@
       </c>
       <c r="I658" s="47"/>
     </row>
-    <row r="659" spans="1:9" ht="45">
+    <row r="659" spans="1:9" ht="30">
       <c r="A659" s="45" t="s">
         <v>626</v>
       </c>
@@ -24087,7 +24116,7 @@
       </c>
       <c r="I659" s="47"/>
     </row>
-    <row r="660" spans="1:9" ht="60">
+    <row r="660" spans="1:9" ht="45">
       <c r="A660" s="18" t="s">
         <v>373</v>
       </c>
@@ -24141,7 +24170,7 @@
       </c>
       <c r="I661" s="27"/>
     </row>
-    <row r="662" spans="1:9" ht="90">
+    <row r="662" spans="1:9" ht="75">
       <c r="A662" s="25" t="s">
         <v>375</v>
       </c>
@@ -24168,7 +24197,7 @@
       </c>
       <c r="I662" s="27"/>
     </row>
-    <row r="663" spans="1:9" ht="75">
+    <row r="663" spans="1:9" ht="60">
       <c r="A663" s="18" t="s">
         <v>376</v>
       </c>
@@ -24195,7 +24224,7 @@
       </c>
       <c r="I663" s="27"/>
     </row>
-    <row r="664" spans="1:9" ht="45">
+    <row r="664" spans="1:9" ht="30">
       <c r="A664" s="45" t="s">
         <v>719</v>
       </c>
@@ -24307,7 +24336,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="668" spans="1:9" ht="60">
+    <row r="668" spans="1:9" ht="45">
       <c r="A668" s="45" t="s">
         <v>878</v>
       </c>
@@ -24811,7 +24840,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="686" spans="1:9" ht="60">
+    <row r="686" spans="1:9" ht="45">
       <c r="A686" s="45" t="s">
         <v>959</v>
       </c>
@@ -25060,7 +25089,7 @@
       </c>
       <c r="I694" s="47"/>
     </row>
-    <row r="695" spans="1:9" ht="45">
+    <row r="695" spans="1:9" ht="30">
       <c r="A695" s="45" t="s">
         <v>968</v>
       </c>
@@ -25087,7 +25116,7 @@
       </c>
       <c r="I695" s="47"/>
     </row>
-    <row r="696" spans="1:9" ht="60">
+    <row r="696" spans="1:9" ht="45">
       <c r="A696" s="45" t="s">
         <v>969</v>
       </c>
@@ -25114,7 +25143,7 @@
       </c>
       <c r="I696" s="47"/>
     </row>
-    <row r="697" spans="1:9" ht="45">
+    <row r="697" spans="1:9" ht="30">
       <c r="A697" s="45" t="s">
         <v>970</v>
       </c>
@@ -25359,7 +25388,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="706" spans="1:9" ht="60">
+    <row r="706" spans="1:9" ht="45">
       <c r="A706" s="45" t="s">
         <v>979</v>
       </c>
@@ -25415,7 +25444,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="708" spans="1:9" ht="45">
+    <row r="708" spans="1:9" ht="30">
       <c r="A708" s="45" t="s">
         <v>981</v>
       </c>
@@ -25583,7 +25612,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="714" spans="1:9" ht="60">
+    <row r="714" spans="1:9" ht="45">
       <c r="A714" s="45" t="s">
         <v>987</v>
       </c>
@@ -25639,7 +25668,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="716" spans="1:9" ht="60">
+    <row r="716" spans="1:9" ht="45">
       <c r="A716" s="45" t="s">
         <v>989</v>
       </c>
@@ -25863,7 +25892,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="724" spans="1:9" ht="45">
+    <row r="724" spans="1:9" ht="30">
       <c r="A724" s="45" t="s">
         <v>997</v>
       </c>
@@ -25919,7 +25948,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="726" spans="1:9" ht="45">
+    <row r="726" spans="1:9" ht="30">
       <c r="A726" s="45" t="s">
         <v>999</v>
       </c>
@@ -26218,7 +26247,7 @@
       </c>
       <c r="I736" s="47"/>
     </row>
-    <row r="737" spans="1:9" ht="30">
+    <row r="737" spans="1:9">
       <c r="A737" s="18" t="s">
         <v>1613</v>
       </c>
@@ -26268,7 +26297,7 @@
       </c>
       <c r="I738" s="47"/>
     </row>
-    <row r="739" spans="1:9" ht="30">
+    <row r="739" spans="1:9">
       <c r="A739" s="18" t="s">
         <v>1615</v>
       </c>
@@ -26318,7 +26347,7 @@
       </c>
       <c r="I740" s="47"/>
     </row>
-    <row r="741" spans="1:9" ht="30">
+    <row r="741" spans="1:9">
       <c r="A741" s="18" t="s">
         <v>1617</v>
       </c>
@@ -26443,7 +26472,7 @@
       </c>
       <c r="I745" s="27"/>
     </row>
-    <row r="746" spans="1:9" ht="165">
+    <row r="746" spans="1:9" ht="150">
       <c r="A746" s="18" t="s">
         <v>384</v>
       </c>
@@ -26568,7 +26597,7 @@
       </c>
       <c r="I750" s="27"/>
     </row>
-    <row r="751" spans="1:9" ht="195">
+    <row r="751" spans="1:9" ht="180">
       <c r="A751" s="25" t="s">
         <v>377</v>
       </c>
@@ -26668,7 +26697,7 @@
       </c>
       <c r="I754" s="27"/>
     </row>
-    <row r="755" spans="1:9" ht="45">
+    <row r="755" spans="1:9" ht="30">
       <c r="A755" s="25" t="s">
         <v>381</v>
       </c>
@@ -26693,7 +26722,7 @@
       </c>
       <c r="I755" s="27"/>
     </row>
-    <row r="756" spans="1:9" ht="45">
+    <row r="756" spans="1:9" ht="30">
       <c r="A756" s="18" t="s">
         <v>382</v>
       </c>
@@ -26739,11 +26768,11 @@
         <v>15</v>
       </c>
       <c r="H757" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I757" s="47"/>
     </row>
-    <row r="758" spans="1:9" ht="45">
+    <row r="758" spans="1:9" ht="30">
       <c r="A758" s="18" t="s">
         <v>1597</v>
       </c>
@@ -26764,7 +26793,7 @@
         <v>15</v>
       </c>
       <c r="H758" s="45" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I758" s="47"/>
     </row>
@@ -26863,105 +26892,4 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all/>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/office/internal/2005/internalDocumentation" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type" ma:readOnly="true"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="lastPrinted" minOccurs="0" maxOccurs="1" type="xsd:dateTime"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update RS of MS-OXWSCONT .
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9CCC2A-DBB7-429F-B979-030668CB1256}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C8F64C-274E-42B7-A76E-EB14861FC315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$778</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$780</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5506" uniqueCount="1721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5521" uniqueCount="1726">
   <si>
     <t>Req ID</t>
   </si>
@@ -6535,6 +6535,21 @@
   </si>
   <si>
     <t>2.2.3.10</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R1275123</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R1275124</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the ContentType element.. (&lt;65&gt; Section 3.1.4.7.3.2:  Exchange 2007,and Exchange 2010  do not support the ContentType element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support  the ContentType element. (Exchange 2013 and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R302156:i</t>
   </si>
 </sst>
 </file>
@@ -6910,6 +6925,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6966,9 +6984,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -7467,8 +7482,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I778" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
-  <autoFilter ref="A19:I778" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I780" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+  <autoFilter ref="A19:I780" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -7836,10 +7851,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M781"/>
+  <dimension ref="A1:M783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C778" sqref="C778"/>
+    <sheetView tabSelected="1" topLeftCell="D747" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I753" sqref="I753"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -7905,16 +7920,16 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="21">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
       <c r="I4" s="32"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -7926,13 +7941,13 @@
       <c r="B5" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="55"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="56"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
@@ -7940,16 +7955,16 @@
       <c r="A6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="54"/>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="55"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
@@ -7957,16 +7972,16 @@
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
@@ -7974,16 +7989,16 @@
       <c r="A8" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
@@ -7991,16 +8006,16 @@
       <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
     </row>
@@ -8008,16 +8023,16 @@
       <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="62"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="63"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
     </row>
@@ -8025,16 +8040,16 @@
       <c r="A11" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="63" t="s">
+      <c r="B11" s="64" t="s">
         <v>594</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="51"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="52"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
@@ -8118,16 +8133,16 @@
       <c r="A16" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="51"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="52"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
@@ -8135,16 +8150,16 @@
       <c r="A17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="67" t="s">
+      <c r="B17" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
@@ -8152,16 +8167,16 @@
       <c r="A18" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="50" t="s">
         <v>595</v>
       </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="50"/>
-      <c r="H18" s="50"/>
-      <c r="I18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="M18" s="4"/>
@@ -22762,7 +22777,7 @@
         <v>15</v>
       </c>
       <c r="H599" s="45" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I599" s="47"/>
     </row>
@@ -23264,7 +23279,7 @@
       <c r="H619" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="I619" s="47" t="s">
+      <c r="I619" s="16" t="s">
         <v>1480</v>
       </c>
     </row>
@@ -24530,7 +24545,7 @@
       <c r="A670" s="18" t="s">
         <v>1642</v>
       </c>
-      <c r="B670" s="68">
+      <c r="B670" s="49">
         <v>8</v>
       </c>
       <c r="C670" s="16" t="s">
@@ -24557,7 +24572,7 @@
       <c r="A671" s="18" t="s">
         <v>1643</v>
       </c>
-      <c r="B671" s="68">
+      <c r="B671" s="49">
         <v>8</v>
       </c>
       <c r="C671" s="16" t="s">
@@ -24576,7 +24591,7 @@
         <v>15</v>
       </c>
       <c r="H671" s="45" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I671" s="47"/>
     </row>
@@ -25447,7 +25462,7 @@
       <c r="A703" s="18" t="s">
         <v>849</v>
       </c>
-      <c r="B703" s="68">
+      <c r="B703" s="49">
         <v>8</v>
       </c>
       <c r="C703" s="16" t="s">
@@ -25476,7 +25491,7 @@
       <c r="A704" s="18" t="s">
         <v>1700</v>
       </c>
-      <c r="B704" s="68">
+      <c r="B704" s="49">
         <v>8</v>
       </c>
       <c r="C704" s="16" t="s">
@@ -25503,7 +25518,7 @@
       <c r="A705" s="18" t="s">
         <v>1701</v>
       </c>
-      <c r="B705" s="68">
+      <c r="B705" s="49">
         <v>8</v>
       </c>
       <c r="C705" s="16" t="s">
@@ -25532,7 +25547,7 @@
       <c r="A706" s="18" t="s">
         <v>1702</v>
       </c>
-      <c r="B706" s="68">
+      <c r="B706" s="49">
         <v>8</v>
       </c>
       <c r="C706" s="16" t="s">
@@ -25559,7 +25574,7 @@
       <c r="A707" s="18" t="s">
         <v>1703</v>
       </c>
-      <c r="B707" s="68">
+      <c r="B707" s="49">
         <v>8</v>
       </c>
       <c r="C707" s="16" t="s">
@@ -25588,7 +25603,7 @@
       <c r="A708" s="18" t="s">
         <v>1704</v>
       </c>
-      <c r="B708" s="68">
+      <c r="B708" s="49">
         <v>8</v>
       </c>
       <c r="C708" s="16" t="s">
@@ -25615,7 +25630,7 @@
       <c r="A709" s="18" t="s">
         <v>1705</v>
       </c>
-      <c r="B709" s="68">
+      <c r="B709" s="49">
         <v>8</v>
       </c>
       <c r="C709" s="16" t="s">
@@ -25644,7 +25659,7 @@
       <c r="A710" s="18" t="s">
         <v>1706</v>
       </c>
-      <c r="B710" s="68">
+      <c r="B710" s="49">
         <v>8</v>
       </c>
       <c r="C710" s="16" t="s">
@@ -25671,7 +25686,7 @@
       <c r="A711" s="18" t="s">
         <v>1707</v>
       </c>
-      <c r="B711" s="68">
+      <c r="B711" s="49">
         <v>8</v>
       </c>
       <c r="C711" s="16" t="s">
@@ -26782,7 +26797,7 @@
       <c r="B751" s="46" t="s">
         <v>615</v>
       </c>
-      <c r="C751" s="47" t="s">
+      <c r="C751" s="16" t="s">
         <v>1668</v>
       </c>
       <c r="D751" s="45" t="s">
@@ -26800,22 +26815,22 @@
       <c r="H751" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I751" s="47" t="s">
+      <c r="I751" s="16" t="s">
         <v>1493</v>
       </c>
     </row>
     <row r="752" spans="1:9" ht="45">
-      <c r="A752" s="45" t="s">
-        <v>890</v>
-      </c>
-      <c r="B752" s="46" t="s">
-        <v>615</v>
+      <c r="A752" s="18" t="s">
+        <v>1721</v>
+      </c>
+      <c r="B752" s="49">
+        <v>8</v>
       </c>
       <c r="C752" s="16" t="s">
-        <v>1699</v>
-      </c>
-      <c r="D752" t="s">
-        <v>1512</v>
+        <v>1723</v>
+      </c>
+      <c r="D752" s="18" t="s">
+        <v>1725</v>
       </c>
       <c r="E752" s="45" t="s">
         <v>22</v>
@@ -26832,17 +26847,17 @@
       <c r="I752" s="47"/>
     </row>
     <row r="753" spans="1:9" ht="45">
-      <c r="A753" s="45" t="s">
-        <v>891</v>
-      </c>
-      <c r="B753" s="46" t="s">
-        <v>615</v>
-      </c>
-      <c r="C753" s="47" t="s">
-        <v>834</v>
-      </c>
-      <c r="D753" t="s">
-        <v>1512</v>
+      <c r="A753" s="18" t="s">
+        <v>1722</v>
+      </c>
+      <c r="B753" s="49">
+        <v>8</v>
+      </c>
+      <c r="C753" s="16" t="s">
+        <v>1724</v>
+      </c>
+      <c r="D753" s="18" t="s">
+        <v>1725</v>
       </c>
       <c r="E753" s="45" t="s">
         <v>22</v>
@@ -26860,19 +26875,21 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="754" spans="1:9" ht="390">
+    <row r="754" spans="1:9" ht="45">
       <c r="A754" s="18" t="s">
-        <v>1448</v>
-      </c>
-      <c r="B754" s="20" t="s">
-        <v>1720</v>
+        <v>890</v>
+      </c>
+      <c r="B754" s="46" t="s">
+        <v>615</v>
       </c>
       <c r="C754" s="16" t="s">
-        <v>1437</v>
-      </c>
-      <c r="D754" s="45"/>
+        <v>1699</v>
+      </c>
+      <c r="D754" t="s">
+        <v>1512</v>
+      </c>
       <c r="E754" s="45" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F754" s="45" t="s">
         <v>3</v>
@@ -26881,23 +26898,25 @@
         <v>15</v>
       </c>
       <c r="H754" s="45" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I754" s="47"/>
     </row>
-    <row r="755" spans="1:9" ht="30">
-      <c r="A755" s="18" t="s">
-        <v>1449</v>
-      </c>
-      <c r="B755" s="20" t="s">
-        <v>1720</v>
+    <row r="755" spans="1:9" ht="45">
+      <c r="A755" s="45" t="s">
+        <v>891</v>
+      </c>
+      <c r="B755" s="46" t="s">
+        <v>615</v>
       </c>
       <c r="C755" s="47" t="s">
-        <v>1438</v>
-      </c>
-      <c r="D755" s="45"/>
+        <v>834</v>
+      </c>
+      <c r="D755" t="s">
+        <v>1512</v>
+      </c>
       <c r="E755" s="45" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F755" s="45" t="s">
         <v>3</v>
@@ -26908,17 +26927,19 @@
       <c r="H755" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="I755" s="47"/>
-    </row>
-    <row r="756" spans="1:9" ht="30">
+      <c r="I755" s="16" t="s">
+        <v>1493</v>
+      </c>
+    </row>
+    <row r="756" spans="1:9" ht="390">
       <c r="A756" s="18" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="B756" s="20" t="s">
         <v>1720</v>
       </c>
-      <c r="C756" s="47" t="s">
-        <v>1439</v>
+      <c r="C756" s="16" t="s">
+        <v>1437</v>
       </c>
       <c r="D756" s="45"/>
       <c r="E756" s="45" t="s">
@@ -26935,15 +26956,15 @@
       </c>
       <c r="I756" s="47"/>
     </row>
-    <row r="757" spans="1:9">
+    <row r="757" spans="1:9" ht="30">
       <c r="A757" s="18" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="B757" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C757" s="47" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="D757" s="45"/>
       <c r="E757" s="45" t="s">
@@ -26962,13 +26983,13 @@
     </row>
     <row r="758" spans="1:9" ht="30">
       <c r="A758" s="18" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="B758" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C758" s="47" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
       <c r="D758" s="45"/>
       <c r="E758" s="45" t="s">
@@ -26987,13 +27008,13 @@
     </row>
     <row r="759" spans="1:9">
       <c r="A759" s="18" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="B759" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C759" s="47" t="s">
-        <v>1447</v>
+        <v>1440</v>
       </c>
       <c r="D759" s="45"/>
       <c r="E759" s="45" t="s">
@@ -27012,13 +27033,13 @@
     </row>
     <row r="760" spans="1:9" ht="30">
       <c r="A760" s="18" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="B760" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C760" s="47" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="D760" s="45"/>
       <c r="E760" s="45" t="s">
@@ -27037,13 +27058,13 @@
     </row>
     <row r="761" spans="1:9">
       <c r="A761" s="18" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="B761" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C761" s="47" t="s">
-        <v>1446</v>
+        <v>1447</v>
       </c>
       <c r="D761" s="45"/>
       <c r="E761" s="45" t="s">
@@ -27062,13 +27083,13 @@
     </row>
     <row r="762" spans="1:9" ht="30">
       <c r="A762" s="18" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="B762" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C762" s="47" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="D762" s="45"/>
       <c r="E762" s="45" t="s">
@@ -27085,15 +27106,15 @@
       </c>
       <c r="I762" s="47"/>
     </row>
-    <row r="763" spans="1:9" ht="30">
+    <row r="763" spans="1:9">
       <c r="A763" s="18" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="B763" s="20" t="s">
         <v>1720</v>
       </c>
       <c r="C763" s="47" t="s">
-        <v>1445</v>
+        <v>1446</v>
       </c>
       <c r="D763" s="45"/>
       <c r="E763" s="45" t="s">
@@ -27110,15 +27131,15 @@
       </c>
       <c r="I763" s="47"/>
     </row>
-    <row r="764" spans="1:9" ht="45">
+    <row r="764" spans="1:9" ht="30">
       <c r="A764" s="18" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="B764" s="20" t="s">
         <v>1720</v>
       </c>
-      <c r="C764" s="16" t="s">
-        <v>1444</v>
+      <c r="C764" s="47" t="s">
+        <v>1443</v>
       </c>
       <c r="D764" s="45"/>
       <c r="E764" s="45" t="s">
@@ -27135,90 +27156,90 @@
       </c>
       <c r="I764" s="47"/>
     </row>
-    <row r="765" spans="1:9" ht="180">
-      <c r="A765" s="25" t="s">
+    <row r="765" spans="1:9" ht="30">
+      <c r="A765" s="18" t="s">
+        <v>1457</v>
+      </c>
+      <c r="B765" s="20" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C765" s="47" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D765" s="45"/>
+      <c r="E765" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F765" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G765" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H765" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I765" s="47"/>
+    </row>
+    <row r="766" spans="1:9" ht="45">
+      <c r="A766" s="18" t="s">
+        <v>1458</v>
+      </c>
+      <c r="B766" s="20" t="s">
+        <v>1720</v>
+      </c>
+      <c r="C766" s="16" t="s">
+        <v>1444</v>
+      </c>
+      <c r="D766" s="45"/>
+      <c r="E766" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F766" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G766" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H766" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I766" s="47"/>
+    </row>
+    <row r="767" spans="1:9" ht="180">
+      <c r="A767" s="25" t="s">
         <v>383</v>
       </c>
-      <c r="B765" s="20" t="s">
+      <c r="B767" s="20" t="s">
         <v>420</v>
       </c>
-      <c r="C765" s="16" t="s">
+      <c r="C767" s="16" t="s">
         <v>586</v>
       </c>
-      <c r="D765" s="25"/>
-      <c r="E765" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F765" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G765" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H765" s="25" t="s">
+      <c r="D767" s="25"/>
+      <c r="E767" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F767" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G767" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H767" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I765" s="27"/>
-    </row>
-    <row r="766" spans="1:9" ht="150">
-      <c r="A766" s="18" t="s">
+      <c r="I767" s="27"/>
+    </row>
+    <row r="768" spans="1:9" ht="150">
+      <c r="A768" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="B766" s="20" t="s">
+      <c r="B768" s="20" t="s">
         <v>1429</v>
       </c>
-      <c r="C766" s="16" t="s">
+      <c r="C768" s="16" t="s">
         <v>587</v>
-      </c>
-      <c r="D766" s="25"/>
-      <c r="E766" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F766" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G766" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H766" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I766" s="27"/>
-    </row>
-    <row r="767" spans="1:9" ht="135">
-      <c r="A767" s="45" t="s">
-        <v>1423</v>
-      </c>
-      <c r="B767" s="46" t="s">
-        <v>1422</v>
-      </c>
-      <c r="C767" s="47" t="s">
-        <v>1424</v>
-      </c>
-      <c r="D767" s="45"/>
-      <c r="E767" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F767" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G767" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H767" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="I767" s="47"/>
-    </row>
-    <row r="768" spans="1:9" ht="409.5">
-      <c r="A768" s="25" t="s">
-        <v>385</v>
-      </c>
-      <c r="B768" s="20" t="s">
-        <v>1430</v>
-      </c>
-      <c r="C768" s="16" t="s">
-        <v>588</v>
       </c>
       <c r="D768" s="25"/>
       <c r="E768" s="25" t="s">
@@ -27231,19 +27252,19 @@
         <v>15</v>
       </c>
       <c r="H768" s="25" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I768" s="27"/>
     </row>
-    <row r="769" spans="1:9" ht="409.5">
-      <c r="A769" s="18" t="s">
-        <v>1459</v>
+    <row r="769" spans="1:9" ht="135">
+      <c r="A769" s="45" t="s">
+        <v>1423</v>
       </c>
       <c r="B769" s="46" t="s">
-        <v>1431</v>
+        <v>1422</v>
       </c>
       <c r="C769" s="47" t="s">
-        <v>1460</v>
+        <v>1424</v>
       </c>
       <c r="D769" s="45"/>
       <c r="E769" s="45" t="s">
@@ -27260,15 +27281,15 @@
       </c>
       <c r="I769" s="47"/>
     </row>
-    <row r="770" spans="1:9" ht="135">
+    <row r="770" spans="1:9" ht="409.5">
       <c r="A770" s="25" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B770" s="20" t="s">
-        <v>1425</v>
+        <v>1430</v>
       </c>
       <c r="C770" s="16" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D770" s="25"/>
       <c r="E770" s="25" t="s">
@@ -27285,40 +27306,40 @@
       </c>
       <c r="I770" s="27"/>
     </row>
-    <row r="771" spans="1:9" ht="180">
-      <c r="A771" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="B771" s="20" t="s">
-        <v>1426</v>
-      </c>
-      <c r="C771" s="16" t="s">
-        <v>580</v>
-      </c>
-      <c r="D771" s="25"/>
-      <c r="E771" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F771" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G771" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="H771" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="I771" s="27"/>
-    </row>
-    <row r="772" spans="1:9" ht="30">
-      <c r="A772" s="18" t="s">
-        <v>378</v>
+    <row r="771" spans="1:9" ht="409.5">
+      <c r="A771" s="18" t="s">
+        <v>1459</v>
+      </c>
+      <c r="B771" s="46" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C771" s="47" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D771" s="45"/>
+      <c r="E771" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F771" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G771" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H771" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="I771" s="47"/>
+    </row>
+    <row r="772" spans="1:9" ht="135">
+      <c r="A772" s="25" t="s">
+        <v>386</v>
       </c>
       <c r="B772" s="20" t="s">
-        <v>1427</v>
+        <v>1425</v>
       </c>
       <c r="C772" s="16" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="D772" s="25"/>
       <c r="E772" s="25" t="s">
@@ -27331,19 +27352,19 @@
         <v>15</v>
       </c>
       <c r="H772" s="25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I772" s="27"/>
     </row>
-    <row r="773" spans="1:9" ht="105">
+    <row r="773" spans="1:9" ht="180">
       <c r="A773" s="25" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B773" s="20" t="s">
-        <v>1427</v>
-      </c>
-      <c r="C773" s="27" t="s">
-        <v>582</v>
+        <v>1426</v>
+      </c>
+      <c r="C773" s="16" t="s">
+        <v>580</v>
       </c>
       <c r="D773" s="25"/>
       <c r="E773" s="25" t="s">
@@ -27360,15 +27381,15 @@
       </c>
       <c r="I773" s="27"/>
     </row>
-    <row r="774" spans="1:9" ht="45">
-      <c r="A774" s="25" t="s">
-        <v>380</v>
+    <row r="774" spans="1:9" ht="30">
+      <c r="A774" s="18" t="s">
+        <v>378</v>
       </c>
       <c r="B774" s="20" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="C774" s="16" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D774" s="25"/>
       <c r="E774" s="25" t="s">
@@ -27381,19 +27402,19 @@
         <v>15</v>
       </c>
       <c r="H774" s="25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I774" s="27"/>
     </row>
-    <row r="775" spans="1:9" ht="30">
+    <row r="775" spans="1:9" ht="105">
       <c r="A775" s="25" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B775" s="20" t="s">
-        <v>1428</v>
-      </c>
-      <c r="C775" s="16" t="s">
-        <v>584</v>
+        <v>1427</v>
+      </c>
+      <c r="C775" s="27" t="s">
+        <v>582</v>
       </c>
       <c r="D775" s="25"/>
       <c r="E775" s="25" t="s">
@@ -27410,15 +27431,15 @@
       </c>
       <c r="I775" s="27"/>
     </row>
-    <row r="776" spans="1:9" ht="30">
-      <c r="A776" s="18" t="s">
-        <v>382</v>
+    <row r="776" spans="1:9" ht="45">
+      <c r="A776" s="25" t="s">
+        <v>380</v>
       </c>
       <c r="B776" s="20" t="s">
         <v>1428</v>
       </c>
       <c r="C776" s="16" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D776" s="25"/>
       <c r="E776" s="25" t="s">
@@ -27431,38 +27452,38 @@
         <v>15</v>
       </c>
       <c r="H776" s="25" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I776" s="27"/>
     </row>
-    <row r="777" spans="1:9" ht="45">
-      <c r="A777" s="18" t="s">
-        <v>1434</v>
+    <row r="777" spans="1:9" ht="30">
+      <c r="A777" s="25" t="s">
+        <v>381</v>
       </c>
       <c r="B777" s="20" t="s">
         <v>1428</v>
       </c>
       <c r="C777" s="16" t="s">
-        <v>1435</v>
-      </c>
-      <c r="D777" s="45"/>
-      <c r="E777" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F777" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G777" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H777" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I777" s="47"/>
+        <v>584</v>
+      </c>
+      <c r="D777" s="25"/>
+      <c r="E777" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F777" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G777" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H777" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I777" s="27"/>
     </row>
     <row r="778" spans="1:9" ht="30">
       <c r="A778" s="18" t="s">
-        <v>1436</v>
+        <v>382</v>
       </c>
       <c r="B778" s="20" t="s">
         <v>1428</v>
@@ -27470,39 +27491,89 @@
       <c r="C778" s="16" t="s">
         <v>585</v>
       </c>
-      <c r="D778" s="45"/>
-      <c r="E778" s="45" t="s">
-        <v>19</v>
-      </c>
-      <c r="F778" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G778" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="H778" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I778" s="47"/>
-    </row>
-    <row r="779" spans="1:9">
-      <c r="A779" s="25"/>
-      <c r="B779" s="26"/>
-      <c r="C779" s="27"/>
-      <c r="D779" s="25"/>
-      <c r="E779" s="25"/>
-      <c r="F779" s="25"/>
-      <c r="G779" s="25"/>
-      <c r="H779" s="25"/>
-      <c r="I779" s="27"/>
-    </row>
-    <row r="780" spans="1:9">
-      <c r="A780" s="3"/>
-      <c r="B780" s="9"/>
+      <c r="D778" s="25"/>
+      <c r="E778" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F778" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="G778" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H778" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I778" s="27"/>
+    </row>
+    <row r="779" spans="1:9" ht="45">
+      <c r="A779" s="18" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B779" s="20" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C779" s="16" t="s">
+        <v>1435</v>
+      </c>
+      <c r="D779" s="45"/>
+      <c r="E779" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F779" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G779" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H779" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I779" s="47"/>
+    </row>
+    <row r="780" spans="1:9" ht="30">
+      <c r="A780" s="18" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B780" s="20" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C780" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="D780" s="45"/>
+      <c r="E780" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F780" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G780" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="H780" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="I780" s="47"/>
     </row>
     <row r="781" spans="1:9">
-      <c r="A781" s="3"/>
-      <c r="B781" s="9"/>
+      <c r="A781" s="25"/>
+      <c r="B781" s="26"/>
+      <c r="C781" s="27"/>
+      <c r="D781" s="25"/>
+      <c r="E781" s="25"/>
+      <c r="F781" s="25"/>
+      <c r="G781" s="25"/>
+      <c r="H781" s="25"/>
+      <c r="I781" s="27"/>
+    </row>
+    <row r="782" spans="1:9">
+      <c r="A782" s="3"/>
+      <c r="B782" s="9"/>
+    </row>
+    <row r="783" spans="1:9">
+      <c r="A783" s="3"/>
+      <c r="B783" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -27519,7 +27590,7 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I779">
+  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I781">
     <cfRule type="expression" dxfId="7" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -27530,7 +27601,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I779">
+  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I781">
     <cfRule type="expression" dxfId="4" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -27541,7 +27612,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F779">
+  <conditionalFormatting sqref="F20:F781">
     <cfRule type="expression" dxfId="1" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -27550,20 +27621,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F712:F779 F20:F711" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F781" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E712:E779 E20:E711" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E781" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G712:G779 G20:G711" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G781" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H712:H779 H20:H711" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H781" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27573,7 +27644,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B780:B781 B10:B27 B54:B63 B28:B51 B65:B67 B70:B235 B244:B270 B273:B596 B598 B712:B753 B601:B669 B672:B702 B765:B778" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B782:B783 B10:B27 B54:B63 B28:B51 B65:B67 B70:B235 B244:B270 B273:B596 B598 B754:B755 B601:B669 B672:B702 B767:B780 B712:B751" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
update RS of MS-OXWSCONT
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C8F64C-274E-42B7-A76E-EB14861FC315}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320D61D7-9BF9-46B5-9B69-11C018B46989}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="19440" windowHeight="15000" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5521" uniqueCount="1726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5522" uniqueCount="1727">
   <si>
     <t>Req ID</t>
   </si>
@@ -6550,6 +6550,9 @@
   </si>
   <si>
     <t>MS-OXWSCONT_R302156:i</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R1275124.</t>
   </si>
 </sst>
 </file>
@@ -6991,50 +6994,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -7353,6 +7312,50 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -7482,34 +7485,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I780" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I780" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
   <autoFilter ref="A19:I780" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="7">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="6">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7518,12 +7521,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7853,8 +7856,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:M783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D747" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I753" sqref="I753"/>
+    <sheetView tabSelected="1" topLeftCell="D593" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I600" sqref="I600"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -22781,7 +22784,7 @@
       </c>
       <c r="I599" s="47"/>
     </row>
-    <row r="600" spans="1:9" ht="30">
+    <row r="600" spans="1:9" ht="45">
       <c r="A600" s="18" t="s">
         <v>1610</v>
       </c>
@@ -22791,7 +22794,7 @@
       <c r="C600" s="16" t="s">
         <v>1612</v>
       </c>
-      <c r="D600" s="45"/>
+      <c r="D600" s="18"/>
       <c r="E600" s="45" t="s">
         <v>19</v>
       </c>
@@ -22801,10 +22804,12 @@
       <c r="G600" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H600" s="45" t="s">
-        <v>18</v>
-      </c>
-      <c r="I600" s="47"/>
+      <c r="H600" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I600" s="16" t="s">
+        <v>1726</v>
+      </c>
     </row>
     <row r="601" spans="1:9" ht="30">
       <c r="A601" s="45" t="s">
@@ -23276,7 +23281,7 @@
       <c r="G619" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H619" s="45" t="s">
+      <c r="H619" s="18" t="s">
         <v>17</v>
       </c>
       <c r="I619" s="16" t="s">
@@ -27591,32 +27596,32 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I781">
-    <cfRule type="expression" dxfId="7" priority="53">
+    <cfRule type="expression" dxfId="24" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="23" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="61">
+    <cfRule type="expression" dxfId="22" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 A81:I270 B271:I271 A272:I781">
-    <cfRule type="expression" dxfId="4" priority="7">
+    <cfRule type="expression" dxfId="21" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="20" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:F781">
-    <cfRule type="expression" dxfId="1" priority="13">
+    <cfRule type="expression" dxfId="18" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
MS-OXWSCONT: Add adapter and test case for GetUserPhoto and SetUserPhoto operation.
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6ADACC-32A1-4D07-875C-56AF30B54D7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342097CB-1452-48FE-8402-1ADEC9FD6096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="16200" windowHeight="9360" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5527" uniqueCount="1739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5527" uniqueCount="1741">
   <si>
     <t>Req ID</t>
   </si>
@@ -5553,9 +5553,6 @@
 </t>
   </si>
   <si>
-    <t>[In GetUserPhotoResponseMessageType] This type [GetUserPhotoResponseMessageType] extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.67.</t>
-  </si>
-  <si>
     <t xml:space="preserve">[In GetUserPhotoResponseMessageType] The following is the GetUserPhotoResponseMessageType complex type specification. 
    &lt;xs:complexType name="GetUserPhotoResponseMessageType"&gt;
      &lt;xs:complexContent&gt;
@@ -5580,9 +5577,6 @@
     <t>MS-OXWSCONT_R302156</t>
   </si>
   <si>
-    <t>[In GetUserPhotoResponseMessageType] The type of the element ContentType is xs:string ([XMLSCHEMA2])</t>
-  </si>
-  <si>
     <t>[In GetUserPhotoResponseMessageType] ContentType element:Specifies the content (MIME) type of the photo.&lt;65&gt;</t>
   </si>
   <si>
@@ -5590,9 +5584,6 @@
   </si>
   <si>
     <t>[In Complex Types]  SetUserPhotoResponseMessageType: This complex type extends the ResponseMessageType complex type, as specified by [MS-OXWSCDATA] section 2.2.4.67.</t>
-  </si>
-  <si>
-    <t>[In SetUserPhotoResponseMessageType] This type extends the ResponseMessageType complex type, as specified by [MS-OXWSCDATA] section 2.2.4.67.</t>
   </si>
   <si>
     <t xml:space="preserve">[In SetUserPhotoResponseMessageType] The following is the SetUserPhotoResponseMessageType complex type specification. 
@@ -5983,18 +5974,6 @@
   </si>
   <si>
     <t>[In Appendix C: Product Behavior] Implementation does support the ContactUrlDictionaryType complex type. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[In t:ContactUrlDictionaryEntryType Complex Type]  The type [ContactUrlDictionaryEntryType] is defined as follow:
- &lt;xs:complexType name="ContactUrlDictionaryEntryType"&gt;
-   &lt;xs:sequence&gt;
-     &lt;xs:element name="Type" type="t:ContactUrlKeyType" minOccurs="1"/&gt;
-     &lt;xs:element name="Name" type="xs:string" minOccurs="0"/&gt;
-     &lt;xs:element name="Address" type="xs:string" minOccurs="0"/&gt;
-   &lt;/xs:sequence&gt;
- &lt;/xs:complexType&gt; 
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -6294,164 +6273,366 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the Urls element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element Urls is t:ContactUrlDictionaryType (section 3.1.4.1.1.9).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R120008:i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryType Complex Type] The type [ContactUrlDictionaryType] is defined as follow:
+&lt;xs:complexType name="ContactUrlDictionaryType"&gt;
+   &lt;xs:sequence&gt;
+     &lt;xs:element name="Url" type="t:ContactUrlDictionaryEntryType" maxOccurs="unbounded"/&gt;
+   &lt;/xs:sequence&gt;
+ &lt;/xs:complexType&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:CompleteNameType Complex Type] The type of the element of YomiLastName is xs:string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type] The type of the element Type is t:ContactUrlKeyType (section 3.1.4.1.2.2).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Type element: specifies the Url type.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type] The type of the element Name is xs:string ([XMLSCHEMA2]).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Name element: Specifies what the url is used for.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type]  The type of the element Address xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Address element: Specifies the Url.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryType Complex Type] The type of the element Url is t:ContactUrlDictionaryEntryType (section 3.1.4.1.1.8).</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactUrlDictionaryType Complex Type] Url element: Specifies a Url associated with a contact.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support element HasPicture. (Exchange 2010 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[In SetUserPhoto] The following is the WSDL port type specification of the SetUserPhoto WSDL operation.
+   &lt;wsdl:operation name="SetUserPhoto"&gt;
+     &lt;wsdl:input message="tns:SetUserPhotoSoapIn"/&gt;
+     &lt;wsdl:output message="tns:SetUserPhotoSoapOut"/&gt;
+   &lt;/wsdl:operation&gt;
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> [In t:AbchEmailAddressTypeType Simple Type] The type [AbchEmailAddressTypeType] is defined as follow:
+&lt;xs:simpleType name="AbchEmailAddressTypeType"&gt;
+   &lt;xs:restriction base="xs:string"&gt;
+     &lt;xs:enumeration value="Personal"/&gt;
+     &lt;xs:enumeration value="Business"/&gt;
+     &lt;xs:enumeration value="Other"/&gt;
+     &lt;xs:enumeration value="Passport"/&gt;
+   &lt;/xs:restriction&gt;
+ &lt;/xs:simpleType&gt; 
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the ContactUrlKeyType simple type. (&lt;55&gt; Section 3.1.4.1.2.2:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the ContactUrlKeyType simple type.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element SourceId is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] Gender element: Specifies the gender of the contact.&lt;11&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element Gender is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the SourceId element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the Cid element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element Cid is xs:long.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element SkypeId is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the SkypeId element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does introduce these elements [PhoneticFullName, PhoneticFirstName, PhoneticLastName, Alias, Notes, Photo, UserSMIMECertificate, MSExchangeCertificate, DirectoryId, ManagerMailbox, and DirectReports]. (&lt;4&gt; These elements were introduced in Exchange 2010 SP2 (and above).)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the DisplayNamePrefix  element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element DisplayNamePrefix is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element YomiSurname is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In t:ContactItemType Complex Type] The type of element YomiGivenName is xs:string.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the YomiGivenName  element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the YomiSurname element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-testable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R1275118.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R334068:i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R1275116.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R1275120.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R334070:i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R334072:i</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the YomiNickname element. (Exchange 2016 and above follow this behavior.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R336004.</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the ObjectId element. (&lt;13&gt; Section 2.2.4.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the ObjectId element.)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In GetUserPhotoResponseMessageType] This type [GetUserPhotoResponseMessageType] extends the ResponseMessageType complex type, as specified in [MS-OXWSCDATA] section 2.2.4.67.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In SetUserPhotoResponseMessageType] This type extends the ResponseMessageType complex type, as specified by [MS-OXWSCDATA] section 2.2.4.67.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Informative</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In GetUserPhotoResponseMessageType] The type of the element ContentType is xs:string ([XMLSCHEMA2])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>[In t:ContactItemType Complex Type] The type [ContactItemType] is defined as follow:
-  &lt;xs:complexType name="ContactItemType"&gt;
-   &lt;xs:complexContent&gt;
-     &lt;xs:extension
-       base="t:ItemType"
-     &gt;
-       &lt;xs:sequence&gt;
-         &lt;xs:element name="FileAs"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="FileAsMapping"
-           type="t:FileAsMappingType" 
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="DisplayName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="GivenName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Initials"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="MiddleName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Nickname"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="CompleteName"
-           type="t:CompleteNameType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="CompanyName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="EmailAddresses"
-           type="t:EmailAddressDictionaryType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="AbchEmailAddresses"
-           type="t:AbchEmailAddressDictionaryType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="PhysicalAddresses"
-           type="t:PhysicalAddressDictionaryType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="PhoneNumbers"
-           type="t:PhoneNumberDictionaryType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="AssistantName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Birthday"
-           type="xs:dateTime"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="BusinessHomePage"
-           type="xs:anyURI"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Children"
-           type="t:ArrayOfStringsType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Companies"
-           type="t:ArrayOfStringsType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="ContactSource"
-           type="t:ContactSourceType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Department"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Generation"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="ImAddresses"
-           type="t:ImAddressDictionaryType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="JobTitle"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Manager"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Mileage"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="OfficeLocation"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="PostalAddressIndex"
-           type="t:PhysicalAddressIndexType"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Profession"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="SpouseName"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="Surname"
-           type="xs:string"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="WeddingAnniversary"
-           type="xs:dateTime"
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="HasPicture"
-           type="xs:boolean" 
-           minOccurs="0"
-          /&gt;
-         &lt;xs:element name="PhoneticFullName" 
-           type="xs:string"
-           minOccurs="0" 
-         /&gt;
-         &lt;xs:element name="PhoneticFirstName" 
-           type="xs:string" 
-           minOccurs="0" 
-         /&gt;
-         &lt;xs:element name="PhoneticLastName" 
-           type="xs:string" 
-           minOccurs="0" 
-         /&gt;
-         &lt;xs:element name="Alias" 
-           type="xs:string" 
-           minOccurs="0" 
-         /&gt;
-         &lt;xs:element name="Notes" 
-           type="xs:string" 
-           minOccurs="0" 
-         /&gt;
-         &lt;xs:element name="Photo" 
-           type="xs:base64Binary" 
-           minOccurs="0" 
+  	&lt;xs:complexType name="ContactItemType"&gt;
+	  &lt;xs:complexContent&gt;
+	    &lt;xs:extension
+	      base="t:ItemType"
+	    &gt;
+	      &lt;xs:sequence&gt;
+	        &lt;xs:element name="FileAs"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="FileAsMapping"
+	          type="t:FileAsMappingType" 
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="DisplayName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="GivenName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Initials"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="MiddleName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Nickname"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="CompleteName"
+	          type="t:CompleteNameType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="CompanyName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="EmailAddresses"
+	          type="t:EmailAddressDictionaryType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="PhysicalAddresses"
+	          type="t:PhysicalAddressDictionaryType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="PhoneNumbers"
+	          type="t:PhoneNumberDictionaryType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="AssistantName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Birthday"
+	          type="xs:dateTime"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="BusinessHomePage"
+	          type="xs:anyURI"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Children"
+	          type="t:ArrayOfStringsType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Companies"
+	          type="t:ArrayOfStringsType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="ContactSource"
+	          type="t:ContactSourceType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Department"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Generation"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="ImAddresses"
+	          type="t:ImAddressDictionaryType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="JobTitle"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Manager"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Mileage"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="OfficeLocation"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="PostalAddressIndex"
+	          type="t:PhysicalAddressIndexType"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Profession"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="SpouseName"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="Surname"
+	          type="xs:string"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="WeddingAnniversary"
+	          type="xs:dateTime"
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="HasPicture"
+	          type="xs:boolean" 
+	          minOccurs="0"
+	         /&gt;
+	        &lt;xs:element name="PhoneticFullName" 
+	          type="xs:string"
+	          minOccurs="0" 
+	        /&gt;
+	        &lt;xs:element name="PhoneticFirstName" 
+	          type="xs:string" 
+	          minOccurs="0" 
+	        /&gt;
+	        &lt;xs:element name="PhoneticLastName" 
+	          type="xs:string" 
+	          minOccurs="0" 
+	        /&gt;
+	        &lt;xs:element name="Alias" 
+	          type="xs:string" 
+	          minOccurs="0" 
+	        /&gt;
+	        &lt;xs:element name="Notes" 
+	          type="xs:string" 
+	          minOccurs="0" 
+	        /&gt;
+	        &lt;xs:element name="Photo" 
+	          type="xs:base64Binary" 
+	          minOccurs="0" 
         /&gt;
         &lt;xs:element name="UserSMIMECertificate" 
           type="t:ArrayOfBinaryType" 
@@ -6512,10 +6693,6 @@
         &lt;xs:element name="PassportId" 
           type="xs:long" 
           minOccurs="0"
-        /&gt;
-        &lt;xs:element name="PersonId" 
-          type="t:ItemIdType" 
-          minOccurs="0"
         /&gt; 
         &lt;xs:element name="IsPrivate" 
           type="xs:boolean" 
@@ -6525,7 +6702,7 @@
           type="xs:string" 
           minOccurs="0"
         /&gt;
-&lt;xs:element name="TrustLevel" 
+        &lt;xs:element name="TrustLevel" 
           type="xs:int" 
           minOccurs="0"
         /&gt;
@@ -6536,7 +6713,11 @@
         &lt;xs:element name="Urls" 
           type="t:ContactUrlDictionaryType" 
           minOccurs="0"
-        /&gt;
+	        /&gt;
+	        &lt;xs:element name="AbchEmailAddresses"
+	          type="t:AbchEmailAddressDictionaryType"
+	          minOccurs="0"
+         /&gt;
         &lt;xs:element name="Cid" 
           type="xs:long" 
           minOccurs="0"
@@ -6592,7 +6773,7 @@
 	        &lt;xs:element name="Mris"
 	          type="t:ArrayOfStringsType" 
 	          minOccurs="0"
-        /&gt;
+	        /&gt;
 	        &lt;xs:element name="Wlid" 
 	          type="xs:string" 
 	          minOccurs="0"
@@ -6605,8 +6786,7 @@
 	           type="xs:boolean"
 	           minOccurs="0"
 	        /&gt;
-        &lt;
-	xs:element name="ShellContactType" 
+	        &lt;xs:element name="ShellContactType" 
 	           type="xs:string" 
 	           minOccurs="0"
 	        /&gt;
@@ -6645,7 +6825,11 @@
 	        &lt;xs:element name="PersonalNotes"  
 	           type="xs:string"
 	           minOccurs="0"
-	        /&gt; 
+	        /&gt;
+	        &lt;xs:element name="PersonId"
+	          type="t:ItemIdType" 
+	          minOccurs="0"
+	        /&gt;  
 	      &lt;/xs:sequence&gt;
 	    &lt;/xs:entension&gt;
 	  &lt;/xs:complexContent&gt;
@@ -6653,189 +6837,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the Urls element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element Urls is t:ContactUrlDictionaryType (section 3.1.4.1.1.9).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-OXWSCONT_R120008:i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryType Complex Type] The type [ContactUrlDictionaryType] is defined as follow:
-&lt;xs:complexType name="ContactUrlDictionaryType"&gt;
+    <t xml:space="preserve">[In t:ContactUrlDictionaryEntryType Complex Type]  The type [ContactUrlDictionaryEntryType] is defined as follow:
+ &lt;xs:complexType name="ContactUrlDictionaryEntryType"&gt;
    &lt;xs:sequence&gt;
-     &lt;xs:element name="Url" type="t:ContactUrlDictionaryEntryType" maxOccurs="unbounded"/&gt;
+     &lt;xs:element name="Type" type="t:ContactUrlKeyType" minOccurs="1"/&gt;
+     &lt;xs:element name="Address" type="xs:string" minOccurs="0"/&gt;
+     &lt;xs:element name="Name" type="xs:string" minOccurs="0"/&gt;
    &lt;/xs:sequence&gt;
- &lt;/xs:complexType&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:CompleteNameType Complex Type] The type of the element of YomiLastName is xs:string</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type] The type of the element Type is t:ContactUrlKeyType (section 3.1.4.1.2.2).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Type element: specifies the Url type.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type] The type of the element Name is xs:string ([XMLSCHEMA2]).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Name element: Specifies what the url is used for.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type]  The type of the element Address xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryEntryType Complex Type] Address element: Specifies the Url.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryType Complex Type] The type of the element Url is t:ContactUrlDictionaryEntryType (section 3.1.4.1.1.8).</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactUrlDictionaryType Complex Type] Url element: Specifies a Url associated with a contact.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support element HasPicture. (Exchange 2010 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">[In SetUserPhoto] The following is the WSDL port type specification of the SetUserPhoto WSDL operation.
-   &lt;wsdl:operation name="SetUserPhoto"&gt;
-     &lt;wsdl:input message="tns:SetUserPhotoSoapIn"/&gt;
-     &lt;wsdl:output message="tns:SetUserPhotoSoapOut"/&gt;
-   &lt;/wsdl:operation&gt;
+ &lt;/xs:complexType&gt; 
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> [In t:AbchEmailAddressTypeType Simple Type] The type [AbchEmailAddressTypeType] is defined as follow:
-&lt;xs:simpleType name="AbchEmailAddressTypeType"&gt;
-   &lt;xs:restriction base="xs:string"&gt;
-     &lt;xs:enumeration value="Personal"/&gt;
-     &lt;xs:enumeration value="Business"/&gt;
-     &lt;xs:enumeration value="Other"/&gt;
-     &lt;xs:enumeration value="Passport"/&gt;
-   &lt;/xs:restriction&gt;
- &lt;/xs:simpleType&gt; 
-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ContactUrlKeyType simple type. (&lt;55&gt; Section 3.1.4.1.2.2:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the ContactUrlKeyType simple type.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element SourceId is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] Gender element: Specifies the gender of the contact.&lt;11&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element Gender is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the SourceId element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the Cid element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element Cid is xs:long.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element SkypeId is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the SkypeId element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does introduce these elements [PhoneticFullName, PhoneticFirstName, PhoneticLastName, Alias, Notes, Photo, UserSMIMECertificate, MSExchangeCertificate, DirectoryId, ManagerMailbox, and DirectReports]. (&lt;4&gt; These elements were introduced in Exchange 2010 SP2 (and above).)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the DisplayNamePrefix  element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element DisplayNamePrefix is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element YomiSurname is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In t:ContactItemType Complex Type] The type of element YomiGivenName is xs:string.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the YomiGivenName  element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the YomiSurname element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Non-testable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXWSCONT_R1275118.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-OXWSCONT_R334068:i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXWSCONT_R1275116.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXWSCONT_R1275120.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-OXWSCONT_R334070:i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MS-OXWSCONT_R334072:i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does support the YomiNickname element. (Exchange 2016 and above follow this behavior.)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OXWSCONT_R336004.</t>
-  </si>
-  <si>
-    <t>[In Appendix C: Product Behavior] Implementation does not support the ObjectId element. (&lt;13&gt; Section 2.2.4.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the ObjectId element.)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7773,13 +7783,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I780" tableType="xml" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" connectionId="1">
-  <autoFilter ref="A19:I780" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="6">
-      <filters>
-        <filter val="Normative"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A19:I780" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -8153,10 +8157,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="9.75" style="3" customWidth="1"/>
-    <col min="3" max="3" width="65" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.75" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" customWidth="1"/>
+    <col min="3" max="3" width="85" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
@@ -8198,14 +8202,14 @@
         <v>25</v>
       </c>
       <c r="C3" s="35">
-        <v>15</v>
+        <v>15.1</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="34" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="36">
-        <v>43374</v>
+        <v>43732</v>
       </c>
       <c r="G3" s="37"/>
       <c r="H3" s="4"/>
@@ -8505,7 +8509,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A20" s="18" t="s">
         <v>42</v>
       </c>
@@ -8530,7 +8534,7 @@
       </c>
       <c r="I20" s="20"/>
     </row>
-    <row r="21" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A21" s="18" t="s">
         <v>43</v>
       </c>
@@ -8555,7 +8559,7 @@
       </c>
       <c r="I21" s="20"/>
     </row>
-    <row r="22" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A22" s="18" t="s">
         <v>44</v>
       </c>
@@ -8580,7 +8584,7 @@
       </c>
       <c r="I22" s="20"/>
     </row>
-    <row r="23" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="18" t="s">
         <v>45</v>
       </c>
@@ -8605,7 +8609,7 @@
       </c>
       <c r="I23" s="20"/>
     </row>
-    <row r="24" spans="1:13" s="19" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:13" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A24" s="18" t="s">
         <v>46</v>
       </c>
@@ -8707,7 +8711,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A28" s="18" t="s">
         <v>48</v>
       </c>
@@ -8732,7 +8736,7 @@
       </c>
       <c r="I28" s="20"/>
     </row>
-    <row r="29" spans="1:13" s="19" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:13" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.15">
       <c r="A29" s="18" t="s">
         <v>49</v>
       </c>
@@ -8757,7 +8761,7 @@
       </c>
       <c r="I29" s="20"/>
     </row>
-    <row r="30" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A30" s="18" t="s">
         <v>50</v>
       </c>
@@ -8782,7 +8786,7 @@
       </c>
       <c r="I30" s="20"/>
     </row>
-    <row r="31" spans="1:13" s="19" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:13" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.15">
       <c r="A31" s="18" t="s">
         <v>51</v>
       </c>
@@ -8807,7 +8811,7 @@
       </c>
       <c r="I31" s="20"/>
     </row>
-    <row r="32" spans="1:13" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:13" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
         <v>52</v>
       </c>
@@ -8832,7 +8836,7 @@
       </c>
       <c r="I32" s="20"/>
     </row>
-    <row r="33" spans="1:9" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A33" s="18" t="s">
         <v>53</v>
       </c>
@@ -8857,7 +8861,7 @@
       </c>
       <c r="I33" s="20"/>
     </row>
-    <row r="34" spans="1:9" s="19" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:9" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.15">
       <c r="A34" s="18" t="s">
         <v>54</v>
       </c>
@@ -8882,7 +8886,7 @@
       </c>
       <c r="I34" s="20"/>
     </row>
-    <row r="35" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>55</v>
       </c>
@@ -8907,7 +8911,7 @@
       </c>
       <c r="I35" s="27"/>
     </row>
-    <row r="36" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>56</v>
       </c>
@@ -8932,7 +8936,7 @@
       </c>
       <c r="I36" s="27"/>
     </row>
-    <row r="37" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>57</v>
       </c>
@@ -8957,7 +8961,7 @@
       </c>
       <c r="I37" s="27"/>
     </row>
-    <row r="38" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>58</v>
       </c>
@@ -8982,7 +8986,7 @@
       </c>
       <c r="I38" s="27"/>
     </row>
-    <row r="39" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>59</v>
       </c>
@@ -9007,7 +9011,7 @@
       </c>
       <c r="I39" s="27"/>
     </row>
-    <row r="40" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>60</v>
       </c>
@@ -9032,7 +9036,7 @@
       </c>
       <c r="I40" s="27"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="45" t="s">
         <v>636</v>
       </c>
@@ -9057,7 +9061,7 @@
       </c>
       <c r="I41" s="47"/>
     </row>
-    <row r="42" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="45" t="s">
         <v>637</v>
       </c>
@@ -9082,7 +9086,7 @@
       </c>
       <c r="I42" s="47"/>
     </row>
-    <row r="43" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>61</v>
       </c>
@@ -9132,7 +9136,7 @@
       </c>
       <c r="I44" s="47"/>
     </row>
-    <row r="45" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>615</v>
       </c>
@@ -9178,11 +9182,11 @@
         <v>15</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I46" s="47"/>
     </row>
-    <row r="47" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
         <v>617</v>
       </c>
@@ -9228,7 +9232,7 @@
         <v>15</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I48" s="47"/>
     </row>
@@ -9253,7 +9257,7 @@
         <v>15</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I49" s="47"/>
     </row>
@@ -9428,7 +9432,7 @@
         <v>15</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I56" s="47"/>
     </row>
@@ -9453,7 +9457,7 @@
         <v>15</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I57" s="47"/>
     </row>
@@ -9728,7 +9732,7 @@
         <v>15</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I68" s="47"/>
     </row>
@@ -9753,10 +9757,10 @@
         <v>15</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>1729</v>
+        <v>1724</v>
       </c>
       <c r="I69" s="47" t="s">
-        <v>1737</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -9784,7 +9788,7 @@
       </c>
       <c r="I70" s="27"/>
     </row>
-    <row r="71" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="45" t="s">
         <v>640</v>
       </c>
@@ -9909,7 +9913,7 @@
       </c>
       <c r="I75" s="27"/>
     </row>
-    <row r="76" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="25" t="s">
         <v>66</v>
       </c>
@@ -9934,7 +9938,7 @@
       </c>
       <c r="I76" s="27"/>
     </row>
-    <row r="77" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
         <v>67</v>
       </c>
@@ -9959,7 +9963,7 @@
       </c>
       <c r="I77" s="27"/>
     </row>
-    <row r="78" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="45" t="s">
         <v>645</v>
       </c>
@@ -9984,7 +9988,7 @@
       </c>
       <c r="I78" s="47"/>
     </row>
-    <row r="79" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="45" t="s">
         <v>646</v>
       </c>
@@ -10017,7 +10021,7 @@
         <v>647</v>
       </c>
       <c r="C80" s="16" t="s">
-        <v>1696</v>
+        <v>1739</v>
       </c>
       <c r="D80" s="25"/>
       <c r="E80" s="25" t="s">
@@ -11657,7 +11661,7 @@
         <v>15</v>
       </c>
       <c r="H145" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I145" s="27"/>
     </row>
@@ -11721,7 +11725,7 @@
         <v>647</v>
       </c>
       <c r="C148" s="16" t="s">
-        <v>1545</v>
+        <v>1542</v>
       </c>
       <c r="D148" s="25"/>
       <c r="E148" s="25" t="s">
@@ -11746,7 +11750,7 @@
         <v>647</v>
       </c>
       <c r="C149" s="16" t="s">
-        <v>1546</v>
+        <v>1543</v>
       </c>
       <c r="D149" s="25"/>
       <c r="E149" s="25" t="s">
@@ -11771,7 +11775,7 @@
         <v>647</v>
       </c>
       <c r="C150" s="16" t="s">
-        <v>1547</v>
+        <v>1544</v>
       </c>
       <c r="D150" s="25"/>
       <c r="E150" s="25" t="s">
@@ -11796,7 +11800,7 @@
         <v>647</v>
       </c>
       <c r="C151" s="16" t="s">
-        <v>1548</v>
+        <v>1545</v>
       </c>
       <c r="D151" s="25"/>
       <c r="E151" s="25" t="s">
@@ -11821,7 +11825,7 @@
         <v>647</v>
       </c>
       <c r="C152" s="16" t="s">
-        <v>1549</v>
+        <v>1546</v>
       </c>
       <c r="D152" s="25"/>
       <c r="E152" s="25" t="s">
@@ -11846,7 +11850,7 @@
         <v>647</v>
       </c>
       <c r="C153" s="16" t="s">
-        <v>1550</v>
+        <v>1547</v>
       </c>
       <c r="D153" s="25"/>
       <c r="E153" s="25" t="s">
@@ -11871,7 +11875,7 @@
         <v>647</v>
       </c>
       <c r="C154" s="16" t="s">
-        <v>1551</v>
+        <v>1548</v>
       </c>
       <c r="D154" s="25"/>
       <c r="E154" s="25" t="s">
@@ -11896,7 +11900,7 @@
         <v>647</v>
       </c>
       <c r="C155" s="16" t="s">
-        <v>1552</v>
+        <v>1549</v>
       </c>
       <c r="D155" s="25"/>
       <c r="E155" s="25" t="s">
@@ -11921,7 +11925,7 @@
         <v>647</v>
       </c>
       <c r="C156" s="16" t="s">
-        <v>1553</v>
+        <v>1550</v>
       </c>
       <c r="D156" s="25"/>
       <c r="E156" s="25" t="s">
@@ -11946,7 +11950,7 @@
         <v>647</v>
       </c>
       <c r="C157" s="16" t="s">
-        <v>1554</v>
+        <v>1551</v>
       </c>
       <c r="D157" s="25"/>
       <c r="E157" s="25" t="s">
@@ -11971,7 +11975,7 @@
         <v>647</v>
       </c>
       <c r="C158" s="16" t="s">
-        <v>1555</v>
+        <v>1552</v>
       </c>
       <c r="D158" s="25"/>
       <c r="E158" s="25" t="s">
@@ -11996,7 +12000,7 @@
         <v>647</v>
       </c>
       <c r="C159" s="16" t="s">
-        <v>1556</v>
+        <v>1553</v>
       </c>
       <c r="D159" s="25"/>
       <c r="E159" s="25" t="s">
@@ -12021,7 +12025,7 @@
         <v>647</v>
       </c>
       <c r="C160" s="16" t="s">
-        <v>1557</v>
+        <v>1554</v>
       </c>
       <c r="D160" s="25"/>
       <c r="E160" s="25" t="s">
@@ -12046,7 +12050,7 @@
         <v>647</v>
       </c>
       <c r="C161" s="16" t="s">
-        <v>1558</v>
+        <v>1555</v>
       </c>
       <c r="D161" s="25"/>
       <c r="E161" s="25" t="s">
@@ -12071,7 +12075,7 @@
         <v>647</v>
       </c>
       <c r="C162" s="16" t="s">
-        <v>1559</v>
+        <v>1556</v>
       </c>
       <c r="D162" s="25"/>
       <c r="E162" s="25" t="s">
@@ -12096,7 +12100,7 @@
         <v>647</v>
       </c>
       <c r="C163" s="16" t="s">
-        <v>1560</v>
+        <v>1557</v>
       </c>
       <c r="D163" s="25"/>
       <c r="E163" s="25" t="s">
@@ -12121,7 +12125,7 @@
         <v>647</v>
       </c>
       <c r="C164" s="16" t="s">
-        <v>1561</v>
+        <v>1558</v>
       </c>
       <c r="D164" s="25"/>
       <c r="E164" s="25" t="s">
@@ -12146,7 +12150,7 @@
         <v>647</v>
       </c>
       <c r="C165" s="16" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="D165" s="25"/>
       <c r="E165" s="25" t="s">
@@ -12171,7 +12175,7 @@
         <v>647</v>
       </c>
       <c r="C166" s="16" t="s">
-        <v>1563</v>
+        <v>1560</v>
       </c>
       <c r="D166" s="25"/>
       <c r="E166" s="25" t="s">
@@ -12196,7 +12200,7 @@
         <v>647</v>
       </c>
       <c r="C167" s="16" t="s">
-        <v>1564</v>
+        <v>1561</v>
       </c>
       <c r="D167" s="25"/>
       <c r="E167" s="25" t="s">
@@ -12221,7 +12225,7 @@
         <v>647</v>
       </c>
       <c r="C168" s="16" t="s">
-        <v>1565</v>
+        <v>1562</v>
       </c>
       <c r="D168" s="25"/>
       <c r="E168" s="25" t="s">
@@ -12246,7 +12250,7 @@
         <v>647</v>
       </c>
       <c r="C169" s="16" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="D169" s="25"/>
       <c r="E169" s="25" t="s">
@@ -12271,7 +12275,7 @@
         <v>647</v>
       </c>
       <c r="C170" s="16" t="s">
-        <v>1638</v>
+        <v>1635</v>
       </c>
       <c r="D170" s="45"/>
       <c r="E170" s="45" t="s">
@@ -12284,7 +12288,7 @@
         <v>15</v>
       </c>
       <c r="H170" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I170" s="47"/>
     </row>
@@ -12296,7 +12300,7 @@
         <v>647</v>
       </c>
       <c r="C171" s="16" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
       <c r="D171" s="45"/>
       <c r="E171" s="45" t="s">
@@ -12323,7 +12327,7 @@
         <v>647</v>
       </c>
       <c r="C172" s="16" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="D172" s="45"/>
       <c r="E172" s="45" t="s">
@@ -12425,7 +12429,7 @@
         <v>647</v>
       </c>
       <c r="C176" s="16" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
       <c r="D176" s="45"/>
       <c r="E176" s="45" t="s">
@@ -12527,7 +12531,7 @@
         <v>647</v>
       </c>
       <c r="C180" s="16" t="s">
-        <v>1645</v>
+        <v>1642</v>
       </c>
       <c r="D180" s="45"/>
       <c r="E180" s="45" t="s">
@@ -12552,7 +12556,7 @@
         <v>647</v>
       </c>
       <c r="C181" s="16" t="s">
-        <v>1647</v>
+        <v>1644</v>
       </c>
       <c r="D181" s="45"/>
       <c r="E181" s="45" t="s">
@@ -12579,7 +12583,7 @@
         <v>647</v>
       </c>
       <c r="C182" s="16" t="s">
-        <v>1716</v>
+        <v>1711</v>
       </c>
       <c r="D182" s="45"/>
       <c r="E182" s="45" t="s">
@@ -12604,7 +12608,7 @@
         <v>647</v>
       </c>
       <c r="C183" s="16" t="s">
-        <v>1715</v>
+        <v>1710</v>
       </c>
       <c r="D183" s="45"/>
       <c r="E183" s="45" t="s">
@@ -12681,7 +12685,7 @@
         <v>647</v>
       </c>
       <c r="C186" s="16" t="s">
-        <v>1649</v>
+        <v>1646</v>
       </c>
       <c r="D186" s="45"/>
       <c r="E186" s="45" t="s">
@@ -12706,7 +12710,7 @@
         <v>647</v>
       </c>
       <c r="C187" s="16" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
       <c r="D187" s="45"/>
       <c r="E187" s="45" t="s">
@@ -12758,7 +12762,7 @@
         <v>647</v>
       </c>
       <c r="C189" s="16" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="D189" s="45"/>
       <c r="E189" s="45" t="s">
@@ -12783,7 +12787,7 @@
         <v>647</v>
       </c>
       <c r="C190" s="16" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
       <c r="D190" s="45"/>
       <c r="E190" s="45" t="s">
@@ -12885,7 +12889,7 @@
         <v>647</v>
       </c>
       <c r="C194" s="16" t="s">
-        <v>1714</v>
+        <v>1709</v>
       </c>
       <c r="D194" s="45"/>
       <c r="E194" s="45" t="s">
@@ -13037,7 +13041,7 @@
         <v>647</v>
       </c>
       <c r="C200" s="16" t="s">
-        <v>1698</v>
+        <v>1693</v>
       </c>
       <c r="D200" s="45"/>
       <c r="E200" s="45" t="s">
@@ -13089,7 +13093,7 @@
         <v>647</v>
       </c>
       <c r="C202" s="16" t="s">
-        <v>1719</v>
+        <v>1714</v>
       </c>
       <c r="D202" s="45"/>
       <c r="E202" s="45" t="s">
@@ -13182,7 +13186,7 @@
         <v>17</v>
       </c>
       <c r="I205" s="16" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="206" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -13243,7 +13247,7 @@
         <v>647</v>
       </c>
       <c r="C208" s="16" t="s">
-        <v>1720</v>
+        <v>1715</v>
       </c>
       <c r="D208" s="45"/>
       <c r="E208" s="45" t="s">
@@ -13320,7 +13324,7 @@
         <v>647</v>
       </c>
       <c r="C211" s="16" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
       <c r="D211" s="45"/>
       <c r="E211" s="45" t="s">
@@ -13345,7 +13349,7 @@
         <v>647</v>
       </c>
       <c r="C212" s="16" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="D212" s="45"/>
       <c r="E212" s="45" t="s">
@@ -13358,7 +13362,7 @@
         <v>15</v>
       </c>
       <c r="H212" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I212" s="47"/>
     </row>
@@ -13386,7 +13390,7 @@
         <v>17</v>
       </c>
       <c r="I213" s="16" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -13897,7 +13901,7 @@
         <v>647</v>
       </c>
       <c r="C234" s="16" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
       <c r="D234" s="45"/>
       <c r="E234" s="45" t="s">
@@ -13947,7 +13951,7 @@
         <v>647</v>
       </c>
       <c r="C236" s="16" t="s">
-        <v>1724</v>
+        <v>1719</v>
       </c>
       <c r="D236" s="45"/>
       <c r="E236" s="45" t="s">
@@ -13960,7 +13964,7 @@
         <v>15</v>
       </c>
       <c r="H236" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I236" s="47"/>
     </row>
@@ -13985,10 +13989,10 @@
         <v>15</v>
       </c>
       <c r="H237" s="18" t="s">
-        <v>1729</v>
+        <v>1724</v>
       </c>
       <c r="I237" s="16" t="s">
-        <v>1732</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="238" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13999,7 +14003,7 @@
         <v>647</v>
       </c>
       <c r="C238" s="16" t="s">
-        <v>1726</v>
+        <v>1721</v>
       </c>
       <c r="D238" s="45"/>
       <c r="E238" s="45" t="s">
@@ -14012,7 +14016,7 @@
         <v>15</v>
       </c>
       <c r="H238" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I238" s="47"/>
     </row>
@@ -14037,10 +14041,10 @@
         <v>15</v>
       </c>
       <c r="H239" s="18" t="s">
-        <v>1729</v>
+        <v>1724</v>
       </c>
       <c r="I239" s="16" t="s">
-        <v>1730</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="240" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14051,7 +14055,7 @@
         <v>647</v>
       </c>
       <c r="C240" s="16" t="s">
-        <v>1725</v>
+        <v>1720</v>
       </c>
       <c r="D240" s="45"/>
       <c r="E240" s="45" t="s">
@@ -14064,7 +14068,7 @@
         <v>15</v>
       </c>
       <c r="H240" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I240" s="47"/>
     </row>
@@ -14089,10 +14093,10 @@
         <v>15</v>
       </c>
       <c r="H241" s="18" t="s">
-        <v>1729</v>
+        <v>1724</v>
       </c>
       <c r="I241" s="16" t="s">
-        <v>1733</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="242" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -14103,7 +14107,7 @@
         <v>647</v>
       </c>
       <c r="C242" s="16" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="D242" s="45"/>
       <c r="E242" s="45" t="s">
@@ -14116,7 +14120,7 @@
         <v>15</v>
       </c>
       <c r="H242" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I242" s="47"/>
     </row>
@@ -14128,7 +14132,7 @@
         <v>647</v>
       </c>
       <c r="C243" s="16" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="D243" s="45"/>
       <c r="E243" s="45" t="s">
@@ -14141,13 +14145,13 @@
         <v>15</v>
       </c>
       <c r="H243" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I243" s="16" t="s">
-        <v>1630</v>
-      </c>
-    </row>
-    <row r="244" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+        <v>1627</v>
+      </c>
+    </row>
+    <row r="244" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A244" s="25" t="s">
         <v>152</v>
       </c>
@@ -14172,7 +14176,7 @@
       </c>
       <c r="I244" s="27"/>
     </row>
-    <row r="245" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="25" t="s">
         <v>153</v>
       </c>
@@ -14197,7 +14201,7 @@
       </c>
       <c r="I245" s="27"/>
     </row>
-    <row r="246" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="25" t="s">
         <v>154</v>
       </c>
@@ -14222,7 +14226,7 @@
       </c>
       <c r="I246" s="27"/>
     </row>
-    <row r="247" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="25" t="s">
         <v>155</v>
       </c>
@@ -14247,7 +14251,7 @@
       </c>
       <c r="I247" s="27"/>
     </row>
-    <row r="248" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A248" s="25" t="s">
         <v>156</v>
       </c>
@@ -14272,7 +14276,7 @@
       </c>
       <c r="I248" s="27"/>
     </row>
-    <row r="249" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A249" s="25" t="s">
         <v>157</v>
       </c>
@@ -14322,7 +14326,7 @@
       </c>
       <c r="I250" s="27"/>
     </row>
-    <row r="251" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A251" s="25" t="s">
         <v>159</v>
       </c>
@@ -14447,7 +14451,7 @@
       </c>
       <c r="I255" s="27"/>
     </row>
-    <row r="256" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A256" s="25" t="s">
         <v>164</v>
       </c>
@@ -14472,7 +14476,7 @@
       </c>
       <c r="I256" s="27"/>
     </row>
-    <row r="257" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A257" s="25" t="s">
         <v>165</v>
       </c>
@@ -14497,7 +14501,7 @@
       </c>
       <c r="I257" s="27"/>
     </row>
-    <row r="258" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A258" s="25" t="s">
         <v>166</v>
       </c>
@@ -14522,7 +14526,7 @@
       </c>
       <c r="I258" s="27"/>
     </row>
-    <row r="259" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="25" t="s">
         <v>167</v>
       </c>
@@ -14547,7 +14551,7 @@
       </c>
       <c r="I259" s="27"/>
     </row>
-    <row r="260" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="25" t="s">
         <v>168</v>
       </c>
@@ -14572,7 +14576,7 @@
       </c>
       <c r="I260" s="27"/>
     </row>
-    <row r="261" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="25" t="s">
         <v>169</v>
       </c>
@@ -14597,7 +14601,7 @@
       </c>
       <c r="I261" s="27"/>
     </row>
-    <row r="262" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="25" t="s">
         <v>170</v>
       </c>
@@ -14622,7 +14626,7 @@
       </c>
       <c r="I262" s="27"/>
     </row>
-    <row r="263" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="25" t="s">
         <v>171</v>
       </c>
@@ -14647,7 +14651,7 @@
       </c>
       <c r="I263" s="27"/>
     </row>
-    <row r="264" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A264" s="25" t="s">
         <v>173</v>
       </c>
@@ -14672,7 +14676,7 @@
       </c>
       <c r="I264" s="27"/>
     </row>
-    <row r="265" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="25" t="s">
         <v>174</v>
       </c>
@@ -14697,7 +14701,7 @@
       </c>
       <c r="I265" s="27"/>
     </row>
-    <row r="266" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="25" t="s">
         <v>175</v>
       </c>
@@ -14722,7 +14726,7 @@
       </c>
       <c r="I266" s="27"/>
     </row>
-    <row r="267" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="25" t="s">
         <v>176</v>
       </c>
@@ -14747,7 +14751,7 @@
       </c>
       <c r="I267" s="27"/>
     </row>
-    <row r="268" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="25" t="s">
         <v>177</v>
       </c>
@@ -14772,7 +14776,7 @@
       </c>
       <c r="I268" s="27"/>
     </row>
-    <row r="269" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A269" s="25" t="s">
         <v>178</v>
       </c>
@@ -14797,7 +14801,7 @@
       </c>
       <c r="I269" s="27"/>
     </row>
-    <row r="270" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A270" s="18" t="s">
         <v>179</v>
       </c>
@@ -14822,7 +14826,7 @@
       </c>
       <c r="I270" s="27"/>
     </row>
-    <row r="271" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="48" t="s">
         <v>1505</v>
       </c>
@@ -14847,7 +14851,7 @@
       </c>
       <c r="I271" s="47"/>
     </row>
-    <row r="272" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="18" t="s">
         <v>1507</v>
       </c>
@@ -14872,7 +14876,7 @@
       </c>
       <c r="I272" s="47"/>
     </row>
-    <row r="273" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="25" t="s">
         <v>180</v>
       </c>
@@ -14922,7 +14926,7 @@
       </c>
       <c r="I274" s="27"/>
     </row>
-    <row r="275" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="25" t="s">
         <v>182</v>
       </c>
@@ -14997,7 +15001,7 @@
       </c>
       <c r="I277" s="27"/>
     </row>
-    <row r="278" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="25" t="s">
         <v>185</v>
       </c>
@@ -15022,7 +15026,7 @@
       </c>
       <c r="I278" s="27"/>
     </row>
-    <row r="279" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="25" t="s">
         <v>255</v>
       </c>
@@ -15097,7 +15101,7 @@
       </c>
       <c r="I281" s="47"/>
     </row>
-    <row r="282" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A282" s="18" t="s">
         <v>977</v>
       </c>
@@ -15372,7 +15376,7 @@
       </c>
       <c r="I292" s="47"/>
     </row>
-    <row r="293" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="45" t="s">
         <v>1019</v>
       </c>
@@ -15497,7 +15501,7 @@
       </c>
       <c r="I297" s="47"/>
     </row>
-    <row r="298" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A298" s="18" t="s">
         <v>1006</v>
       </c>
@@ -15722,7 +15726,7 @@
       </c>
       <c r="I306" s="47"/>
     </row>
-    <row r="307" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A307" s="18" t="s">
         <v>1015</v>
       </c>
@@ -15797,7 +15801,7 @@
       </c>
       <c r="I309" s="47"/>
     </row>
-    <row r="310" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A310" s="25" t="s">
         <v>256</v>
       </c>
@@ -15830,7 +15834,7 @@
         <v>405</v>
       </c>
       <c r="C311" s="16" t="s">
-        <v>1682</v>
+        <v>1678</v>
       </c>
       <c r="D311" s="25"/>
       <c r="E311" s="25" t="s">
@@ -15855,7 +15859,7 @@
         <v>405</v>
       </c>
       <c r="C312" s="16" t="s">
-        <v>1683</v>
+        <v>1679</v>
       </c>
       <c r="D312" s="25"/>
       <c r="E312" s="25" t="s">
@@ -16380,7 +16384,7 @@
         <v>405</v>
       </c>
       <c r="C333" s="16" t="s">
-        <v>1701</v>
+        <v>1696</v>
       </c>
       <c r="D333" s="25"/>
       <c r="E333" s="25" t="s">
@@ -16882,7 +16886,7 @@
         <v>1049</v>
       </c>
       <c r="C353" s="16" t="s">
-        <v>1658</v>
+        <v>1740</v>
       </c>
       <c r="D353" s="45"/>
       <c r="E353" s="45" t="s">
@@ -16899,7 +16903,7 @@
       </c>
       <c r="I353" s="47"/>
     </row>
-    <row r="354" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A354" s="45" t="s">
         <v>1053</v>
       </c>
@@ -16932,7 +16936,7 @@
         <v>1049</v>
       </c>
       <c r="C355" s="16" t="s">
-        <v>1702</v>
+        <v>1697</v>
       </c>
       <c r="D355" s="45"/>
       <c r="E355" s="45" t="s">
@@ -16945,7 +16949,7 @@
         <v>15</v>
       </c>
       <c r="H355" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I355" s="47"/>
     </row>
@@ -16957,7 +16961,7 @@
         <v>1049</v>
       </c>
       <c r="C356" s="16" t="s">
-        <v>1703</v>
+        <v>1698</v>
       </c>
       <c r="D356" s="45"/>
       <c r="E356" s="45" t="s">
@@ -16970,7 +16974,7 @@
         <v>15</v>
       </c>
       <c r="H356" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I356" s="47"/>
     </row>
@@ -16982,7 +16986,7 @@
         <v>1049</v>
       </c>
       <c r="C357" s="16" t="s">
-        <v>1704</v>
+        <v>1699</v>
       </c>
       <c r="D357" s="45"/>
       <c r="E357" s="45" t="s">
@@ -16995,7 +16999,7 @@
         <v>15</v>
       </c>
       <c r="H357" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I357" s="47"/>
     </row>
@@ -17007,7 +17011,7 @@
         <v>1049</v>
       </c>
       <c r="C358" s="16" t="s">
-        <v>1705</v>
+        <v>1700</v>
       </c>
       <c r="D358" s="45"/>
       <c r="E358" s="45" t="s">
@@ -17020,7 +17024,7 @@
         <v>15</v>
       </c>
       <c r="H358" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I358" s="47"/>
     </row>
@@ -17032,7 +17036,7 @@
         <v>1049</v>
       </c>
       <c r="C359" s="16" t="s">
-        <v>1706</v>
+        <v>1701</v>
       </c>
       <c r="D359" s="45"/>
       <c r="E359" s="45" t="s">
@@ -17045,7 +17049,7 @@
         <v>15</v>
       </c>
       <c r="H359" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I359" s="47"/>
     </row>
@@ -17057,7 +17061,7 @@
         <v>1049</v>
       </c>
       <c r="C360" s="16" t="s">
-        <v>1707</v>
+        <v>1702</v>
       </c>
       <c r="D360" s="45"/>
       <c r="E360" s="45" t="s">
@@ -17070,7 +17074,7 @@
         <v>15</v>
       </c>
       <c r="H360" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I360" s="47"/>
     </row>
@@ -17109,7 +17113,7 @@
         <v>1060</v>
       </c>
       <c r="C362" s="16" t="s">
-        <v>1700</v>
+        <v>1695</v>
       </c>
       <c r="D362" s="45"/>
       <c r="E362" s="45" t="s">
@@ -17126,7 +17130,7 @@
       </c>
       <c r="I362" s="47"/>
     </row>
-    <row r="363" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A363" s="45" t="s">
         <v>1065</v>
       </c>
@@ -17159,7 +17163,7 @@
         <v>1060</v>
       </c>
       <c r="C364" s="16" t="s">
-        <v>1708</v>
+        <v>1703</v>
       </c>
       <c r="D364" s="45"/>
       <c r="E364" s="45" t="s">
@@ -17172,7 +17176,7 @@
         <v>15</v>
       </c>
       <c r="H364" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I364" s="47"/>
     </row>
@@ -17184,7 +17188,7 @@
         <v>1060</v>
       </c>
       <c r="C365" s="16" t="s">
-        <v>1709</v>
+        <v>1704</v>
       </c>
       <c r="D365" s="45"/>
       <c r="E365" s="45" t="s">
@@ -17197,7 +17201,7 @@
         <v>15</v>
       </c>
       <c r="H365" s="18" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="I365" s="47"/>
     </row>
@@ -18413,7 +18417,7 @@
       </c>
       <c r="I413" s="27"/>
     </row>
-    <row r="414" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A414" s="18" t="s">
         <v>186</v>
       </c>
@@ -18473,7 +18477,7 @@
         <v>408</v>
       </c>
       <c r="C416" s="16" t="s">
-        <v>1712</v>
+        <v>1707</v>
       </c>
       <c r="D416" s="45"/>
       <c r="E416" s="45" t="s">
@@ -18490,7 +18494,7 @@
       </c>
       <c r="I416" s="47"/>
     </row>
-    <row r="417" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A417" s="45" t="s">
         <v>896</v>
       </c>
@@ -18623,7 +18627,7 @@
         <v>409</v>
       </c>
       <c r="C422" s="16" t="s">
-        <v>1695</v>
+        <v>1691</v>
       </c>
       <c r="D422" s="45"/>
       <c r="E422" s="45" t="s">
@@ -18650,7 +18654,7 @@
         <v>409</v>
       </c>
       <c r="C423" s="16" t="s">
-        <v>1659</v>
+        <v>1655</v>
       </c>
       <c r="D423" s="45"/>
       <c r="E423" s="45" t="s">
@@ -18667,7 +18671,7 @@
       </c>
       <c r="I423" s="47"/>
     </row>
-    <row r="424" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A424" s="45" t="s">
         <v>914</v>
       </c>
@@ -18942,7 +18946,7 @@
       </c>
       <c r="I434" s="47"/>
     </row>
-    <row r="435" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A435" s="25" t="s">
         <v>187</v>
       </c>
@@ -18992,7 +18996,7 @@
       </c>
       <c r="I436" s="27"/>
     </row>
-    <row r="437" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A437" s="25" t="s">
         <v>189</v>
       </c>
@@ -19092,7 +19096,7 @@
       </c>
       <c r="I440" s="27"/>
     </row>
-    <row r="441" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A441" s="25" t="s">
         <v>193</v>
       </c>
@@ -19142,7 +19146,7 @@
       </c>
       <c r="I442" s="27"/>
     </row>
-    <row r="443" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A443" s="25" t="s">
         <v>195</v>
       </c>
@@ -19608,7 +19612,7 @@
         <v>411</v>
       </c>
       <c r="C461" s="16" t="s">
-        <v>1690</v>
+        <v>1686</v>
       </c>
       <c r="D461" s="25"/>
       <c r="E461" s="25" t="s">
@@ -19627,7 +19631,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="462" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A462" s="25" t="s">
         <v>214</v>
       </c>
@@ -19660,7 +19664,7 @@
         <v>412</v>
       </c>
       <c r="C463" s="16" t="s">
-        <v>1691</v>
+        <v>1687</v>
       </c>
       <c r="D463" s="25"/>
       <c r="E463" s="25" t="s">
@@ -19677,7 +19681,7 @@
       </c>
       <c r="I463" s="27"/>
     </row>
-    <row r="464" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A464" s="25" t="s">
         <v>216</v>
       </c>
@@ -19777,7 +19781,7 @@
       </c>
       <c r="I467" s="27"/>
     </row>
-    <row r="468" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A468" s="25" t="s">
         <v>220</v>
       </c>
@@ -19827,7 +19831,7 @@
       </c>
       <c r="I469" s="27"/>
     </row>
-    <row r="470" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A470" s="25" t="s">
         <v>222</v>
       </c>
@@ -20481,7 +20485,7 @@
       </c>
       <c r="I495" s="27"/>
     </row>
-    <row r="496" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A496" s="25" t="s">
         <v>244</v>
       </c>
@@ -20656,7 +20660,7 @@
       </c>
       <c r="I502" s="27"/>
     </row>
-    <row r="503" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A503" s="25" t="s">
         <v>251</v>
       </c>
@@ -20756,7 +20760,7 @@
       </c>
       <c r="I506" s="27"/>
     </row>
-    <row r="507" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A507" s="25" t="s">
         <v>341</v>
       </c>
@@ -20806,7 +20810,7 @@
       </c>
       <c r="I508" s="27"/>
     </row>
-    <row r="509" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A509" s="25" t="s">
         <v>343</v>
       </c>
@@ -20881,7 +20885,7 @@
       </c>
       <c r="I511" s="27"/>
     </row>
-    <row r="512" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A512" s="25" t="s">
         <v>346</v>
       </c>
@@ -20906,7 +20910,7 @@
       </c>
       <c r="I512" s="27"/>
     </row>
-    <row r="513" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A513" s="25" t="s">
         <v>347</v>
       </c>
@@ -20956,7 +20960,7 @@
       </c>
       <c r="I514" s="27"/>
     </row>
-    <row r="515" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A515" s="25" t="s">
         <v>349</v>
       </c>
@@ -21031,7 +21035,7 @@
       </c>
       <c r="I517" s="27"/>
     </row>
-    <row r="518" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A518" s="25" t="s">
         <v>352</v>
       </c>
@@ -21056,7 +21060,7 @@
       </c>
       <c r="I518" s="27"/>
     </row>
-    <row r="519" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A519" s="25" t="s">
         <v>353</v>
       </c>
@@ -21106,7 +21110,7 @@
       </c>
       <c r="I520" s="27"/>
     </row>
-    <row r="521" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A521" s="25" t="s">
         <v>355</v>
       </c>
@@ -21181,7 +21185,7 @@
       </c>
       <c r="I523" s="27"/>
     </row>
-    <row r="524" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A524" s="25" t="s">
         <v>358</v>
       </c>
@@ -21206,7 +21210,7 @@
       </c>
       <c r="I524" s="27"/>
     </row>
-    <row r="525" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A525" s="25" t="s">
         <v>359</v>
       </c>
@@ -21256,7 +21260,7 @@
       </c>
       <c r="I526" s="27"/>
     </row>
-    <row r="527" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A527" s="25" t="s">
         <v>361</v>
       </c>
@@ -21331,7 +21335,7 @@
       </c>
       <c r="I529" s="27"/>
     </row>
-    <row r="530" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A530" s="25" t="s">
         <v>364</v>
       </c>
@@ -21356,7 +21360,7 @@
       </c>
       <c r="I530" s="27"/>
     </row>
-    <row r="531" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A531" s="25" t="s">
         <v>365</v>
       </c>
@@ -21406,7 +21410,7 @@
       </c>
       <c r="I532" s="27"/>
     </row>
-    <row r="533" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A533" s="25" t="s">
         <v>367</v>
       </c>
@@ -21506,7 +21510,7 @@
       </c>
       <c r="I536" s="47"/>
     </row>
-    <row r="537" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A537" s="18" t="s">
         <v>370</v>
       </c>
@@ -21531,7 +21535,7 @@
       </c>
       <c r="I537" s="27"/>
     </row>
-    <row r="538" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A538" s="45" t="s">
         <v>1244</v>
       </c>
@@ -21556,7 +21560,7 @@
       </c>
       <c r="I538" s="47"/>
     </row>
-    <row r="539" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:9" s="50" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A539" s="45" t="s">
         <v>1245</v>
       </c>
@@ -21576,12 +21580,12 @@
       <c r="G539" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H539" s="45" t="s">
-        <v>18</v>
+      <c r="H539" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I539" s="47"/>
     </row>
-    <row r="540" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:9" s="50" customFormat="1" ht="300" x14ac:dyDescent="0.25">
       <c r="A540" s="45" t="s">
         <v>1246</v>
       </c>
@@ -21601,8 +21605,8 @@
       <c r="G540" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H540" s="45" t="s">
-        <v>18</v>
+      <c r="H540" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I540" s="47"/>
     </row>
@@ -21648,15 +21652,15 @@
       <c r="F542" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G542" s="45" t="s">
-        <v>15</v>
+      <c r="G542" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H542" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I542" s="47"/>
     </row>
-    <row r="543" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A543" s="45" t="s">
         <v>1248</v>
       </c>
@@ -21706,7 +21710,7 @@
       </c>
       <c r="I544" s="47"/>
     </row>
-    <row r="545" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A545" s="45" t="s">
         <v>1250</v>
       </c>
@@ -21948,15 +21952,15 @@
       <c r="F554" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G554" s="45" t="s">
-        <v>15</v>
+      <c r="G554" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H554" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I554" s="47"/>
     </row>
-    <row r="555" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:9" s="50" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A555" s="45" t="s">
         <v>1260</v>
       </c>
@@ -21976,12 +21980,12 @@
       <c r="G555" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H555" s="45" t="s">
-        <v>18</v>
+      <c r="H555" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I555" s="47"/>
     </row>
-    <row r="556" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A556" s="45" t="s">
         <v>1261</v>
       </c>
@@ -21998,15 +22002,15 @@
       <c r="F556" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G556" s="45" t="s">
-        <v>15</v>
+      <c r="G556" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H556" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I556" s="47"/>
     </row>
-    <row r="557" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A557" s="45" t="s">
         <v>1262</v>
       </c>
@@ -22031,7 +22035,7 @@
       </c>
       <c r="I557" s="47"/>
     </row>
-    <row r="558" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A558" s="45" t="s">
         <v>1263</v>
       </c>
@@ -22051,12 +22055,12 @@
       <c r="G558" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H558" s="45" t="s">
-        <v>18</v>
+      <c r="H558" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I558" s="47"/>
     </row>
-    <row r="559" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A559" s="45" t="s">
         <v>1264</v>
       </c>
@@ -22076,12 +22080,12 @@
       <c r="G559" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H559" s="45" t="s">
-        <v>18</v>
+      <c r="H559" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I559" s="47"/>
     </row>
-    <row r="560" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A560" s="45" t="s">
         <v>1265</v>
       </c>
@@ -22101,12 +22105,12 @@
       <c r="G560" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H560" s="45" t="s">
-        <v>18</v>
+      <c r="H560" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I560" s="47"/>
     </row>
-    <row r="561" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A561" s="45" t="s">
         <v>1266</v>
       </c>
@@ -22126,8 +22130,8 @@
       <c r="G561" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H561" s="45" t="s">
-        <v>18</v>
+      <c r="H561" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I561" s="47"/>
     </row>
@@ -22181,7 +22185,7 @@
       </c>
       <c r="I563" s="47"/>
     </row>
-    <row r="564" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A564" s="45" t="s">
         <v>1269</v>
       </c>
@@ -22206,7 +22210,7 @@
       </c>
       <c r="I564" s="47"/>
     </row>
-    <row r="565" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A565" s="45" t="s">
         <v>1270</v>
       </c>
@@ -22231,7 +22235,7 @@
       </c>
       <c r="I565" s="47"/>
     </row>
-    <row r="566" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A566" s="45" t="s">
         <v>1271</v>
       </c>
@@ -22281,7 +22285,7 @@
       </c>
       <c r="I567" s="47"/>
     </row>
-    <row r="568" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A568" s="45" t="s">
         <v>1273</v>
       </c>
@@ -22356,7 +22360,7 @@
       </c>
       <c r="I570" s="47"/>
     </row>
-    <row r="571" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A571" s="45" t="s">
         <v>1276</v>
       </c>
@@ -22373,15 +22377,15 @@
       <c r="F571" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G571" s="45" t="s">
-        <v>15</v>
+      <c r="G571" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H571" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I571" s="47"/>
     </row>
-    <row r="572" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:9" s="50" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A572" s="45" t="s">
         <v>1277</v>
       </c>
@@ -22401,12 +22405,12 @@
       <c r="G572" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H572" s="45" t="s">
-        <v>18</v>
+      <c r="H572" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I572" s="47"/>
     </row>
-    <row r="573" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A573" s="45" t="s">
         <v>1278</v>
       </c>
@@ -22456,7 +22460,7 @@
       </c>
       <c r="I574" s="47"/>
     </row>
-    <row r="575" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A575" s="45" t="s">
         <v>1280</v>
       </c>
@@ -22481,7 +22485,7 @@
       </c>
       <c r="I575" s="47"/>
     </row>
-    <row r="576" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A576" s="45" t="s">
         <v>1281</v>
       </c>
@@ -22506,7 +22510,7 @@
       </c>
       <c r="I576" s="47"/>
     </row>
-    <row r="577" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A577" s="45" t="s">
         <v>1282</v>
       </c>
@@ -22531,7 +22535,7 @@
       </c>
       <c r="I577" s="47"/>
     </row>
-    <row r="578" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A578" s="45" t="s">
         <v>1283</v>
       </c>
@@ -22606,7 +22610,7 @@
       </c>
       <c r="I580" s="47"/>
     </row>
-    <row r="581" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A581" s="45" t="s">
         <v>1286</v>
       </c>
@@ -22731,7 +22735,7 @@
       </c>
       <c r="I585" s="47"/>
     </row>
-    <row r="586" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A586" s="45" t="s">
         <v>1291</v>
       </c>
@@ -22756,7 +22760,7 @@
       </c>
       <c r="I586" s="47"/>
     </row>
-    <row r="587" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A587" s="45" t="s">
         <v>1292</v>
       </c>
@@ -22781,7 +22785,7 @@
       </c>
       <c r="I587" s="47"/>
     </row>
-    <row r="588" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A588" s="45" t="s">
         <v>1293</v>
       </c>
@@ -22806,7 +22810,7 @@
       </c>
       <c r="I588" s="47"/>
     </row>
-    <row r="589" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A589" s="45" t="s">
         <v>1294</v>
       </c>
@@ -22823,15 +22827,15 @@
       <c r="F589" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G589" s="45" t="s">
-        <v>15</v>
+      <c r="G589" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H589" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I589" s="47"/>
     </row>
-    <row r="590" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A590" s="45" t="s">
         <v>1295</v>
       </c>
@@ -22839,7 +22843,7 @@
         <v>1165</v>
       </c>
       <c r="C590" s="16" t="s">
-        <v>1532</v>
+        <v>1734</v>
       </c>
       <c r="D590" s="45"/>
       <c r="E590" s="45" t="s">
@@ -22851,12 +22855,12 @@
       <c r="G590" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H590" s="45" t="s">
-        <v>18</v>
+      <c r="H590" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I590" s="47"/>
     </row>
-    <row r="591" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="591" spans="1:9" s="50" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A591" s="45" t="s">
         <v>1296</v>
       </c>
@@ -22864,7 +22868,7 @@
         <v>1165</v>
       </c>
       <c r="C591" s="16" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="D591" s="45"/>
       <c r="E591" s="45" t="s">
@@ -22876,12 +22880,12 @@
       <c r="G591" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H591" s="45" t="s">
-        <v>18</v>
+      <c r="H591" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I591" s="47"/>
     </row>
-    <row r="592" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A592" s="45" t="s">
         <v>1297</v>
       </c>
@@ -22906,7 +22910,7 @@
       </c>
       <c r="I592" s="47"/>
     </row>
-    <row r="593" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A593" s="45" t="s">
         <v>1298</v>
       </c>
@@ -22926,12 +22930,12 @@
       <c r="G593" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H593" s="45" t="s">
-        <v>18</v>
+      <c r="H593" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I593" s="47"/>
     </row>
-    <row r="594" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A594" s="45" t="s">
         <v>1299</v>
       </c>
@@ -22956,7 +22960,7 @@
       </c>
       <c r="I594" s="47"/>
     </row>
-    <row r="595" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A595" s="45" t="s">
         <v>1435</v>
       </c>
@@ -22983,7 +22987,7 @@
       </c>
       <c r="I595" s="47"/>
     </row>
-    <row r="596" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A596" s="45" t="s">
         <v>1436</v>
       </c>
@@ -23010,7 +23014,7 @@
       </c>
       <c r="I596" s="47"/>
     </row>
-    <row r="597" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A597" s="45" t="s">
         <v>1300</v>
       </c>
@@ -23030,12 +23034,12 @@
       <c r="G597" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H597" s="45" t="s">
-        <v>18</v>
+      <c r="H597" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I597" s="47"/>
     </row>
-    <row r="598" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A598" s="18" t="s">
         <v>1301</v>
       </c>
@@ -23055,20 +23059,20 @@
       <c r="G598" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H598" s="45" t="s">
-        <v>18</v>
+      <c r="H598" s="18" t="s">
+        <v>1624</v>
       </c>
       <c r="I598" s="47"/>
     </row>
-    <row r="599" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A599" s="18" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B599" s="20" t="s">
         <v>1165</v>
       </c>
       <c r="C599" s="16" t="s">
-        <v>1536</v>
+        <v>1738</v>
       </c>
       <c r="D599" s="45"/>
       <c r="E599" s="45" t="s">
@@ -23080,20 +23084,20 @@
       <c r="G599" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H599" s="45" t="s">
-        <v>20</v>
+      <c r="H599" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I599" s="47"/>
     </row>
-    <row r="600" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A600" s="18" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B600" s="20" t="s">
         <v>1165</v>
       </c>
       <c r="C600" s="16" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="D600" s="18"/>
       <c r="E600" s="45" t="s">
@@ -23109,7 +23113,7 @@
         <v>17</v>
       </c>
       <c r="I600" s="16" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="601" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -23187,7 +23191,7 @@
       </c>
       <c r="I603" s="47"/>
     </row>
-    <row r="604" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A604" s="45" t="s">
         <v>1305</v>
       </c>
@@ -23212,7 +23216,7 @@
       </c>
       <c r="I604" s="47"/>
     </row>
-    <row r="605" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="605" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A605" s="45" t="s">
         <v>1306</v>
       </c>
@@ -23237,7 +23241,7 @@
       </c>
       <c r="I605" s="47"/>
     </row>
-    <row r="606" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A606" s="45" t="s">
         <v>1307</v>
       </c>
@@ -23262,7 +23266,7 @@
       </c>
       <c r="I606" s="47"/>
     </row>
-    <row r="607" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A607" s="45" t="s">
         <v>1308</v>
       </c>
@@ -23312,7 +23316,7 @@
       </c>
       <c r="I608" s="47"/>
     </row>
-    <row r="609" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A609" s="45" t="s">
         <v>1310</v>
       </c>
@@ -23570,7 +23574,7 @@
         <v>1196</v>
       </c>
       <c r="C619" s="16" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="D619" s="45"/>
       <c r="E619" s="45" t="s">
@@ -23597,7 +23601,7 @@
         <v>1196</v>
       </c>
       <c r="C620" s="16" t="s">
-        <v>1711</v>
+        <v>1706</v>
       </c>
       <c r="D620" s="45"/>
       <c r="E620" s="45" t="s">
@@ -23609,12 +23613,12 @@
       <c r="G620" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H620" s="45" t="s">
-        <v>18</v>
+      <c r="H620" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I620" s="47"/>
     </row>
-    <row r="621" spans="1:9" ht="255" x14ac:dyDescent="0.25">
+    <row r="621" spans="1:9" s="50" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A621" s="45" t="s">
         <v>1322</v>
       </c>
@@ -23634,8 +23638,8 @@
       <c r="G621" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H621" s="45" t="s">
-        <v>18</v>
+      <c r="H621" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I621" s="47"/>
     </row>
@@ -23664,7 +23668,7 @@
       </c>
       <c r="I622" s="47"/>
     </row>
-    <row r="623" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A623" s="45" t="s">
         <v>1324</v>
       </c>
@@ -23684,12 +23688,12 @@
       <c r="G623" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H623" s="45" t="s">
-        <v>18</v>
+      <c r="H623" s="18" t="s">
+        <v>1624</v>
       </c>
       <c r="I623" s="47"/>
     </row>
-    <row r="624" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A624" s="45" t="s">
         <v>1325</v>
       </c>
@@ -23714,7 +23718,7 @@
       </c>
       <c r="I624" s="47"/>
     </row>
-    <row r="625" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="625" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A625" s="45" t="s">
         <v>1326</v>
       </c>
@@ -23739,7 +23743,7 @@
       </c>
       <c r="I625" s="47"/>
     </row>
-    <row r="626" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A626" s="45" t="s">
         <v>1327</v>
       </c>
@@ -23981,15 +23985,15 @@
       <c r="F635" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G635" s="45" t="s">
-        <v>15</v>
+      <c r="G635" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H635" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I635" s="47"/>
     </row>
-    <row r="636" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:9" s="50" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A636" s="45" t="s">
         <v>1337</v>
       </c>
@@ -24009,12 +24013,12 @@
       <c r="G636" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H636" s="45" t="s">
-        <v>18</v>
+      <c r="H636" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I636" s="47"/>
     </row>
-    <row r="637" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A637" s="45" t="s">
         <v>1338</v>
       </c>
@@ -24031,15 +24035,15 @@
       <c r="F637" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G637" s="45" t="s">
-        <v>15</v>
+      <c r="G637" s="18" t="s">
+        <v>1737</v>
       </c>
       <c r="H637" s="45" t="s">
         <v>18</v>
       </c>
       <c r="I637" s="47"/>
     </row>
-    <row r="638" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="638" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A638" s="45" t="s">
         <v>1339</v>
       </c>
@@ -24064,7 +24068,7 @@
       </c>
       <c r="I638" s="47"/>
     </row>
-    <row r="639" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A639" s="45" t="s">
         <v>1340</v>
       </c>
@@ -24084,12 +24088,12 @@
       <c r="G639" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H639" s="45" t="s">
-        <v>18</v>
+      <c r="H639" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I639" s="47"/>
     </row>
-    <row r="640" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="640" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A640" s="45" t="s">
         <v>1341</v>
       </c>
@@ -24109,12 +24113,12 @@
       <c r="G640" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H640" s="45" t="s">
-        <v>18</v>
+      <c r="H640" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I640" s="47"/>
     </row>
-    <row r="641" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A641" s="45" t="s">
         <v>1342</v>
       </c>
@@ -24134,12 +24138,12 @@
       <c r="G641" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H641" s="45" t="s">
-        <v>18</v>
+      <c r="H641" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I641" s="47"/>
     </row>
-    <row r="642" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:9" s="50" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A642" s="45" t="s">
         <v>1343</v>
       </c>
@@ -24159,12 +24163,12 @@
       <c r="G642" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H642" s="45" t="s">
-        <v>18</v>
+      <c r="H642" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I642" s="47"/>
     </row>
-    <row r="643" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="643" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A643" s="45" t="s">
         <v>1344</v>
       </c>
@@ -24189,7 +24193,7 @@
       </c>
       <c r="I643" s="47"/>
     </row>
-    <row r="644" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A644" s="45" t="s">
         <v>1345</v>
       </c>
@@ -24214,7 +24218,7 @@
       </c>
       <c r="I644" s="47"/>
     </row>
-    <row r="645" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A645" s="45" t="s">
         <v>1346</v>
       </c>
@@ -24289,7 +24293,7 @@
       </c>
       <c r="I647" s="47"/>
     </row>
-    <row r="648" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="648" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A648" s="45" t="s">
         <v>1349</v>
       </c>
@@ -24314,7 +24318,7 @@
       </c>
       <c r="I648" s="47"/>
     </row>
-    <row r="649" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A649" s="45" t="s">
         <v>1350</v>
       </c>
@@ -24334,12 +24338,12 @@
       <c r="G649" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H649" s="45" t="s">
-        <v>18</v>
+      <c r="H649" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I649" s="47"/>
     </row>
-    <row r="650" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="650" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A650" s="45" t="s">
         <v>1351</v>
       </c>
@@ -24389,7 +24393,7 @@
       </c>
       <c r="I651" s="47"/>
     </row>
-    <row r="652" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A652" s="45" t="s">
         <v>1353</v>
       </c>
@@ -24414,7 +24418,7 @@
       </c>
       <c r="I652" s="47"/>
     </row>
-    <row r="653" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A653" s="45" t="s">
         <v>1354</v>
       </c>
@@ -24422,7 +24426,7 @@
         <v>1230</v>
       </c>
       <c r="C653" s="16" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="D653" s="45"/>
       <c r="E653" s="45" t="s">
@@ -24639,7 +24643,7 @@
       </c>
       <c r="I661" s="47"/>
     </row>
-    <row r="662" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="662" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A662" s="45" t="s">
         <v>1363</v>
       </c>
@@ -24664,7 +24668,7 @@
       </c>
       <c r="I662" s="47"/>
     </row>
-    <row r="663" spans="1:9" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A663" s="45" t="s">
         <v>1364</v>
       </c>
@@ -24672,7 +24676,7 @@
         <v>1242</v>
       </c>
       <c r="C663" s="16" t="s">
-        <v>1540</v>
+        <v>1735</v>
       </c>
       <c r="D663" s="45"/>
       <c r="E663" s="45" t="s">
@@ -24681,15 +24685,15 @@
       <c r="F663" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G663" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="H663" s="45" t="s">
-        <v>18</v>
+      <c r="G663" s="18" t="s">
+        <v>1736</v>
+      </c>
+      <c r="H663" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I663" s="47"/>
     </row>
-    <row r="664" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:9" s="50" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A664" s="45" t="s">
         <v>1365</v>
       </c>
@@ -24697,7 +24701,7 @@
         <v>1242</v>
       </c>
       <c r="C664" s="16" t="s">
-        <v>1541</v>
+        <v>1538</v>
       </c>
       <c r="D664" s="45"/>
       <c r="E664" s="45" t="s">
@@ -24709,12 +24713,12 @@
       <c r="G664" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="H664" s="45" t="s">
-        <v>18</v>
+      <c r="H664" s="18" t="s">
+        <v>1628</v>
       </c>
       <c r="I664" s="47"/>
     </row>
-    <row r="665" spans="1:9" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="665" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A665" s="18" t="s">
         <v>371</v>
       </c>
@@ -24722,7 +24726,7 @@
         <v>610</v>
       </c>
       <c r="C665" s="16" t="s">
-        <v>1542</v>
+        <v>1539</v>
       </c>
       <c r="D665" s="25"/>
       <c r="E665" s="25" t="s">
@@ -24739,7 +24743,7 @@
       </c>
       <c r="I665" s="27"/>
     </row>
-    <row r="666" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A666" s="18" t="s">
         <v>1438</v>
       </c>
@@ -24747,7 +24751,7 @@
         <v>610</v>
       </c>
       <c r="C666" s="16" t="s">
-        <v>1543</v>
+        <v>1540</v>
       </c>
       <c r="D666" s="45" t="s">
         <v>1440</v>
@@ -24768,7 +24772,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="667" spans="1:9" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A667" s="25" t="s">
         <v>372</v>
       </c>
@@ -24776,7 +24780,7 @@
         <v>610</v>
       </c>
       <c r="C667" s="16" t="s">
-        <v>1544</v>
+        <v>1541</v>
       </c>
       <c r="D667" s="25"/>
       <c r="E667" s="25" t="s">
@@ -24793,7 +24797,7 @@
       </c>
       <c r="I667" s="27"/>
     </row>
-    <row r="668" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A668" s="18" t="s">
         <v>611</v>
       </c>
@@ -24820,7 +24824,7 @@
       </c>
       <c r="I668" s="47"/>
     </row>
-    <row r="669" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A669" s="18" t="s">
         <v>613</v>
       </c>
@@ -24843,24 +24847,24 @@
         <v>15</v>
       </c>
       <c r="H669" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I669" s="47" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="670" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A670" s="18" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="B670" s="49">
         <v>8</v>
       </c>
       <c r="C670" s="16" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
       <c r="D670" s="18" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="E670" s="45" t="s">
         <v>22</v>
@@ -24878,16 +24882,16 @@
     </row>
     <row r="671" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A671" s="18" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="B671" s="49">
         <v>8</v>
       </c>
       <c r="C671" s="16" t="s">
-        <v>1570</v>
+        <v>1567</v>
       </c>
       <c r="D671" s="18" t="s">
-        <v>1571</v>
+        <v>1568</v>
       </c>
       <c r="E671" s="45" t="s">
         <v>22</v>
@@ -24905,7 +24909,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="672" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A672" s="18" t="s">
         <v>373</v>
       </c>
@@ -24913,7 +24917,7 @@
         <v>610</v>
       </c>
       <c r="C672" s="16" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="D672" s="18" t="s">
         <v>587</v>
@@ -24932,7 +24936,7 @@
       </c>
       <c r="I672" s="27"/>
     </row>
-    <row r="673" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="673" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A673" s="18" t="s">
         <v>374</v>
       </c>
@@ -24940,7 +24944,7 @@
         <v>610</v>
       </c>
       <c r="C673" s="16" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
       <c r="D673" s="25" t="s">
         <v>587</v>
@@ -24959,7 +24963,7 @@
       </c>
       <c r="I673" s="27"/>
     </row>
-    <row r="674" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:9" s="50" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A674" s="25" t="s">
         <v>375</v>
       </c>
@@ -24967,7 +24971,7 @@
         <v>610</v>
       </c>
       <c r="C674" s="16" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="D674" s="18" t="s">
         <v>588</v>
@@ -24986,7 +24990,7 @@
       </c>
       <c r="I674" s="27"/>
     </row>
-    <row r="675" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:9" s="50" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A675" s="18" t="s">
         <v>376</v>
       </c>
@@ -24994,7 +24998,7 @@
         <v>610</v>
       </c>
       <c r="C675" s="16" t="s">
-        <v>1722</v>
+        <v>1717</v>
       </c>
       <c r="D675" s="18" t="s">
         <v>588</v>
@@ -25013,7 +25017,7 @@
       </c>
       <c r="I675" s="27"/>
     </row>
-    <row r="676" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A676" s="45" t="s">
         <v>698</v>
       </c>
@@ -25021,7 +25025,7 @@
         <v>610</v>
       </c>
       <c r="C676" s="16" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="D676" s="45" t="s">
         <v>1443</v>
@@ -25048,7 +25052,7 @@
         <v>610</v>
       </c>
       <c r="C677" s="16" t="s">
-        <v>1710</v>
+        <v>1705</v>
       </c>
       <c r="D677" s="45" t="s">
         <v>1443</v>
@@ -25063,13 +25067,13 @@
         <v>15</v>
       </c>
       <c r="H677" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I677" s="47" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="678" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A678" s="45" t="s">
         <v>743</v>
       </c>
@@ -25077,7 +25081,7 @@
         <v>610</v>
       </c>
       <c r="C678" s="16" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="D678" s="45" t="s">
         <v>859</v>
@@ -25104,7 +25108,7 @@
         <v>610</v>
       </c>
       <c r="C679" s="16" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="D679" s="45" t="s">
         <v>859</v>
@@ -25125,7 +25129,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="680" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A680" s="45" t="s">
         <v>789</v>
       </c>
@@ -25133,7 +25137,7 @@
         <v>610</v>
       </c>
       <c r="C680" s="16" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="D680" s="45" t="s">
         <v>860</v>
@@ -25160,7 +25164,7 @@
         <v>610</v>
       </c>
       <c r="C681" s="16" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
       <c r="D681" s="45" t="s">
         <v>860</v>
@@ -25181,7 +25185,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="682" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="682" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A682" s="45" t="s">
         <v>791</v>
       </c>
@@ -25189,7 +25193,7 @@
         <v>610</v>
       </c>
       <c r="C682" s="16" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="D682" s="45" t="s">
         <v>861</v>
@@ -25216,7 +25220,7 @@
         <v>610</v>
       </c>
       <c r="C683" s="16" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
       <c r="D683" s="45" t="s">
         <v>861</v>
@@ -25237,7 +25241,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="684" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="684" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A684" s="45" t="s">
         <v>793</v>
       </c>
@@ -25245,7 +25249,7 @@
         <v>610</v>
       </c>
       <c r="C684" s="16" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="D684" s="45" t="s">
         <v>862</v>
@@ -25272,7 +25276,7 @@
         <v>610</v>
       </c>
       <c r="C685" s="16" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
       <c r="D685" s="45" t="s">
         <v>862</v>
@@ -25293,7 +25297,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="686" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A686" s="45" t="s">
         <v>795</v>
       </c>
@@ -25301,7 +25305,7 @@
         <v>610</v>
       </c>
       <c r="C686" s="16" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="D686" s="45" t="s">
         <v>863</v>
@@ -25328,7 +25332,7 @@
         <v>610</v>
       </c>
       <c r="C687" s="47" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="D687" s="45" t="s">
         <v>863</v>
@@ -25349,7 +25353,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="688" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="688" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A688" s="45" t="s">
         <v>797</v>
       </c>
@@ -25357,7 +25361,7 @@
         <v>610</v>
       </c>
       <c r="C688" s="16" t="s">
-        <v>1738</v>
+        <v>1733</v>
       </c>
       <c r="D688" s="45" t="s">
         <v>864</v>
@@ -25384,7 +25388,7 @@
         <v>610</v>
       </c>
       <c r="C689" s="47" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
       <c r="D689" s="45" t="s">
         <v>864</v>
@@ -25405,7 +25409,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="690" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A690" s="45" t="s">
         <v>799</v>
       </c>
@@ -25413,7 +25417,7 @@
         <v>610</v>
       </c>
       <c r="C690" s="47" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="D690" s="45" t="s">
         <v>865</v>
@@ -25440,7 +25444,7 @@
         <v>610</v>
       </c>
       <c r="C691" s="16" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
       <c r="D691" s="45" t="s">
         <v>865</v>
@@ -25455,11 +25459,11 @@
         <v>15</v>
       </c>
       <c r="H691" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I691" s="47"/>
     </row>
-    <row r="692" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="692" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A692" s="45" t="s">
         <v>801</v>
       </c>
@@ -25467,7 +25471,7 @@
         <v>610</v>
       </c>
       <c r="C692" s="16" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="D692" s="45" t="s">
         <v>866</v>
@@ -25494,7 +25498,7 @@
         <v>610</v>
       </c>
       <c r="C693" s="16" t="s">
-        <v>1717</v>
+        <v>1712</v>
       </c>
       <c r="D693" s="45" t="s">
         <v>866</v>
@@ -25515,7 +25519,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="694" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A694" s="45" t="s">
         <v>803</v>
       </c>
@@ -25523,7 +25527,7 @@
         <v>610</v>
       </c>
       <c r="C694" s="16" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
       <c r="D694" s="45" t="s">
         <v>867</v>
@@ -25550,7 +25554,7 @@
         <v>610</v>
       </c>
       <c r="C695" s="16" t="s">
-        <v>1697</v>
+        <v>1692</v>
       </c>
       <c r="D695" s="45" t="s">
         <v>867</v>
@@ -25571,7 +25575,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="696" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A696" s="45" t="s">
         <v>812</v>
       </c>
@@ -25579,7 +25583,7 @@
         <v>610</v>
       </c>
       <c r="C696" s="16" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="D696" s="45" t="s">
         <v>868</v>
@@ -25606,7 +25610,7 @@
         <v>610</v>
       </c>
       <c r="C697" s="16" t="s">
-        <v>1718</v>
+        <v>1713</v>
       </c>
       <c r="D697" s="45" t="s">
         <v>868</v>
@@ -25627,7 +25631,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="698" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="698" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A698" s="45" t="s">
         <v>814</v>
       </c>
@@ -25635,7 +25639,7 @@
         <v>610</v>
       </c>
       <c r="C698" s="16" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="D698" s="45" t="s">
         <v>869</v>
@@ -25662,7 +25666,7 @@
         <v>610</v>
       </c>
       <c r="C699" s="16" t="s">
-        <v>1660</v>
+        <v>1656</v>
       </c>
       <c r="D699" s="45" t="s">
         <v>869</v>
@@ -25683,7 +25687,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="700" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A700" s="45" t="s">
         <v>816</v>
       </c>
@@ -25691,7 +25695,7 @@
         <v>610</v>
       </c>
       <c r="C700" s="16" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="D700" s="45" t="s">
         <v>870</v>
@@ -25718,7 +25722,7 @@
         <v>610</v>
       </c>
       <c r="C701" s="16" t="s">
-        <v>1721</v>
+        <v>1716</v>
       </c>
       <c r="D701" s="45" t="s">
         <v>870</v>
@@ -25739,7 +25743,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="702" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="702" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A702" s="18" t="s">
         <v>818</v>
       </c>
@@ -25747,7 +25751,7 @@
         <v>610</v>
       </c>
       <c r="C702" s="16" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="D702" s="45" t="s">
         <v>871</v>
@@ -25774,7 +25778,7 @@
         <v>8</v>
       </c>
       <c r="C703" s="16" t="s">
-        <v>1736</v>
+        <v>1731</v>
       </c>
       <c r="D703" s="45" t="s">
         <v>871</v>
@@ -25789,24 +25793,24 @@
         <v>15</v>
       </c>
       <c r="H703" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I703" s="47" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="704" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A704" s="18" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
       <c r="B704" s="49">
         <v>8</v>
       </c>
       <c r="C704" s="16" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="D704" s="18" t="s">
-        <v>1731</v>
+        <v>1726</v>
       </c>
       <c r="E704" s="45" t="s">
         <v>22</v>
@@ -25824,16 +25828,16 @@
     </row>
     <row r="705" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A705" s="18" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
       <c r="B705" s="49">
         <v>8</v>
       </c>
       <c r="C705" s="16" t="s">
-        <v>1723</v>
+        <v>1718</v>
       </c>
       <c r="D705" s="18" t="s">
-        <v>1731</v>
+        <v>1726</v>
       </c>
       <c r="E705" s="45" t="s">
         <v>22</v>
@@ -25845,24 +25849,24 @@
         <v>15</v>
       </c>
       <c r="H705" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I705" s="16" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="706" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A706" s="18" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
       <c r="B706" s="49">
         <v>8</v>
       </c>
       <c r="C706" s="16" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
       <c r="D706" s="18" t="s">
-        <v>1734</v>
+        <v>1729</v>
       </c>
       <c r="E706" s="45" t="s">
         <v>22</v>
@@ -25880,16 +25884,16 @@
     </row>
     <row r="707" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A707" s="18" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="B707" s="49">
         <v>8</v>
       </c>
       <c r="C707" s="16" t="s">
-        <v>1727</v>
+        <v>1722</v>
       </c>
       <c r="D707" s="18" t="s">
-        <v>1734</v>
+        <v>1729</v>
       </c>
       <c r="E707" s="45" t="s">
         <v>22</v>
@@ -25901,24 +25905,24 @@
         <v>15</v>
       </c>
       <c r="H707" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I707" s="16" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="708" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="708" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A708" s="18" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
       <c r="B708" s="49">
         <v>8</v>
       </c>
       <c r="C708" s="16" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="D708" s="18" t="s">
-        <v>1735</v>
+        <v>1730</v>
       </c>
       <c r="E708" s="45" t="s">
         <v>22</v>
@@ -25936,16 +25940,16 @@
     </row>
     <row r="709" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A709" s="18" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="B709" s="49">
         <v>8</v>
       </c>
       <c r="C709" s="16" t="s">
-        <v>1728</v>
+        <v>1723</v>
       </c>
       <c r="D709" s="18" t="s">
-        <v>1735</v>
+        <v>1730</v>
       </c>
       <c r="E709" s="45" t="s">
         <v>22</v>
@@ -25957,24 +25961,24 @@
         <v>15</v>
       </c>
       <c r="H709" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I709" s="16" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="710" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="710" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A710" s="18" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="B710" s="49">
         <v>8</v>
       </c>
       <c r="C710" s="16" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
       <c r="D710" s="18" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="E710" s="45" t="s">
         <v>22</v>
@@ -25992,16 +25996,16 @@
     </row>
     <row r="711" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A711" s="18" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
       <c r="B711" s="49">
         <v>8</v>
       </c>
       <c r="C711" s="16" t="s">
-        <v>1637</v>
+        <v>1634</v>
       </c>
       <c r="D711" s="18" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
       <c r="E711" s="45" t="s">
         <v>22</v>
@@ -26013,13 +26017,13 @@
         <v>15</v>
       </c>
       <c r="H711" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I711" s="16" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="712" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="712" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A712" s="45" t="s">
         <v>820</v>
       </c>
@@ -26027,7 +26031,7 @@
         <v>610</v>
       </c>
       <c r="C712" s="16" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="D712" s="45" t="s">
         <v>1425</v>
@@ -26046,7 +26050,7 @@
       </c>
       <c r="I712" s="47"/>
     </row>
-    <row r="713" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="713" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A713" s="45" t="s">
         <v>821</v>
       </c>
@@ -26073,7 +26077,7 @@
       </c>
       <c r="I713" s="47"/>
     </row>
-    <row r="714" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A714" s="45" t="s">
         <v>822</v>
       </c>
@@ -26081,7 +26085,7 @@
         <v>610</v>
       </c>
       <c r="C714" s="16" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="D714" s="45" t="s">
         <v>1426</v>
@@ -26100,7 +26104,7 @@
       </c>
       <c r="I714" s="47"/>
     </row>
-    <row r="715" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="715" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A715" s="45" t="s">
         <v>823</v>
       </c>
@@ -26127,7 +26131,7 @@
       </c>
       <c r="I715" s="47"/>
     </row>
-    <row r="716" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="716" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A716" s="45" t="s">
         <v>824</v>
       </c>
@@ -26135,7 +26139,7 @@
         <v>610</v>
       </c>
       <c r="C716" s="16" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
       <c r="D716" s="45" t="s">
         <v>1427</v>
@@ -26154,7 +26158,7 @@
       </c>
       <c r="I716" s="47"/>
     </row>
-    <row r="717" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="717" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A717" s="45" t="s">
         <v>825</v>
       </c>
@@ -26181,7 +26185,7 @@
       </c>
       <c r="I717" s="47"/>
     </row>
-    <row r="718" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:9" s="50" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A718" s="45" t="s">
         <v>826</v>
       </c>
@@ -26189,7 +26193,7 @@
         <v>610</v>
       </c>
       <c r="C718" s="16" t="s">
-        <v>1681</v>
+        <v>1677</v>
       </c>
       <c r="D718" s="45" t="s">
         <v>1428</v>
@@ -26243,7 +26247,7 @@
         <v>610</v>
       </c>
       <c r="C720" s="16" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="D720" s="45" t="s">
         <v>1043</v>
@@ -26297,7 +26301,7 @@
         <v>610</v>
       </c>
       <c r="C722" s="16" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="D722" s="45" t="s">
         <v>1044</v>
@@ -26351,7 +26355,7 @@
         <v>610</v>
       </c>
       <c r="C724" s="16" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="D724" s="45" t="s">
         <v>1431</v>
@@ -26378,7 +26382,7 @@
         <v>610</v>
       </c>
       <c r="C725" s="16" t="s">
-        <v>1661</v>
+        <v>1657</v>
       </c>
       <c r="D725" s="45" t="s">
         <v>1431</v>
@@ -26407,7 +26411,7 @@
         <v>610</v>
       </c>
       <c r="C726" s="16" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="D726" s="45" t="s">
         <v>1429</v>
@@ -26434,7 +26438,7 @@
         <v>610</v>
       </c>
       <c r="C727" s="16" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="D727" s="45" t="s">
         <v>1430</v>
@@ -26463,7 +26467,7 @@
         <v>610</v>
       </c>
       <c r="C728" s="16" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="D728" s="45" t="s">
         <v>1422</v>
@@ -26490,7 +26494,7 @@
         <v>610</v>
       </c>
       <c r="C729" s="16" t="s">
-        <v>1662</v>
+        <v>1658</v>
       </c>
       <c r="D729" s="45" t="s">
         <v>1422</v>
@@ -26519,7 +26523,7 @@
         <v>610</v>
       </c>
       <c r="C730" s="16" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="D730" s="45" t="s">
         <v>1423</v>
@@ -26546,7 +26550,7 @@
         <v>610</v>
       </c>
       <c r="C731" s="16" t="s">
-        <v>1663</v>
+        <v>1659</v>
       </c>
       <c r="D731" s="45" t="s">
         <v>1423</v>
@@ -26575,7 +26579,7 @@
         <v>610</v>
       </c>
       <c r="C732" s="16" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="D732" s="45" t="s">
         <v>1424</v>
@@ -26631,7 +26635,7 @@
         <v>610</v>
       </c>
       <c r="C734" s="16" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="D734" s="45" t="s">
         <v>1432</v>
@@ -26658,7 +26662,7 @@
         <v>610</v>
       </c>
       <c r="C735" s="16" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="D735" s="45" t="s">
         <v>1432</v>
@@ -26673,7 +26677,7 @@
         <v>15</v>
       </c>
       <c r="H735" s="18" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="I735" s="47"/>
     </row>
@@ -26685,7 +26689,7 @@
         <v>610</v>
       </c>
       <c r="C736" s="16" t="s">
-        <v>1713</v>
+        <v>1708</v>
       </c>
       <c r="D736" s="45" t="s">
         <v>1433</v>
@@ -26712,10 +26716,10 @@
         <v>610</v>
       </c>
       <c r="C737" s="16" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
       <c r="D737" s="18" t="s">
-        <v>1699</v>
+        <v>1694</v>
       </c>
       <c r="E737" s="45" t="s">
         <v>22</v>
@@ -26741,7 +26745,7 @@
         <v>610</v>
       </c>
       <c r="C738" s="16" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="D738" s="45" t="s">
         <v>942</v>
@@ -26768,7 +26772,7 @@
         <v>610</v>
       </c>
       <c r="C739" s="16" t="s">
-        <v>1664</v>
+        <v>1660</v>
       </c>
       <c r="D739" s="45" t="s">
         <v>942</v>
@@ -26797,7 +26801,7 @@
         <v>610</v>
       </c>
       <c r="C740" s="16" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="D740" s="45" t="s">
         <v>944</v>
@@ -26824,7 +26828,7 @@
         <v>610</v>
       </c>
       <c r="C741" s="16" t="s">
-        <v>1694</v>
+        <v>1690</v>
       </c>
       <c r="D741" s="45" t="s">
         <v>944</v>
@@ -26853,7 +26857,7 @@
         <v>610</v>
       </c>
       <c r="C742" s="16" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="D742" s="45" t="s">
         <v>946</v>
@@ -26880,7 +26884,7 @@
         <v>610</v>
       </c>
       <c r="C743" s="16" t="s">
-        <v>1665</v>
+        <v>1661</v>
       </c>
       <c r="D743" s="45" t="s">
         <v>946</v>
@@ -26909,7 +26913,7 @@
         <v>610</v>
       </c>
       <c r="C744" s="16" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="D744" s="45" t="s">
         <v>948</v>
@@ -26936,7 +26940,7 @@
         <v>610</v>
       </c>
       <c r="C745" s="16" t="s">
-        <v>1693</v>
+        <v>1689</v>
       </c>
       <c r="D745" s="45" t="s">
         <v>948</v>
@@ -26965,7 +26969,7 @@
         <v>610</v>
       </c>
       <c r="C746" s="16" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="D746" s="45" t="s">
         <v>950</v>
@@ -26986,13 +26990,13 @@
     </row>
     <row r="747" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A747" s="18" t="s">
-        <v>1692</v>
+        <v>1688</v>
       </c>
       <c r="B747" s="46" t="s">
         <v>610</v>
       </c>
       <c r="C747" s="16" t="s">
-        <v>1689</v>
+        <v>1685</v>
       </c>
       <c r="D747" s="45" t="s">
         <v>950</v>
@@ -27021,7 +27025,7 @@
         <v>610</v>
       </c>
       <c r="C748" s="16" t="s">
-        <v>1688</v>
+        <v>1684</v>
       </c>
       <c r="D748" s="45" t="s">
         <v>960</v>
@@ -27048,7 +27052,7 @@
         <v>610</v>
       </c>
       <c r="C749" s="16" t="s">
-        <v>1666</v>
+        <v>1662</v>
       </c>
       <c r="D749" s="45" t="s">
         <v>960</v>
@@ -27063,7 +27067,7 @@
         <v>15</v>
       </c>
       <c r="H749" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I749" s="47" t="s">
         <v>1434</v>
@@ -27077,7 +27081,7 @@
         <v>610</v>
       </c>
       <c r="C750" s="16" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="D750" s="45" t="s">
         <v>962</v>
@@ -27098,13 +27102,13 @@
     </row>
     <row r="751" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A751" s="18" t="s">
-        <v>1686</v>
+        <v>1682</v>
       </c>
       <c r="B751" s="46" t="s">
         <v>610</v>
       </c>
       <c r="C751" s="16" t="s">
-        <v>1687</v>
+        <v>1683</v>
       </c>
       <c r="D751" s="45" t="s">
         <v>962</v>
@@ -27119,7 +27123,7 @@
         <v>15</v>
       </c>
       <c r="H751" s="18" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="I751" s="16" t="s">
         <v>1434</v>
@@ -27127,16 +27131,16 @@
     </row>
     <row r="752" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A752" s="18" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
       <c r="B752" s="49">
         <v>8</v>
       </c>
       <c r="C752" s="16" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="D752" s="18" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="E752" s="45" t="s">
         <v>22</v>
@@ -27154,16 +27158,16 @@
     </row>
     <row r="753" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A753" s="18" t="s">
-        <v>1685</v>
+        <v>1681</v>
       </c>
       <c r="B753" s="49">
         <v>8</v>
       </c>
       <c r="C753" s="16" t="s">
-        <v>1667</v>
+        <v>1663</v>
       </c>
       <c r="D753" s="18" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="E753" s="45" t="s">
         <v>22</v>
@@ -27181,7 +27185,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="754" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A754" s="18" t="s">
         <v>858</v>
       </c>
@@ -27189,9 +27193,9 @@
         <v>610</v>
       </c>
       <c r="C754" s="16" t="s">
-        <v>1607</v>
-      </c>
-      <c r="D754" t="s">
+        <v>1604</v>
+      </c>
+      <c r="D754" s="51" t="s">
         <v>1451</v>
       </c>
       <c r="E754" s="45" t="s">
@@ -27210,16 +27214,16 @@
     </row>
     <row r="755" spans="1:9" s="50" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A755" s="18" t="s">
-        <v>1684</v>
+        <v>1680</v>
       </c>
       <c r="B755" s="46" t="s">
         <v>610</v>
       </c>
       <c r="C755" s="16" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
       <c r="D755" s="51" t="s">
-        <v>1668</v>
+        <v>1664</v>
       </c>
       <c r="E755" s="45" t="s">
         <v>22</v>
@@ -27242,10 +27246,10 @@
         <v>1391</v>
       </c>
       <c r="B756" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C756" s="16" t="s">
-        <v>1675</v>
+        <v>1671</v>
       </c>
       <c r="D756" s="45"/>
       <c r="E756" s="45" t="s">
@@ -27267,7 +27271,7 @@
         <v>1392</v>
       </c>
       <c r="B757" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C757" s="47" t="s">
         <v>1390</v>
@@ -27292,10 +27296,10 @@
         <v>1393</v>
       </c>
       <c r="B758" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C758" s="16" t="s">
-        <v>1680</v>
+        <v>1676</v>
       </c>
       <c r="D758" s="45"/>
       <c r="E758" s="45" t="s">
@@ -27317,10 +27321,10 @@
         <v>1394</v>
       </c>
       <c r="B759" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C759" s="16" t="s">
-        <v>1677</v>
+        <v>1673</v>
       </c>
       <c r="D759" s="45"/>
       <c r="E759" s="45" t="s">
@@ -27342,10 +27346,10 @@
         <v>1395</v>
       </c>
       <c r="B760" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C760" s="16" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="D760" s="45"/>
       <c r="E760" s="45" t="s">
@@ -27367,10 +27371,10 @@
         <v>1396</v>
       </c>
       <c r="B761" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C761" s="16" t="s">
-        <v>1674</v>
+        <v>1670</v>
       </c>
       <c r="D761" s="45"/>
       <c r="E761" s="45" t="s">
@@ -27392,10 +27396,10 @@
         <v>1397</v>
       </c>
       <c r="B762" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C762" s="16" t="s">
-        <v>1669</v>
+        <v>1665</v>
       </c>
       <c r="D762" s="45"/>
       <c r="E762" s="45" t="s">
@@ -27417,10 +27421,10 @@
         <v>1398</v>
       </c>
       <c r="B763" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C763" s="16" t="s">
-        <v>1676</v>
+        <v>1672</v>
       </c>
       <c r="D763" s="45"/>
       <c r="E763" s="45" t="s">
@@ -27442,10 +27446,10 @@
         <v>1399</v>
       </c>
       <c r="B764" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C764" s="16" t="s">
-        <v>1679</v>
+        <v>1675</v>
       </c>
       <c r="D764" s="45"/>
       <c r="E764" s="45" t="s">
@@ -27467,10 +27471,10 @@
         <v>1400</v>
       </c>
       <c r="B765" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C765" s="16" t="s">
-        <v>1678</v>
+        <v>1674</v>
       </c>
       <c r="D765" s="45"/>
       <c r="E765" s="45" t="s">
@@ -27492,10 +27496,10 @@
         <v>1401</v>
       </c>
       <c r="B766" s="20" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C766" s="16" t="s">
-        <v>1673</v>
+        <v>1669</v>
       </c>
       <c r="D766" s="45"/>
       <c r="E766" s="45" t="s">
@@ -27545,7 +27549,7 @@
         <v>1382</v>
       </c>
       <c r="C768" s="16" t="s">
-        <v>1672</v>
+        <v>1668</v>
       </c>
       <c r="D768" s="25"/>
       <c r="E768" s="25" t="s">
@@ -27570,7 +27574,7 @@
         <v>1376</v>
       </c>
       <c r="C769" s="16" t="s">
-        <v>1670</v>
+        <v>1666</v>
       </c>
       <c r="D769" s="45"/>
       <c r="E769" s="45" t="s">
@@ -27620,7 +27624,7 @@
         <v>1384</v>
       </c>
       <c r="C771" s="16" t="s">
-        <v>1671</v>
+        <v>1667</v>
       </c>
       <c r="D771" s="45"/>
       <c r="E771" s="45" t="s">
@@ -27950,7 +27954,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B782:B783 B10:B27 B54:B63 B28:B51 B65:B67 B70:B235 B244:B270 B273:B596 B598 B754:B755 B601:B669 B672:B702 B767:B780 B712:B751" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B782:B783 B10:B27 B53:B64 B28:B52 B65:B600 B753:B766 B601:B711 B767:B780 B712:B752 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Added BirthdayLocal R12750102Enabled and WeddingAnniversaryLocal R12750104Enabled
</commit_message>
<xml_diff>
--- a/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
+++ b/ExchangeWebServices/Docs/MS-OXWSCONT/MS-OXWSCONT_RequirementSpecification.xlsx
@@ -3,15 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7092CE3B-F645-4246-8550-8AE556DBADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10117086-19B2-45AB-9EB3-5B43CF99CC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$780</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$784</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5526" uniqueCount="1740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5558" uniqueCount="1752">
   <si>
     <t>Req ID</t>
   </si>
@@ -6871,6 +6871,42 @@
   <si>
     <t>[In t:ContactItemType Complex Type] WeddingAnniversaryLocal element: Contains the wedding anniversary date of a contact (2) in the client's local time zone.&lt;7&gt;</t>
   </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the BirthdayLocal element. (&lt;6&gt; Section 2.2.4.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the BirthdayLocal element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the BirthdayLocal element. (Exchange 2016 and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R4701:i</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R12750101</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R12750102</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R12750102.</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does not support the WeddingAnniversaryLocal element. (&lt;7&gt; Section 2.2.4.3:  Exchange 2007, Exchange 2010, and Exchange 2013 do not support the WeddingAnniversaryLocal element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix C: Product Behavior] Implementation does support the WeddingAnniversaryLocal element. (Exchange 2016 and above follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R12750103</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R12750104</t>
+  </si>
+  <si>
+    <t>MS-OXWSCONT_R7902:i</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-OXWSCONT_R12750104.</t>
+  </si>
 </sst>
 </file>
 
@@ -7137,7 +7173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7244,6 +7280,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7301,10 +7340,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7312,20 +7351,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike/>
@@ -7355,6 +7380,20 @@
       <font>
         <strike/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -7804,8 +7843,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I780" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
-  <autoFilter ref="A19:I780" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I784" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
+  <autoFilter ref="A19:I784" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -8173,10 +8212,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I783"/>
+  <dimension ref="A1:I787"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C148" sqref="C148"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8232,16 +8271,16 @@
       <c r="I3" s="28"/>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
       <c r="I4" s="28"/>
     </row>
     <row r="5" spans="1:9">
@@ -8251,103 +8290,103 @@
       <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="51"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="52" t="s">
+      <c r="B7" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="54"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="52" t="s">
+      <c r="B8" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="54"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="55"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="58"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1">
       <c r="A11" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="59" t="s">
         <v>589</v>
       </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="46"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="47"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="18" t="s">
@@ -8421,46 +8460,46 @@
       <c r="A16" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="46"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="1:9" ht="64.5" customHeight="1">
       <c r="A17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="62" t="s">
+      <c r="B17" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="47"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1">
       <c r="A18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="45" t="s">
         <v>590</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="46"/>
+      <c r="C18" s="46"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="47"/>
     </row>
     <row r="19" spans="1:9" ht="30">
       <c r="A19" s="3" t="s">
@@ -10855,7 +10894,7 @@
       <c r="C114" s="13" t="s">
         <v>1628</v>
       </c>
-      <c r="D114" s="63"/>
+      <c r="D114" s="44"/>
       <c r="E114" s="21" t="s">
         <v>19</v>
       </c>
@@ -10865,12 +10904,12 @@
       <c r="G114" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H114" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I114" s="64"/>
-    </row>
-    <row r="115" spans="1:9" ht="30">
+      <c r="H114" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I114" s="41"/>
+    </row>
+    <row r="115" spans="1:9" ht="45">
       <c r="A115" s="14" t="s">
         <v>1627</v>
       </c>
@@ -10880,7 +10919,7 @@
       <c r="C115" s="13" t="s">
         <v>1629</v>
       </c>
-      <c r="D115" s="63"/>
+      <c r="D115" s="44"/>
       <c r="E115" s="21" t="s">
         <v>19</v>
       </c>
@@ -10890,10 +10929,12 @@
       <c r="G115" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H115" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I115" s="64"/>
+      <c r="H115" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="I115" s="13" t="s">
+        <v>1745</v>
+      </c>
     </row>
     <row r="116" spans="1:9" ht="30">
       <c r="A116" s="21" t="s">
@@ -11715,12 +11756,12 @@
       <c r="G148" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="H148" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I148" s="64"/>
-    </row>
-    <row r="149" spans="1:9" ht="30">
+      <c r="H148" s="14" t="s">
+        <v>1484</v>
+      </c>
+      <c r="I148" s="23"/>
+    </row>
+    <row r="149" spans="1:9" ht="45">
       <c r="A149" s="14" t="s">
         <v>1738</v>
       </c>
@@ -11741,9 +11782,11 @@
         <v>15</v>
       </c>
       <c r="H149" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="I149" s="64"/>
+        <v>17</v>
+      </c>
+      <c r="I149" s="13" t="s">
+        <v>1751</v>
+      </c>
     </row>
     <row r="150" spans="1:9" ht="30">
       <c r="A150" s="14" t="s">
@@ -12420,7 +12463,7 @@
       <c r="H176" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="I176" s="41" t="s">
+      <c r="I176" s="13" t="s">
         <v>1426</v>
       </c>
     </row>
@@ -24995,18 +25038,18 @@
       </c>
       <c r="I675" s="23"/>
     </row>
-    <row r="676" spans="1:9" ht="30">
-      <c r="A676" s="39" t="s">
-        <v>688</v>
-      </c>
-      <c r="B676" s="40" t="s">
-        <v>607</v>
+    <row r="676" spans="1:9" ht="45">
+      <c r="A676" s="14" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B676" s="65">
+        <v>8</v>
       </c>
       <c r="C676" s="13" t="s">
-        <v>1702</v>
-      </c>
-      <c r="D676" s="14" t="s">
-        <v>1701</v>
+        <v>1740</v>
+      </c>
+      <c r="D676" s="64" t="s">
+        <v>1742</v>
       </c>
       <c r="E676" s="39" t="s">
         <v>22</v>
@@ -25024,16 +25067,16 @@
     </row>
     <row r="677" spans="1:9" ht="45">
       <c r="A677" s="14" t="s">
-        <v>1421</v>
-      </c>
-      <c r="B677" s="40" t="s">
-        <v>607</v>
+        <v>1744</v>
+      </c>
+      <c r="B677" s="65">
+        <v>8</v>
       </c>
       <c r="C677" s="13" t="s">
-        <v>1554</v>
-      </c>
-      <c r="D677" s="39" t="s">
-        <v>1420</v>
+        <v>1741</v>
+      </c>
+      <c r="D677" s="64" t="s">
+        <v>1742</v>
       </c>
       <c r="E677" s="39" t="s">
         <v>22</v>
@@ -25044,25 +25087,25 @@
       <c r="G677" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H677" s="14" t="s">
-        <v>1487</v>
+      <c r="H677" s="39" t="s">
+        <v>21</v>
       </c>
       <c r="I677" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="678" spans="1:9" ht="45">
-      <c r="A678" s="39" t="s">
-        <v>733</v>
-      </c>
-      <c r="B678" s="40" t="s">
-        <v>607</v>
+      <c r="A678" s="14" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B678" s="65">
+        <v>8</v>
       </c>
       <c r="C678" s="13" t="s">
-        <v>1703</v>
-      </c>
-      <c r="D678" s="14" t="s">
-        <v>848</v>
+        <v>1746</v>
+      </c>
+      <c r="D678" s="64" t="s">
+        <v>1750</v>
       </c>
       <c r="E678" s="39" t="s">
         <v>22</v>
@@ -25079,17 +25122,17 @@
       <c r="I678" s="41"/>
     </row>
     <row r="679" spans="1:9" ht="45">
-      <c r="A679" s="39" t="s">
-        <v>734</v>
-      </c>
-      <c r="B679" s="40" t="s">
-        <v>607</v>
+      <c r="A679" s="14" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B679" s="65">
+        <v>8</v>
       </c>
       <c r="C679" s="13" t="s">
-        <v>1493</v>
-      </c>
-      <c r="D679" s="39" t="s">
-        <v>848</v>
+        <v>1747</v>
+      </c>
+      <c r="D679" s="64" t="s">
+        <v>1750</v>
       </c>
       <c r="E679" s="39" t="s">
         <v>22</v>
@@ -25107,18 +25150,18 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="680" spans="1:9" ht="45">
+    <row r="680" spans="1:9" ht="30">
       <c r="A680" s="39" t="s">
-        <v>778</v>
+        <v>688</v>
       </c>
       <c r="B680" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C680" s="13" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="D680" s="14" t="s">
-        <v>849</v>
+        <v>1701</v>
       </c>
       <c r="E680" s="39" t="s">
         <v>22</v>
@@ -25135,17 +25178,17 @@
       <c r="I680" s="41"/>
     </row>
     <row r="681" spans="1:9" ht="45">
-      <c r="A681" s="39" t="s">
-        <v>779</v>
+      <c r="A681" s="14" t="s">
+        <v>1421</v>
       </c>
       <c r="B681" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C681" s="13" t="s">
-        <v>1495</v>
+        <v>1554</v>
       </c>
       <c r="D681" s="39" t="s">
-        <v>849</v>
+        <v>1420</v>
       </c>
       <c r="E681" s="39" t="s">
         <v>22</v>
@@ -25156,8 +25199,8 @@
       <c r="G681" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H681" s="39" t="s">
-        <v>21</v>
+      <c r="H681" s="14" t="s">
+        <v>1487</v>
       </c>
       <c r="I681" s="41" t="s">
         <v>1411</v>
@@ -25165,16 +25208,16 @@
     </row>
     <row r="682" spans="1:9" ht="45">
       <c r="A682" s="39" t="s">
-        <v>780</v>
+        <v>733</v>
       </c>
       <c r="B682" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C682" s="13" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="D682" s="14" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E682" s="39" t="s">
         <v>22</v>
@@ -25192,16 +25235,16 @@
     </row>
     <row r="683" spans="1:9" ht="45">
       <c r="A683" s="39" t="s">
-        <v>781</v>
+        <v>734</v>
       </c>
       <c r="B683" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C683" s="13" t="s">
-        <v>1497</v>
+        <v>1493</v>
       </c>
       <c r="D683" s="39" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="E683" s="39" t="s">
         <v>22</v>
@@ -25221,16 +25264,16 @@
     </row>
     <row r="684" spans="1:9" ht="45">
       <c r="A684" s="39" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="B684" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C684" s="13" t="s">
-        <v>1706</v>
-      </c>
-      <c r="D684" s="39" t="s">
-        <v>851</v>
+        <v>1704</v>
+      </c>
+      <c r="D684" s="14" t="s">
+        <v>849</v>
       </c>
       <c r="E684" s="39" t="s">
         <v>22</v>
@@ -25248,16 +25291,16 @@
     </row>
     <row r="685" spans="1:9" ht="45">
       <c r="A685" s="39" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
       <c r="B685" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C685" s="13" t="s">
-        <v>1499</v>
+        <v>1495</v>
       </c>
       <c r="D685" s="39" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="E685" s="39" t="s">
         <v>22</v>
@@ -25277,16 +25320,16 @@
     </row>
     <row r="686" spans="1:9" ht="45">
       <c r="A686" s="39" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
       <c r="B686" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C686" s="13" t="s">
-        <v>1707</v>
-      </c>
-      <c r="D686" s="39" t="s">
-        <v>852</v>
+        <v>1705</v>
+      </c>
+      <c r="D686" s="14" t="s">
+        <v>850</v>
       </c>
       <c r="E686" s="39" t="s">
         <v>22</v>
@@ -25304,16 +25347,16 @@
     </row>
     <row r="687" spans="1:9" ht="45">
       <c r="A687" s="39" t="s">
-        <v>785</v>
+        <v>781</v>
       </c>
       <c r="B687" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C687" s="41" t="s">
-        <v>1463</v>
+      <c r="C687" s="13" t="s">
+        <v>1497</v>
       </c>
       <c r="D687" s="39" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="E687" s="39" t="s">
         <v>22</v>
@@ -25333,16 +25376,16 @@
     </row>
     <row r="688" spans="1:9" ht="45">
       <c r="A688" s="39" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="B688" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C688" s="13" t="s">
-        <v>1614</v>
+        <v>1706</v>
       </c>
       <c r="D688" s="39" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="E688" s="39" t="s">
         <v>22</v>
@@ -25360,16 +25403,16 @@
     </row>
     <row r="689" spans="1:9" ht="45">
       <c r="A689" s="39" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
       <c r="B689" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C689" s="41" t="s">
-        <v>1464</v>
+      <c r="C689" s="13" t="s">
+        <v>1499</v>
       </c>
       <c r="D689" s="39" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="E689" s="39" t="s">
         <v>22</v>
@@ -25389,16 +25432,16 @@
     </row>
     <row r="690" spans="1:9" ht="45">
       <c r="A690" s="39" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B690" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C690" s="13" t="s">
-        <v>1735</v>
-      </c>
-      <c r="D690" s="14" t="s">
-        <v>854</v>
+        <v>1707</v>
+      </c>
+      <c r="D690" s="39" t="s">
+        <v>852</v>
       </c>
       <c r="E690" s="39" t="s">
         <v>22</v>
@@ -25416,16 +25459,16 @@
     </row>
     <row r="691" spans="1:9" ht="45">
       <c r="A691" s="39" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="B691" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C691" s="13" t="s">
-        <v>1734</v>
+      <c r="C691" s="41" t="s">
+        <v>1463</v>
       </c>
       <c r="D691" s="39" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="E691" s="39" t="s">
         <v>22</v>
@@ -25445,16 +25488,16 @@
     </row>
     <row r="692" spans="1:9" ht="45">
       <c r="A692" s="39" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="B692" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C692" s="13" t="s">
-        <v>1708</v>
+        <v>1614</v>
       </c>
       <c r="D692" s="39" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="E692" s="39" t="s">
         <v>22</v>
@@ -25472,16 +25515,16 @@
     </row>
     <row r="693" spans="1:9" ht="45">
       <c r="A693" s="39" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
       <c r="B693" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C693" s="13" t="s">
-        <v>1558</v>
+      <c r="C693" s="41" t="s">
+        <v>1464</v>
       </c>
       <c r="D693" s="39" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="E693" s="39" t="s">
         <v>22</v>
@@ -25501,16 +25544,16 @@
     </row>
     <row r="694" spans="1:9" ht="45">
       <c r="A694" s="39" t="s">
-        <v>792</v>
+        <v>788</v>
       </c>
       <c r="B694" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C694" s="13" t="s">
-        <v>1465</v>
-      </c>
-      <c r="D694" s="39" t="s">
-        <v>856</v>
+        <v>1735</v>
+      </c>
+      <c r="D694" s="14" t="s">
+        <v>854</v>
       </c>
       <c r="E694" s="39" t="s">
         <v>22</v>
@@ -25528,16 +25571,16 @@
     </row>
     <row r="695" spans="1:9" ht="45">
       <c r="A695" s="39" t="s">
-        <v>793</v>
+        <v>789</v>
       </c>
       <c r="B695" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C695" s="13" t="s">
-        <v>1541</v>
+        <v>1734</v>
       </c>
       <c r="D695" s="39" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="E695" s="39" t="s">
         <v>22</v>
@@ -25557,16 +25600,16 @@
     </row>
     <row r="696" spans="1:9" ht="45">
       <c r="A696" s="39" t="s">
-        <v>801</v>
+        <v>790</v>
       </c>
       <c r="B696" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C696" s="13" t="s">
-        <v>1466</v>
+        <v>1708</v>
       </c>
       <c r="D696" s="39" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E696" s="39" t="s">
         <v>22</v>
@@ -25584,16 +25627,16 @@
     </row>
     <row r="697" spans="1:9" ht="45">
       <c r="A697" s="39" t="s">
-        <v>802</v>
+        <v>791</v>
       </c>
       <c r="B697" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C697" s="13" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="D697" s="39" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="E697" s="39" t="s">
         <v>22</v>
@@ -25613,16 +25656,16 @@
     </row>
     <row r="698" spans="1:9" ht="45">
       <c r="A698" s="39" t="s">
-        <v>803</v>
+        <v>792</v>
       </c>
       <c r="B698" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C698" s="13" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="D698" s="39" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E698" s="39" t="s">
         <v>22</v>
@@ -25640,16 +25683,16 @@
     </row>
     <row r="699" spans="1:9" ht="45">
       <c r="A699" s="39" t="s">
-        <v>804</v>
+        <v>793</v>
       </c>
       <c r="B699" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C699" s="13" t="s">
-        <v>1509</v>
+        <v>1541</v>
       </c>
       <c r="D699" s="39" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="E699" s="39" t="s">
         <v>22</v>
@@ -25669,16 +25712,16 @@
     </row>
     <row r="700" spans="1:9" ht="45">
       <c r="A700" s="39" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="B700" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C700" s="13" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
       <c r="D700" s="39" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="E700" s="39" t="s">
         <v>22</v>
@@ -25696,16 +25739,16 @@
     </row>
     <row r="701" spans="1:9" ht="45">
       <c r="A701" s="39" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
       <c r="B701" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C701" s="13" t="s">
-        <v>1562</v>
+        <v>1559</v>
       </c>
       <c r="D701" s="39" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="E701" s="39" t="s">
         <v>22</v>
@@ -25719,22 +25762,22 @@
       <c r="H701" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I701" s="13" t="s">
+      <c r="I701" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="702" spans="1:9" ht="45">
-      <c r="A702" s="14" t="s">
-        <v>807</v>
+      <c r="A702" s="39" t="s">
+        <v>803</v>
       </c>
       <c r="B702" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C702" s="13" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="D702" s="39" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="E702" s="39" t="s">
         <v>22</v>
@@ -25751,17 +25794,17 @@
       <c r="I702" s="41"/>
     </row>
     <row r="703" spans="1:9" ht="45">
-      <c r="A703" s="14" t="s">
-        <v>808</v>
-      </c>
-      <c r="B703" s="43">
-        <v>8</v>
+      <c r="A703" s="39" t="s">
+        <v>804</v>
+      </c>
+      <c r="B703" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C703" s="13" t="s">
-        <v>1576</v>
+        <v>1509</v>
       </c>
       <c r="D703" s="39" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="E703" s="39" t="s">
         <v>22</v>
@@ -25772,25 +25815,25 @@
       <c r="G703" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H703" s="14" t="s">
-        <v>1487</v>
+      <c r="H703" s="39" t="s">
+        <v>21</v>
       </c>
       <c r="I703" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="704" spans="1:9" ht="45">
-      <c r="A704" s="14" t="s">
-        <v>1470</v>
-      </c>
-      <c r="B704" s="43">
-        <v>8</v>
+      <c r="A704" s="39" t="s">
+        <v>805</v>
+      </c>
+      <c r="B704" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C704" s="13" t="s">
-        <v>1709</v>
-      </c>
-      <c r="D704" s="14" t="s">
-        <v>1571</v>
+        <v>1468</v>
+      </c>
+      <c r="D704" s="39" t="s">
+        <v>859</v>
       </c>
       <c r="E704" s="39" t="s">
         <v>22</v>
@@ -25807,17 +25850,17 @@
       <c r="I704" s="41"/>
     </row>
     <row r="705" spans="1:9" ht="45">
-      <c r="A705" s="14" t="s">
-        <v>1471</v>
-      </c>
-      <c r="B705" s="43">
-        <v>8</v>
+      <c r="A705" s="39" t="s">
+        <v>806</v>
+      </c>
+      <c r="B705" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C705" s="13" t="s">
-        <v>1563</v>
-      </c>
-      <c r="D705" s="14" t="s">
-        <v>1571</v>
+        <v>1562</v>
+      </c>
+      <c r="D705" s="39" t="s">
+        <v>859</v>
       </c>
       <c r="E705" s="39" t="s">
         <v>22</v>
@@ -25828,8 +25871,8 @@
       <c r="G705" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H705" s="14" t="s">
-        <v>1487</v>
+      <c r="H705" s="39" t="s">
+        <v>21</v>
       </c>
       <c r="I705" s="13" t="s">
         <v>1411</v>
@@ -25837,16 +25880,16 @@
     </row>
     <row r="706" spans="1:9" ht="45">
       <c r="A706" s="14" t="s">
-        <v>1472</v>
-      </c>
-      <c r="B706" s="43">
-        <v>8</v>
+        <v>807</v>
+      </c>
+      <c r="B706" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C706" s="13" t="s">
-        <v>1710</v>
-      </c>
-      <c r="D706" s="14" t="s">
-        <v>1574</v>
+        <v>1469</v>
+      </c>
+      <c r="D706" s="39" t="s">
+        <v>860</v>
       </c>
       <c r="E706" s="39" t="s">
         <v>22</v>
@@ -25864,16 +25907,16 @@
     </row>
     <row r="707" spans="1:9" ht="45">
       <c r="A707" s="14" t="s">
-        <v>1473</v>
+        <v>808</v>
       </c>
       <c r="B707" s="43">
         <v>8</v>
       </c>
       <c r="C707" s="13" t="s">
-        <v>1567</v>
-      </c>
-      <c r="D707" s="14" t="s">
-        <v>1574</v>
+        <v>1576</v>
+      </c>
+      <c r="D707" s="39" t="s">
+        <v>860</v>
       </c>
       <c r="E707" s="39" t="s">
         <v>22</v>
@@ -25887,22 +25930,22 @@
       <c r="H707" s="14" t="s">
         <v>1487</v>
       </c>
-      <c r="I707" s="13" t="s">
+      <c r="I707" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="708" spans="1:9" ht="45">
       <c r="A708" s="14" t="s">
-        <v>1474</v>
+        <v>1470</v>
       </c>
       <c r="B708" s="43">
         <v>8</v>
       </c>
       <c r="C708" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="D708" s="14" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="E708" s="39" t="s">
         <v>22</v>
@@ -25920,16 +25963,16 @@
     </row>
     <row r="709" spans="1:9" ht="45">
       <c r="A709" s="14" t="s">
-        <v>1475</v>
+        <v>1471</v>
       </c>
       <c r="B709" s="43">
         <v>8</v>
       </c>
       <c r="C709" s="13" t="s">
-        <v>1568</v>
+        <v>1563</v>
       </c>
       <c r="D709" s="14" t="s">
-        <v>1575</v>
+        <v>1571</v>
       </c>
       <c r="E709" s="39" t="s">
         <v>22</v>
@@ -25949,16 +25992,16 @@
     </row>
     <row r="710" spans="1:9" ht="45">
       <c r="A710" s="14" t="s">
-        <v>1476</v>
+        <v>1472</v>
       </c>
       <c r="B710" s="43">
         <v>8</v>
       </c>
       <c r="C710" s="13" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="D710" s="14" t="s">
-        <v>1482</v>
+        <v>1574</v>
       </c>
       <c r="E710" s="39" t="s">
         <v>22</v>
@@ -25976,16 +26019,16 @@
     </row>
     <row r="711" spans="1:9" ht="45">
       <c r="A711" s="14" t="s">
-        <v>1488</v>
+        <v>1473</v>
       </c>
       <c r="B711" s="43">
         <v>8</v>
       </c>
       <c r="C711" s="13" t="s">
-        <v>1491</v>
+        <v>1567</v>
       </c>
       <c r="D711" s="14" t="s">
-        <v>1482</v>
+        <v>1574</v>
       </c>
       <c r="E711" s="39" t="s">
         <v>22</v>
@@ -25997,24 +26040,24 @@
         <v>15</v>
       </c>
       <c r="H711" s="14" t="s">
-        <v>1484</v>
+        <v>1487</v>
       </c>
       <c r="I711" s="13" t="s">
         <v>1411</v>
       </c>
     </row>
-    <row r="712" spans="1:9" ht="60">
-      <c r="A712" s="39" t="s">
-        <v>809</v>
-      </c>
-      <c r="B712" s="40" t="s">
-        <v>607</v>
+    <row r="712" spans="1:9" ht="45">
+      <c r="A712" s="14" t="s">
+        <v>1474</v>
+      </c>
+      <c r="B712" s="43">
+        <v>8</v>
       </c>
       <c r="C712" s="13" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="D712" s="14" t="s">
-        <v>1402</v>
+        <v>1575</v>
       </c>
       <c r="E712" s="39" t="s">
         <v>22</v>
@@ -26031,17 +26074,17 @@
       <c r="I712" s="41"/>
     </row>
     <row r="713" spans="1:9" ht="45">
-      <c r="A713" s="39" t="s">
-        <v>810</v>
-      </c>
-      <c r="B713" s="40" t="s">
-        <v>607</v>
-      </c>
-      <c r="C713" s="41" t="s">
-        <v>795</v>
-      </c>
-      <c r="D713" s="39" t="s">
-        <v>1402</v>
+      <c r="A713" s="14" t="s">
+        <v>1475</v>
+      </c>
+      <c r="B713" s="43">
+        <v>8</v>
+      </c>
+      <c r="C713" s="13" t="s">
+        <v>1568</v>
+      </c>
+      <c r="D713" s="14" t="s">
+        <v>1575</v>
       </c>
       <c r="E713" s="39" t="s">
         <v>22</v>
@@ -26052,23 +26095,25 @@
       <c r="G713" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H713" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I713" s="41"/>
-    </row>
-    <row r="714" spans="1:9" ht="60">
-      <c r="A714" s="39" t="s">
-        <v>811</v>
-      </c>
-      <c r="B714" s="40" t="s">
-        <v>607</v>
+      <c r="H713" s="14" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I713" s="13" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="714" spans="1:9" ht="45">
+      <c r="A714" s="14" t="s">
+        <v>1476</v>
+      </c>
+      <c r="B714" s="43">
+        <v>8</v>
       </c>
       <c r="C714" s="13" t="s">
-        <v>1714</v>
-      </c>
-      <c r="D714" s="39" t="s">
-        <v>1403</v>
+        <v>1712</v>
+      </c>
+      <c r="D714" s="14" t="s">
+        <v>1482</v>
       </c>
       <c r="E714" s="39" t="s">
         <v>22</v>
@@ -26084,18 +26129,18 @@
       </c>
       <c r="I714" s="41"/>
     </row>
-    <row r="715" spans="1:9" ht="30">
-      <c r="A715" s="39" t="s">
-        <v>812</v>
-      </c>
-      <c r="B715" s="40" t="s">
-        <v>607</v>
-      </c>
-      <c r="C715" s="41" t="s">
-        <v>796</v>
-      </c>
-      <c r="D715" s="39" t="s">
-        <v>1403</v>
+    <row r="715" spans="1:9" ht="45">
+      <c r="A715" s="14" t="s">
+        <v>1488</v>
+      </c>
+      <c r="B715" s="43">
+        <v>8</v>
+      </c>
+      <c r="C715" s="13" t="s">
+        <v>1491</v>
+      </c>
+      <c r="D715" s="14" t="s">
+        <v>1482</v>
       </c>
       <c r="E715" s="39" t="s">
         <v>22</v>
@@ -26106,23 +26151,25 @@
       <c r="G715" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H715" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I715" s="41"/>
-    </row>
-    <row r="716" spans="1:9" ht="45">
+      <c r="H715" s="14" t="s">
+        <v>1484</v>
+      </c>
+      <c r="I715" s="13" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="716" spans="1:9" ht="60">
       <c r="A716" s="39" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="B716" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C716" s="13" t="s">
-        <v>1715</v>
-      </c>
-      <c r="D716" s="39" t="s">
-        <v>1404</v>
+        <v>1713</v>
+      </c>
+      <c r="D716" s="14" t="s">
+        <v>1402</v>
       </c>
       <c r="E716" s="39" t="s">
         <v>22</v>
@@ -26138,18 +26185,18 @@
       </c>
       <c r="I716" s="41"/>
     </row>
-    <row r="717" spans="1:9" ht="30">
+    <row r="717" spans="1:9" ht="45">
       <c r="A717" s="39" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B717" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C717" s="41" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D717" s="39" t="s">
-        <v>1404</v>
+        <v>1402</v>
       </c>
       <c r="E717" s="39" t="s">
         <v>22</v>
@@ -26167,16 +26214,16 @@
     </row>
     <row r="718" spans="1:9" ht="60">
       <c r="A718" s="39" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="B718" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C718" s="13" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="D718" s="39" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="E718" s="39" t="s">
         <v>22</v>
@@ -26192,18 +26239,18 @@
       </c>
       <c r="I718" s="41"/>
     </row>
-    <row r="719" spans="1:9" ht="45">
+    <row r="719" spans="1:9" ht="30">
       <c r="A719" s="39" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B719" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C719" s="41" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D719" s="39" t="s">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="E719" s="39" t="s">
         <v>22</v>
@@ -26221,16 +26268,16 @@
     </row>
     <row r="720" spans="1:9" ht="45">
       <c r="A720" s="39" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="B720" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C720" s="13" t="s">
-        <v>1717</v>
-      </c>
-      <c r="D720" s="14" t="s">
-        <v>1031</v>
+        <v>1715</v>
+      </c>
+      <c r="D720" s="39" t="s">
+        <v>1404</v>
       </c>
       <c r="E720" s="39" t="s">
         <v>22</v>
@@ -26248,16 +26295,16 @@
     </row>
     <row r="721" spans="1:9" ht="30">
       <c r="A721" s="39" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B721" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C721" s="41" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="D721" s="39" t="s">
-        <v>1031</v>
+        <v>1404</v>
       </c>
       <c r="E721" s="39" t="s">
         <v>22</v>
@@ -26273,18 +26320,18 @@
       </c>
       <c r="I721" s="41"/>
     </row>
-    <row r="722" spans="1:9" ht="45">
+    <row r="722" spans="1:9" ht="60">
       <c r="A722" s="39" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
       <c r="B722" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C722" s="13" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="D722" s="39" t="s">
-        <v>1032</v>
+        <v>1405</v>
       </c>
       <c r="E722" s="39" t="s">
         <v>22</v>
@@ -26300,18 +26347,18 @@
       </c>
       <c r="I722" s="41"/>
     </row>
-    <row r="723" spans="1:9" ht="30">
+    <row r="723" spans="1:9" ht="45">
       <c r="A723" s="39" t="s">
-        <v>820</v>
+        <v>816</v>
       </c>
       <c r="B723" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C723" s="41" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="D723" s="39" t="s">
-        <v>1032</v>
+        <v>1405</v>
       </c>
       <c r="E723" s="39" t="s">
         <v>22</v>
@@ -26327,18 +26374,18 @@
       </c>
       <c r="I723" s="41"/>
     </row>
-    <row r="724" spans="1:9" ht="60">
+    <row r="724" spans="1:9" ht="45">
       <c r="A724" s="39" t="s">
-        <v>821</v>
+        <v>817</v>
       </c>
       <c r="B724" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C724" s="13" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="D724" s="14" t="s">
-        <v>1408</v>
+        <v>1031</v>
       </c>
       <c r="E724" s="39" t="s">
         <v>22</v>
@@ -26354,18 +26401,18 @@
       </c>
       <c r="I724" s="41"/>
     </row>
-    <row r="725" spans="1:9" ht="45">
+    <row r="725" spans="1:9" ht="30">
       <c r="A725" s="39" t="s">
-        <v>822</v>
+        <v>818</v>
       </c>
       <c r="B725" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C725" s="13" t="s">
-        <v>1510</v>
-      </c>
-      <c r="D725" s="14" t="s">
-        <v>1408</v>
+      <c r="C725" s="41" t="s">
+        <v>799</v>
+      </c>
+      <c r="D725" s="39" t="s">
+        <v>1031</v>
       </c>
       <c r="E725" s="39" t="s">
         <v>22</v>
@@ -26377,24 +26424,22 @@
         <v>15</v>
       </c>
       <c r="H725" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I725" s="41" t="s">
-        <v>1411</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I725" s="41"/>
     </row>
     <row r="726" spans="1:9" ht="45">
       <c r="A726" s="39" t="s">
-        <v>823</v>
+        <v>819</v>
       </c>
       <c r="B726" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C726" s="13" t="s">
-        <v>1720</v>
-      </c>
-      <c r="D726" s="14" t="s">
-        <v>1406</v>
+        <v>1718</v>
+      </c>
+      <c r="D726" s="39" t="s">
+        <v>1032</v>
       </c>
       <c r="E726" s="39" t="s">
         <v>22</v>
@@ -26410,18 +26455,18 @@
       </c>
       <c r="I726" s="41"/>
     </row>
-    <row r="727" spans="1:9" ht="45">
+    <row r="727" spans="1:9" ht="30">
       <c r="A727" s="39" t="s">
-        <v>824</v>
+        <v>820</v>
       </c>
       <c r="B727" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C727" s="13" t="s">
-        <v>1507</v>
-      </c>
-      <c r="D727" s="14" t="s">
-        <v>1407</v>
+      <c r="C727" s="41" t="s">
+        <v>800</v>
+      </c>
+      <c r="D727" s="39" t="s">
+        <v>1032</v>
       </c>
       <c r="E727" s="39" t="s">
         <v>22</v>
@@ -26433,24 +26478,22 @@
         <v>15</v>
       </c>
       <c r="H727" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I727" s="41" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="728" spans="1:9" ht="30">
+        <v>18</v>
+      </c>
+      <c r="I727" s="41"/>
+    </row>
+    <row r="728" spans="1:9" ht="60">
       <c r="A728" s="39" t="s">
-        <v>825</v>
+        <v>821</v>
       </c>
       <c r="B728" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C728" s="13" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="D728" s="14" t="s">
-        <v>1399</v>
+        <v>1408</v>
       </c>
       <c r="E728" s="39" t="s">
         <v>22</v>
@@ -26468,16 +26511,16 @@
     </row>
     <row r="729" spans="1:9" ht="45">
       <c r="A729" s="39" t="s">
-        <v>826</v>
+        <v>822</v>
       </c>
       <c r="B729" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C729" s="13" t="s">
-        <v>1511</v>
-      </c>
-      <c r="D729" s="39" t="s">
-        <v>1399</v>
+        <v>1510</v>
+      </c>
+      <c r="D729" s="14" t="s">
+        <v>1408</v>
       </c>
       <c r="E729" s="39" t="s">
         <v>22</v>
@@ -26497,16 +26540,16 @@
     </row>
     <row r="730" spans="1:9" ht="45">
       <c r="A730" s="39" t="s">
-        <v>827</v>
+        <v>823</v>
       </c>
       <c r="B730" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C730" s="13" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="D730" s="14" t="s">
-        <v>1400</v>
+        <v>1406</v>
       </c>
       <c r="E730" s="39" t="s">
         <v>22</v>
@@ -26524,16 +26567,16 @@
     </row>
     <row r="731" spans="1:9" ht="45">
       <c r="A731" s="39" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="B731" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C731" s="13" t="s">
-        <v>1512</v>
-      </c>
-      <c r="D731" s="39" t="s">
-        <v>1400</v>
+        <v>1507</v>
+      </c>
+      <c r="D731" s="14" t="s">
+        <v>1407</v>
       </c>
       <c r="E731" s="39" t="s">
         <v>22</v>
@@ -26551,18 +26594,18 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="732" spans="1:9" ht="45">
+    <row r="732" spans="1:9" ht="30">
       <c r="A732" s="39" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
       <c r="B732" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C732" s="13" t="s">
-        <v>1723</v>
-      </c>
-      <c r="D732" s="39" t="s">
-        <v>1401</v>
+        <v>1721</v>
+      </c>
+      <c r="D732" s="14" t="s">
+        <v>1399</v>
       </c>
       <c r="E732" s="39" t="s">
         <v>22</v>
@@ -26580,16 +26623,16 @@
     </row>
     <row r="733" spans="1:9" ht="45">
       <c r="A733" s="39" t="s">
-        <v>830</v>
+        <v>826</v>
       </c>
       <c r="B733" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C733" s="41" t="s">
-        <v>794</v>
+      <c r="C733" s="13" t="s">
+        <v>1511</v>
       </c>
       <c r="D733" s="39" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="E733" s="39" t="s">
         <v>22</v>
@@ -26609,16 +26652,16 @@
     </row>
     <row r="734" spans="1:9" ht="45">
       <c r="A734" s="39" t="s">
-        <v>831</v>
+        <v>827</v>
       </c>
       <c r="B734" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C734" s="13" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="D734" s="14" t="s">
-        <v>1409</v>
+        <v>1400</v>
       </c>
       <c r="E734" s="39" t="s">
         <v>22</v>
@@ -26634,18 +26677,18 @@
       </c>
       <c r="I734" s="41"/>
     </row>
-    <row r="735" spans="1:9" ht="30">
+    <row r="735" spans="1:9" ht="45">
       <c r="A735" s="39" t="s">
-        <v>832</v>
+        <v>828</v>
       </c>
       <c r="B735" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C735" s="13" t="s">
-        <v>1503</v>
+        <v>1512</v>
       </c>
       <c r="D735" s="39" t="s">
-        <v>1409</v>
+        <v>1400</v>
       </c>
       <c r="E735" s="39" t="s">
         <v>22</v>
@@ -26656,23 +26699,25 @@
       <c r="G735" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H735" s="14" t="s">
-        <v>1484</v>
-      </c>
-      <c r="I735" s="41"/>
+      <c r="H735" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I735" s="41" t="s">
+        <v>1411</v>
+      </c>
     </row>
     <row r="736" spans="1:9" ht="45">
       <c r="A736" s="39" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="B736" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C736" s="13" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="D736" s="39" t="s">
-        <v>1410</v>
+        <v>1401</v>
       </c>
       <c r="E736" s="39" t="s">
         <v>22</v>
@@ -26690,16 +26735,16 @@
     </row>
     <row r="737" spans="1:9" ht="45">
       <c r="A737" s="39" t="s">
-        <v>834</v>
+        <v>830</v>
       </c>
       <c r="B737" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="C737" s="13" t="s">
-        <v>1504</v>
-      </c>
-      <c r="D737" s="14" t="s">
-        <v>1543</v>
+      <c r="C737" s="41" t="s">
+        <v>794</v>
+      </c>
+      <c r="D737" s="39" t="s">
+        <v>1401</v>
       </c>
       <c r="E737" s="39" t="s">
         <v>22</v>
@@ -26719,16 +26764,16 @@
     </row>
     <row r="738" spans="1:9" ht="45">
       <c r="A738" s="39" t="s">
-        <v>835</v>
+        <v>831</v>
       </c>
       <c r="B738" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C738" s="13" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="D738" s="14" t="s">
-        <v>930</v>
+        <v>1409</v>
       </c>
       <c r="E738" s="39" t="s">
         <v>22</v>
@@ -26744,18 +26789,18 @@
       </c>
       <c r="I738" s="41"/>
     </row>
-    <row r="739" spans="1:9" ht="45">
+    <row r="739" spans="1:9" ht="30">
       <c r="A739" s="39" t="s">
-        <v>836</v>
+        <v>832</v>
       </c>
       <c r="B739" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C739" s="13" t="s">
-        <v>1513</v>
+        <v>1503</v>
       </c>
       <c r="D739" s="39" t="s">
-        <v>930</v>
+        <v>1409</v>
       </c>
       <c r="E739" s="39" t="s">
         <v>22</v>
@@ -26766,25 +26811,23 @@
       <c r="G739" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H739" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I739" s="41" t="s">
-        <v>1411</v>
-      </c>
+      <c r="H739" s="14" t="s">
+        <v>1484</v>
+      </c>
+      <c r="I739" s="41"/>
     </row>
     <row r="740" spans="1:9" ht="45">
       <c r="A740" s="39" t="s">
-        <v>837</v>
+        <v>833</v>
       </c>
       <c r="B740" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C740" s="13" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="D740" s="39" t="s">
-        <v>932</v>
+        <v>1410</v>
       </c>
       <c r="E740" s="39" t="s">
         <v>22</v>
@@ -26802,16 +26845,16 @@
     </row>
     <row r="741" spans="1:9" ht="45">
       <c r="A741" s="39" t="s">
-        <v>838</v>
+        <v>834</v>
       </c>
       <c r="B741" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C741" s="13" t="s">
-        <v>1540</v>
-      </c>
-      <c r="D741" s="39" t="s">
-        <v>932</v>
+        <v>1504</v>
+      </c>
+      <c r="D741" s="14" t="s">
+        <v>1543</v>
       </c>
       <c r="E741" s="39" t="s">
         <v>22</v>
@@ -26831,16 +26874,16 @@
     </row>
     <row r="742" spans="1:9" ht="45">
       <c r="A742" s="39" t="s">
-        <v>839</v>
+        <v>835</v>
       </c>
       <c r="B742" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C742" s="13" t="s">
-        <v>1728</v>
-      </c>
-      <c r="D742" s="39" t="s">
-        <v>934</v>
+        <v>1726</v>
+      </c>
+      <c r="D742" s="14" t="s">
+        <v>930</v>
       </c>
       <c r="E742" s="39" t="s">
         <v>22</v>
@@ -26858,16 +26901,16 @@
     </row>
     <row r="743" spans="1:9" ht="45">
       <c r="A743" s="39" t="s">
-        <v>840</v>
+        <v>836</v>
       </c>
       <c r="B743" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C743" s="13" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D743" s="39" t="s">
-        <v>934</v>
+        <v>930</v>
       </c>
       <c r="E743" s="39" t="s">
         <v>22</v>
@@ -26885,18 +26928,18 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="744" spans="1:9" ht="30">
+    <row r="744" spans="1:9" ht="45">
       <c r="A744" s="39" t="s">
-        <v>841</v>
+        <v>837</v>
       </c>
       <c r="B744" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C744" s="13" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="D744" s="39" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E744" s="39" t="s">
         <v>22</v>
@@ -26914,16 +26957,16 @@
     </row>
     <row r="745" spans="1:9" ht="45">
       <c r="A745" s="39" t="s">
-        <v>842</v>
+        <v>838</v>
       </c>
       <c r="B745" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C745" s="13" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="D745" s="39" t="s">
-        <v>936</v>
+        <v>932</v>
       </c>
       <c r="E745" s="39" t="s">
         <v>22</v>
@@ -26941,18 +26984,18 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="746" spans="1:9" ht="30">
+    <row r="746" spans="1:9" ht="45">
       <c r="A746" s="39" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="B746" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C746" s="13" t="s">
-        <v>1615</v>
+        <v>1728</v>
       </c>
       <c r="D746" s="39" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="E746" s="39" t="s">
         <v>22</v>
@@ -26969,17 +27012,17 @@
       <c r="I746" s="41"/>
     </row>
     <row r="747" spans="1:9" ht="45">
-      <c r="A747" s="14" t="s">
-        <v>1538</v>
+      <c r="A747" s="39" t="s">
+        <v>840</v>
       </c>
       <c r="B747" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C747" s="13" t="s">
-        <v>1536</v>
+        <v>1514</v>
       </c>
       <c r="D747" s="39" t="s">
-        <v>938</v>
+        <v>934</v>
       </c>
       <c r="E747" s="39" t="s">
         <v>22</v>
@@ -26997,18 +27040,18 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="748" spans="1:9" ht="45">
+    <row r="748" spans="1:9" ht="30">
       <c r="A748" s="39" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B748" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C748" s="13" t="s">
-        <v>1730</v>
-      </c>
-      <c r="D748" s="14" t="s">
-        <v>948</v>
+        <v>1729</v>
+      </c>
+      <c r="D748" s="39" t="s">
+        <v>936</v>
       </c>
       <c r="E748" s="39" t="s">
         <v>22</v>
@@ -27026,16 +27069,16 @@
     </row>
     <row r="749" spans="1:9" ht="45">
       <c r="A749" s="39" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B749" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C749" s="13" t="s">
-        <v>1515</v>
+        <v>1539</v>
       </c>
       <c r="D749" s="39" t="s">
-        <v>948</v>
+        <v>936</v>
       </c>
       <c r="E749" s="39" t="s">
         <v>22</v>
@@ -27046,25 +27089,25 @@
       <c r="G749" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H749" s="14" t="s">
-        <v>1487</v>
+      <c r="H749" s="39" t="s">
+        <v>21</v>
       </c>
       <c r="I749" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
-    <row r="750" spans="1:9" ht="45">
+    <row r="750" spans="1:9" ht="30">
       <c r="A750" s="39" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B750" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C750" s="13" t="s">
-        <v>1731</v>
+        <v>1615</v>
       </c>
       <c r="D750" s="39" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="E750" s="39" t="s">
         <v>22</v>
@@ -27082,16 +27125,16 @@
     </row>
     <row r="751" spans="1:9" ht="45">
       <c r="A751" s="14" t="s">
-        <v>1534</v>
+        <v>1538</v>
       </c>
       <c r="B751" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C751" s="13" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="D751" s="39" t="s">
-        <v>950</v>
+        <v>938</v>
       </c>
       <c r="E751" s="39" t="s">
         <v>22</v>
@@ -27102,25 +27145,25 @@
       <c r="G751" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H751" s="14" t="s">
-        <v>1487</v>
-      </c>
-      <c r="I751" s="13" t="s">
+      <c r="H751" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I751" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="752" spans="1:9" ht="45">
-      <c r="A752" s="14" t="s">
-        <v>1478</v>
-      </c>
-      <c r="B752" s="43">
-        <v>8</v>
+      <c r="A752" s="39" t="s">
+        <v>844</v>
+      </c>
+      <c r="B752" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C752" s="13" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="D752" s="14" t="s">
-        <v>1479</v>
+        <v>948</v>
       </c>
       <c r="E752" s="39" t="s">
         <v>22</v>
@@ -27137,17 +27180,17 @@
       <c r="I752" s="41"/>
     </row>
     <row r="753" spans="1:9" ht="45">
-      <c r="A753" s="14" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B753" s="43">
-        <v>8</v>
+      <c r="A753" s="39" t="s">
+        <v>845</v>
+      </c>
+      <c r="B753" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C753" s="13" t="s">
-        <v>1516</v>
-      </c>
-      <c r="D753" s="14" t="s">
-        <v>1479</v>
+        <v>1515</v>
+      </c>
+      <c r="D753" s="39" t="s">
+        <v>948</v>
       </c>
       <c r="E753" s="39" t="s">
         <v>22</v>
@@ -27158,25 +27201,25 @@
       <c r="G753" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H753" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I753" s="13" t="s">
+      <c r="H753" s="14" t="s">
+        <v>1487</v>
+      </c>
+      <c r="I753" s="41" t="s">
         <v>1411</v>
       </c>
     </row>
     <row r="754" spans="1:9" ht="45">
-      <c r="A754" s="14" t="s">
-        <v>847</v>
+      <c r="A754" s="39" t="s">
+        <v>846</v>
       </c>
       <c r="B754" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C754" s="13" t="s">
-        <v>1733</v>
-      </c>
-      <c r="D754" t="s">
-        <v>1428</v>
+        <v>1731</v>
+      </c>
+      <c r="D754" s="39" t="s">
+        <v>950</v>
       </c>
       <c r="E754" s="39" t="s">
         <v>22</v>
@@ -27194,16 +27237,16 @@
     </row>
     <row r="755" spans="1:9" ht="45">
       <c r="A755" s="14" t="s">
-        <v>1532</v>
+        <v>1534</v>
       </c>
       <c r="B755" s="40" t="s">
         <v>607</v>
       </c>
       <c r="C755" s="13" t="s">
-        <v>1506</v>
-      </c>
-      <c r="D755" t="s">
-        <v>1517</v>
+        <v>1535</v>
+      </c>
+      <c r="D755" s="39" t="s">
+        <v>950</v>
       </c>
       <c r="E755" s="39" t="s">
         <v>22</v>
@@ -27214,26 +27257,28 @@
       <c r="G755" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="H755" s="39" t="s">
-        <v>21</v>
+      <c r="H755" s="14" t="s">
+        <v>1487</v>
       </c>
       <c r="I755" s="13" t="s">
         <v>1411</v>
       </c>
     </row>
-    <row r="756" spans="1:9" ht="390">
+    <row r="756" spans="1:9" ht="45">
       <c r="A756" s="14" t="s">
-        <v>1368</v>
-      </c>
-      <c r="B756" s="16" t="s">
-        <v>1477</v>
+        <v>1478</v>
+      </c>
+      <c r="B756" s="43">
+        <v>8</v>
       </c>
       <c r="C756" s="13" t="s">
-        <v>1524</v>
-      </c>
-      <c r="D756" s="39"/>
+        <v>1732</v>
+      </c>
+      <c r="D756" s="14" t="s">
+        <v>1479</v>
+      </c>
       <c r="E756" s="39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F756" s="39" t="s">
         <v>3</v>
@@ -27242,23 +27287,25 @@
         <v>15</v>
       </c>
       <c r="H756" s="39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I756" s="41"/>
     </row>
-    <row r="757" spans="1:9" ht="30">
+    <row r="757" spans="1:9" ht="45">
       <c r="A757" s="14" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B757" s="16" t="s">
-        <v>1477</v>
-      </c>
-      <c r="C757" s="41" t="s">
-        <v>1367</v>
-      </c>
-      <c r="D757" s="39"/>
+        <v>1533</v>
+      </c>
+      <c r="B757" s="43">
+        <v>8</v>
+      </c>
+      <c r="C757" s="13" t="s">
+        <v>1516</v>
+      </c>
+      <c r="D757" s="14" t="s">
+        <v>1479</v>
+      </c>
       <c r="E757" s="39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F757" s="39" t="s">
         <v>3</v>
@@ -27269,21 +27316,25 @@
       <c r="H757" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I757" s="41"/>
-    </row>
-    <row r="758" spans="1:9" ht="30">
+      <c r="I757" s="13" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="758" spans="1:9" ht="45">
       <c r="A758" s="14" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B758" s="16" t="s">
-        <v>1477</v>
+        <v>847</v>
+      </c>
+      <c r="B758" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C758" s="13" t="s">
-        <v>1529</v>
-      </c>
-      <c r="D758" s="39"/>
+        <v>1733</v>
+      </c>
+      <c r="D758" t="s">
+        <v>1428</v>
+      </c>
       <c r="E758" s="39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F758" s="39" t="s">
         <v>3</v>
@@ -27292,23 +27343,25 @@
         <v>15</v>
       </c>
       <c r="H758" s="39" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I758" s="41"/>
     </row>
-    <row r="759" spans="1:9">
+    <row r="759" spans="1:9" ht="45">
       <c r="A759" s="14" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B759" s="16" t="s">
-        <v>1477</v>
+        <v>1532</v>
+      </c>
+      <c r="B759" s="40" t="s">
+        <v>607</v>
       </c>
       <c r="C759" s="13" t="s">
-        <v>1526</v>
-      </c>
-      <c r="D759" s="39"/>
+        <v>1506</v>
+      </c>
+      <c r="D759" t="s">
+        <v>1517</v>
+      </c>
       <c r="E759" s="39" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F759" s="39" t="s">
         <v>3</v>
@@ -27319,17 +27372,19 @@
       <c r="H759" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I759" s="41"/>
-    </row>
-    <row r="760" spans="1:9" ht="30">
+      <c r="I759" s="13" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="760" spans="1:9" ht="390">
       <c r="A760" s="14" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="B760" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C760" s="13" t="s">
-        <v>1505</v>
+        <v>1524</v>
       </c>
       <c r="D760" s="39"/>
       <c r="E760" s="39" t="s">
@@ -27346,15 +27401,15 @@
       </c>
       <c r="I760" s="41"/>
     </row>
-    <row r="761" spans="1:9">
+    <row r="761" spans="1:9" ht="30">
       <c r="A761" s="14" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="B761" s="16" t="s">
         <v>1477</v>
       </c>
-      <c r="C761" s="13" t="s">
-        <v>1523</v>
+      <c r="C761" s="41" t="s">
+        <v>1367</v>
       </c>
       <c r="D761" s="39"/>
       <c r="E761" s="39" t="s">
@@ -27373,13 +27428,13 @@
     </row>
     <row r="762" spans="1:9" ht="30">
       <c r="A762" s="14" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="B762" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C762" s="13" t="s">
-        <v>1518</v>
+        <v>1529</v>
       </c>
       <c r="D762" s="39"/>
       <c r="E762" s="39" t="s">
@@ -27398,13 +27453,13 @@
     </row>
     <row r="763" spans="1:9">
       <c r="A763" s="14" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="B763" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C763" s="13" t="s">
-        <v>1525</v>
+        <v>1526</v>
       </c>
       <c r="D763" s="39"/>
       <c r="E763" s="39" t="s">
@@ -27423,13 +27478,13 @@
     </row>
     <row r="764" spans="1:9" ht="30">
       <c r="A764" s="14" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="B764" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C764" s="13" t="s">
-        <v>1528</v>
+        <v>1505</v>
       </c>
       <c r="D764" s="39"/>
       <c r="E764" s="39" t="s">
@@ -27446,15 +27501,15 @@
       </c>
       <c r="I764" s="41"/>
     </row>
-    <row r="765" spans="1:9" ht="30">
+    <row r="765" spans="1:9">
       <c r="A765" s="14" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="B765" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C765" s="13" t="s">
-        <v>1527</v>
+        <v>1523</v>
       </c>
       <c r="D765" s="39"/>
       <c r="E765" s="39" t="s">
@@ -27471,15 +27526,15 @@
       </c>
       <c r="I765" s="41"/>
     </row>
-    <row r="766" spans="1:9" ht="45">
+    <row r="766" spans="1:9" ht="30">
       <c r="A766" s="14" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="B766" s="16" t="s">
         <v>1477</v>
       </c>
       <c r="C766" s="13" t="s">
-        <v>1522</v>
+        <v>1518</v>
       </c>
       <c r="D766" s="39"/>
       <c r="E766" s="39" t="s">
@@ -27496,65 +27551,65 @@
       </c>
       <c r="I766" s="41"/>
     </row>
-    <row r="767" spans="1:9" ht="180">
-      <c r="A767" s="21" t="s">
-        <v>383</v>
+    <row r="767" spans="1:9">
+      <c r="A767" s="14" t="s">
+        <v>1375</v>
       </c>
       <c r="B767" s="16" t="s">
-        <v>420</v>
+        <v>1477</v>
       </c>
       <c r="C767" s="13" t="s">
-        <v>582</v>
-      </c>
-      <c r="D767" s="21"/>
-      <c r="E767" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F767" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G767" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H767" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="I767" s="23"/>
-    </row>
-    <row r="768" spans="1:9" ht="150">
+        <v>1525</v>
+      </c>
+      <c r="D767" s="39"/>
+      <c r="E767" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F767" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G767" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H767" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I767" s="41"/>
+    </row>
+    <row r="768" spans="1:9" ht="30">
       <c r="A768" s="14" t="s">
-        <v>384</v>
+        <v>1376</v>
       </c>
       <c r="B768" s="16" t="s">
-        <v>1359</v>
+        <v>1477</v>
       </c>
       <c r="C768" s="13" t="s">
-        <v>1521</v>
-      </c>
-      <c r="D768" s="21"/>
-      <c r="E768" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F768" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G768" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H768" s="21" t="s">
+        <v>1528</v>
+      </c>
+      <c r="D768" s="39"/>
+      <c r="E768" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F768" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G768" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H768" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="I768" s="23"/>
-    </row>
-    <row r="769" spans="1:9" ht="135">
-      <c r="A769" s="39" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B769" s="40" t="s">
-        <v>1353</v>
+      <c r="I768" s="41"/>
+    </row>
+    <row r="769" spans="1:9" ht="30">
+      <c r="A769" s="14" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B769" s="16" t="s">
+        <v>1477</v>
       </c>
       <c r="C769" s="13" t="s">
-        <v>1519</v>
+        <v>1527</v>
       </c>
       <c r="D769" s="39"/>
       <c r="E769" s="39" t="s">
@@ -27571,65 +27626,65 @@
       </c>
       <c r="I769" s="41"/>
     </row>
-    <row r="770" spans="1:9" ht="409.5">
-      <c r="A770" s="21" t="s">
-        <v>385</v>
+    <row r="770" spans="1:9" ht="45">
+      <c r="A770" s="14" t="s">
+        <v>1378</v>
       </c>
       <c r="B770" s="16" t="s">
-        <v>1360</v>
+        <v>1477</v>
       </c>
       <c r="C770" s="13" t="s">
-        <v>583</v>
-      </c>
-      <c r="D770" s="21"/>
-      <c r="E770" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F770" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G770" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H770" s="21" t="s">
+        <v>1522</v>
+      </c>
+      <c r="D770" s="39"/>
+      <c r="E770" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F770" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G770" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H770" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I770" s="41"/>
+    </row>
+    <row r="771" spans="1:9" ht="180">
+      <c r="A771" s="21" t="s">
+        <v>383</v>
+      </c>
+      <c r="B771" s="16" t="s">
+        <v>420</v>
+      </c>
+      <c r="C771" s="13" t="s">
+        <v>582</v>
+      </c>
+      <c r="D771" s="21"/>
+      <c r="E771" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F771" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G771" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H771" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="I770" s="23"/>
-    </row>
-    <row r="771" spans="1:9" ht="409.5">
-      <c r="A771" s="14" t="s">
-        <v>1379</v>
-      </c>
-      <c r="B771" s="40" t="s">
-        <v>1361</v>
-      </c>
-      <c r="C771" s="13" t="s">
-        <v>1520</v>
-      </c>
-      <c r="D771" s="39"/>
-      <c r="E771" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F771" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G771" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H771" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="I771" s="41"/>
-    </row>
-    <row r="772" spans="1:9" ht="135">
-      <c r="A772" s="21" t="s">
-        <v>386</v>
+      <c r="I771" s="23"/>
+    </row>
+    <row r="772" spans="1:9" ht="150">
+      <c r="A772" s="14" t="s">
+        <v>384</v>
       </c>
       <c r="B772" s="16" t="s">
-        <v>1355</v>
+        <v>1359</v>
       </c>
       <c r="C772" s="13" t="s">
-        <v>584</v>
+        <v>1521</v>
       </c>
       <c r="D772" s="21"/>
       <c r="E772" s="21" t="s">
@@ -27642,44 +27697,44 @@
         <v>15</v>
       </c>
       <c r="H772" s="21" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I772" s="23"/>
     </row>
-    <row r="773" spans="1:9" ht="180">
-      <c r="A773" s="21" t="s">
-        <v>377</v>
-      </c>
-      <c r="B773" s="16" t="s">
-        <v>1356</v>
+    <row r="773" spans="1:9" ht="135">
+      <c r="A773" s="39" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B773" s="40" t="s">
+        <v>1353</v>
       </c>
       <c r="C773" s="13" t="s">
-        <v>576</v>
-      </c>
-      <c r="D773" s="21"/>
-      <c r="E773" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F773" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G773" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H773" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I773" s="23"/>
-    </row>
-    <row r="774" spans="1:9" ht="30">
-      <c r="A774" s="14" t="s">
-        <v>378</v>
+        <v>1519</v>
+      </c>
+      <c r="D773" s="39"/>
+      <c r="E773" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F773" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G773" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H773" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I773" s="41"/>
+    </row>
+    <row r="774" spans="1:9" ht="409.5">
+      <c r="A774" s="21" t="s">
+        <v>385</v>
       </c>
       <c r="B774" s="16" t="s">
-        <v>1357</v>
+        <v>1360</v>
       </c>
       <c r="C774" s="13" t="s">
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="D774" s="21"/>
       <c r="E774" s="21" t="s">
@@ -27692,44 +27747,44 @@
         <v>15</v>
       </c>
       <c r="H774" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I774" s="23"/>
     </row>
-    <row r="775" spans="1:9" ht="105">
-      <c r="A775" s="21" t="s">
-        <v>379</v>
-      </c>
-      <c r="B775" s="16" t="s">
-        <v>1357</v>
-      </c>
-      <c r="C775" s="23" t="s">
-        <v>578</v>
-      </c>
-      <c r="D775" s="21"/>
-      <c r="E775" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F775" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="G775" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H775" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I775" s="23"/>
-    </row>
-    <row r="776" spans="1:9" ht="45">
+    <row r="775" spans="1:9" ht="409.5">
+      <c r="A775" s="14" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B775" s="40" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C775" s="13" t="s">
+        <v>1520</v>
+      </c>
+      <c r="D775" s="39"/>
+      <c r="E775" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F775" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G775" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H775" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="I775" s="41"/>
+    </row>
+    <row r="776" spans="1:9" ht="135">
       <c r="A776" s="21" t="s">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="B776" s="16" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="C776" s="13" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="D776" s="21"/>
       <c r="E776" s="21" t="s">
@@ -27742,19 +27797,19 @@
         <v>15</v>
       </c>
       <c r="H776" s="21" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I776" s="23"/>
     </row>
-    <row r="777" spans="1:9" ht="30">
+    <row r="777" spans="1:9" ht="180">
       <c r="A777" s="21" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B777" s="16" t="s">
-        <v>1358</v>
+        <v>1356</v>
       </c>
       <c r="C777" s="13" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D777" s="21"/>
       <c r="E777" s="21" t="s">
@@ -27773,13 +27828,13 @@
     </row>
     <row r="778" spans="1:9" ht="30">
       <c r="A778" s="14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B778" s="16" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="C778" s="13" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D778" s="21"/>
       <c r="E778" s="21" t="s">
@@ -27796,72 +27851,172 @@
       </c>
       <c r="I778" s="23"/>
     </row>
-    <row r="779" spans="1:9" ht="45">
-      <c r="A779" s="14" t="s">
-        <v>1364</v>
+    <row r="779" spans="1:9" ht="105">
+      <c r="A779" s="21" t="s">
+        <v>379</v>
       </c>
       <c r="B779" s="16" t="s">
-        <v>1358</v>
-      </c>
-      <c r="C779" s="13" t="s">
-        <v>1365</v>
-      </c>
-      <c r="D779" s="39"/>
-      <c r="E779" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F779" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G779" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H779" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I779" s="41"/>
-    </row>
-    <row r="780" spans="1:9" ht="30">
-      <c r="A780" s="14" t="s">
-        <v>1366</v>
+        <v>1357</v>
+      </c>
+      <c r="C779" s="23" t="s">
+        <v>578</v>
+      </c>
+      <c r="D779" s="21"/>
+      <c r="E779" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F779" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G779" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H779" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I779" s="23"/>
+    </row>
+    <row r="780" spans="1:9" ht="45">
+      <c r="A780" s="21" t="s">
+        <v>380</v>
       </c>
       <c r="B780" s="16" t="s">
         <v>1358</v>
       </c>
       <c r="C780" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="D780" s="21"/>
+      <c r="E780" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F780" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G780" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H780" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I780" s="23"/>
+    </row>
+    <row r="781" spans="1:9" ht="30">
+      <c r="A781" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="B781" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C781" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="D781" s="21"/>
+      <c r="E781" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F781" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G781" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H781" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I781" s="23"/>
+    </row>
+    <row r="782" spans="1:9" ht="30">
+      <c r="A782" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="B782" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C782" s="13" t="s">
         <v>581</v>
       </c>
-      <c r="D780" s="39"/>
-      <c r="E780" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="F780" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="G780" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H780" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="I780" s="41"/>
-    </row>
-    <row r="781" spans="1:9">
-      <c r="A781" s="21"/>
-      <c r="B781" s="22"/>
-      <c r="C781" s="23"/>
-      <c r="D781" s="21"/>
-      <c r="E781" s="21"/>
-      <c r="F781" s="21"/>
-      <c r="G781" s="21"/>
-      <c r="H781" s="21"/>
-      <c r="I781" s="23"/>
-    </row>
-    <row r="782" spans="1:9">
-      <c r="B782" s="7"/>
-    </row>
-    <row r="783" spans="1:9">
-      <c r="B783" s="7"/>
+      <c r="D782" s="21"/>
+      <c r="E782" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F782" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G782" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H782" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I782" s="23"/>
+    </row>
+    <row r="783" spans="1:9" ht="45">
+      <c r="A783" s="14" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B783" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C783" s="13" t="s">
+        <v>1365</v>
+      </c>
+      <c r="D783" s="39"/>
+      <c r="E783" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F783" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G783" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H783" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I783" s="41"/>
+    </row>
+    <row r="784" spans="1:9" ht="30">
+      <c r="A784" s="14" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B784" s="16" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C784" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="D784" s="39"/>
+      <c r="E784" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="F784" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="G784" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="H784" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="I784" s="41"/>
+    </row>
+    <row r="785" spans="1:9">
+      <c r="A785" s="21"/>
+      <c r="B785" s="22"/>
+      <c r="C785" s="23"/>
+      <c r="D785" s="21"/>
+      <c r="E785" s="21"/>
+      <c r="F785" s="21"/>
+      <c r="G785" s="21"/>
+      <c r="H785" s="21"/>
+      <c r="I785" s="23"/>
+    </row>
+    <row r="786" spans="1:9">
+      <c r="B786" s="7"/>
+    </row>
+    <row r="787" spans="1:9">
+      <c r="B787" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -27878,51 +28033,51 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 B276:I276 A277:I781 A81:I275">
-    <cfRule type="expression" dxfId="7" priority="53">
+  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 B276:I276 A277:I785 A81:I275">
+    <cfRule type="expression" dxfId="5" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="54">
+    <cfRule type="expression" dxfId="4" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="61">
+    <cfRule type="expression" dxfId="3" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 B276:I276 A277:I781 A81:I275">
-    <cfRule type="expression" dxfId="4" priority="7">
+  <conditionalFormatting sqref="A20:H45 A80:H80 I20:I50 A35:I79 B276:I276 A277:I785 A81:I275">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F781">
-    <cfRule type="expression" dxfId="1" priority="13">
+  <conditionalFormatting sqref="F20:F785">
+    <cfRule type="expression" dxfId="7" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="6" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F781" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 F20:F785" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E781" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 E20:E785" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G781" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4 G20:G785" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H781" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H785" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27932,7 +28087,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1:B9 B782:B783 B10:B27 B28:B104 B150:B780 B106:B113 B116:B147" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:B9 B786:B787 B10:B27 B28:B104 B680:B784 B106:B113 B116:B147 B150:B675" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>